<commit_message>
new function : channel data retrieval and channel data check function\n refactor data handling: change data types from double to float, update related functions and headers
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F943CA35-707F-4EB6-B873-0EBCECA3F697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB92D0C9-C4DC-4C14-AD0F-739445F6561C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="-11323" yWindow="-13817" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>Import file</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>Test the C program by comparing result of MATLAB and C program, throw error when not the same</t>
+  </si>
+  <si>
+    <t>Channel signal retrieval</t>
   </si>
 </sst>
 </file>
@@ -174,7 +177,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -272,19 +275,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -621,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -633,8 +636,8 @@
     <col min="2" max="2" width="25.921875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.4609375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="72.23046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.3828125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.23046875" style="10"/>
+    <col min="5" max="5" width="6.3828125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.23046875" style="9"/>
     <col min="7" max="16384" width="9.23046875" style="1"/>
   </cols>
   <sheetData>
@@ -654,10 +657,10 @@
       <c r="D2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>32</v>
       </c>
       <c r="G2" s="6" t="s">
@@ -665,16 +668,16 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="12">
+      <c r="E3" s="11">
         <v>45708</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="11">
         <v>45708</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -682,7 +685,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -690,10 +693,10 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <v>45708</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="11">
         <v>45709</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -701,56 +704,52 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A5" s="9"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="5" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="12">
+      <c r="E5" s="11">
+        <v>45716</v>
+      </c>
+      <c r="F5" s="11">
+        <v>45716</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A6" s="13"/>
+      <c r="B6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="11">
         <v>45709</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="4" t="s">
+      <c r="F6" s="11"/>
+      <c r="G6" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A6" s="9" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E7" s="11">
         <v>45709</v>
       </c>
-      <c r="F6" s="12">
-        <v>45709</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A7" s="9"/>
-      <c r="B7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="12">
-        <v>45709</v>
-      </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <v>45709</v>
       </c>
       <c r="G7" s="4" t="s">
@@ -758,110 +757,122 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="13"/>
+      <c r="B8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="11">
+        <v>45709</v>
+      </c>
+      <c r="F8" s="11">
+        <v>45709</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A9" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A9" s="9"/>
-      <c r="B9" s="5" t="s">
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A10" s="13"/>
+      <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A10" s="9" t="s">
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A11" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A11" s="9"/>
-      <c r="B11" s="5" t="s">
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A12" s="13"/>
+      <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A12" s="5" t="s">
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A13" s="5" t="s">
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
@@ -869,8 +880,8 @@
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
@@ -878,8 +889,8 @@
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
@@ -887,8 +898,8 @@
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
@@ -896,16 +907,25 @@
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
       <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: enhance file name validation to extract frequency and update related functions
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB92D0C9-C4DC-4C14-AD0F-739445F6561C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A1AA6B-319B-4545-BB76-C45C9CA5E189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-11323" yWindow="-13817" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>Import file</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Downsampling</t>
   </si>
   <si>
-    <t>ongoing</t>
-  </si>
-  <si>
     <t>Result Compare</t>
   </si>
   <si>
@@ -170,6 +167,9 @@
   </si>
   <si>
     <t>Channel signal retrieval</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -624,52 +624,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="15.23046875" style="2" customWidth="1"/>
     <col min="2" max="2" width="25.921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.4609375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.23046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.4609375" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="72.23046875" style="2" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="6.3828125" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.23046875" style="9"/>
-    <col min="7" max="16384" width="9.23046875" style="1"/>
+    <col min="7" max="7" width="9.23046875" style="1"/>
+    <col min="8" max="8" width="60.84375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.23046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="26.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="8"/>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" ht="31.3" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="31.3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>32</v>
-      </c>
       <c r="G2" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+        <v>29</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -683,8 +688,9 @@
       <c r="G3" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
@@ -702,11 +708,12 @@
       <c r="G4" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="13"/>
       <c r="B5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -719,8 +726,9 @@
       <c r="G5" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="13"/>
       <c r="B6" s="5" t="s">
         <v>25</v>
@@ -730,21 +738,24 @@
       <c r="E6" s="11">
         <v>45709</v>
       </c>
-      <c r="F6" s="11"/>
+      <c r="F6" s="11">
+        <v>45718</v>
+      </c>
       <c r="G6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A7" s="13" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A7" s="13" t="s">
+      <c r="B7" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" s="11">
         <v>45709</v>
@@ -755,17 +766,18 @@
       <c r="G7" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A8" s="13"/>
       <c r="B8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="E8" s="11">
         <v>45709</v>
@@ -776,8 +788,9 @@
       <c r="G8" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A9" s="13" t="s">
         <v>2</v>
       </c>
@@ -793,8 +806,9 @@
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A10" s="13"/>
       <c r="B10" s="5" t="s">
         <v>5</v>
@@ -808,8 +822,9 @@
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A11" s="13" t="s">
         <v>7</v>
       </c>
@@ -825,8 +840,9 @@
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A12" s="13"/>
       <c r="B12" s="5" t="s">
         <v>9</v>
@@ -840,8 +856,9 @@
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
@@ -857,8 +874,9 @@
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
@@ -874,8 +892,9 @@
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -883,8 +902,9 @@
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -892,8 +912,9 @@
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -901,8 +922,9 @@
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -910,8 +932,9 @@
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -919,6 +942,7 @@
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
signal filtering functionailtiy - initial commit
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A1AA6B-319B-4545-BB76-C45C9CA5E189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811234ED-F132-4A62-88DC-009272E902E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11323" yWindow="-13817" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="10620" yWindow="-13826" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>Import file</t>
   </si>
@@ -170,6 +170,13 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Est
+Start</t>
+  </si>
+  <si>
+    <t>Testing and Refactoring</t>
   </si>
 </sst>
 </file>
@@ -249,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -285,6 +292,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -624,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -636,17 +646,18 @@
     <col min="2" max="2" width="25.921875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.4609375" style="2" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="72.23046875" style="2" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="6.3828125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.23046875" style="9"/>
-    <col min="7" max="7" width="9.23046875" style="1"/>
-    <col min="8" max="8" width="60.84375" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.23046875" style="1"/>
+    <col min="5" max="5" width="6.4609375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="6.3828125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.23046875" style="9"/>
+    <col min="8" max="8" width="9.23046875" style="1"/>
+    <col min="9" max="9" width="60.84375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.23046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="26.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="8"/>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" ht="31.3" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="31.3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>35</v>
       </c>
@@ -659,39 +670,43 @@
       <c r="D2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="11">
-        <v>45708</v>
-      </c>
+      <c r="E3" s="5"/>
       <c r="F3" s="11">
         <v>45708</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="11">
+        <v>45708</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A4" s="13" t="s">
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -699,55 +714,58 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="11">
+      <c r="E4" s="5"/>
+      <c r="F4" s="11">
         <v>45708</v>
       </c>
-      <c r="F4" s="11">
+      <c r="G4" s="11">
         <v>45709</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A5" s="13"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A5" s="14"/>
       <c r="B5" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="11">
-        <v>45716</v>
-      </c>
+      <c r="E5" s="5"/>
       <c r="F5" s="11">
         <v>45716</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="11">
+        <v>45716</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A6" s="13"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A6" s="14"/>
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="11">
+      <c r="E6" s="5"/>
+      <c r="F6" s="11">
         <v>45709</v>
       </c>
-      <c r="F6" s="11">
+      <c r="G6" s="11">
         <v>45718</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A7" s="13" t="s">
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A7" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -757,19 +775,20 @@
       <c r="D7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="11">
-        <v>45709</v>
-      </c>
+      <c r="E7" s="5"/>
       <c r="F7" s="11">
         <v>45709</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="11">
+        <v>45709</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A8" s="13"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A8" s="14"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -779,19 +798,20 @@
       <c r="D8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="11">
-        <v>45709</v>
-      </c>
+      <c r="E8" s="5"/>
       <c r="F8" s="11">
         <v>45709</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="11">
+        <v>45709</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A9" s="13" t="s">
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A9" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -803,13 +823,18 @@
       <c r="D9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="4"/>
+      <c r="E9" s="13">
+        <v>45719</v>
+      </c>
+      <c r="F9" s="13">
+        <v>45719</v>
+      </c>
+      <c r="G9" s="11"/>
       <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A10" s="13"/>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A10" s="14"/>
       <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
@@ -819,13 +844,16 @@
       <c r="D10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="11"/>
+      <c r="E10" s="13">
+        <v>45722</v>
+      </c>
       <c r="F10" s="11"/>
-      <c r="G10" s="4"/>
+      <c r="G10" s="11"/>
       <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A11" s="13" t="s">
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A11" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -837,13 +865,16 @@
       <c r="D11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="11"/>
+      <c r="E11" s="13">
+        <v>45726</v>
+      </c>
       <c r="F11" s="11"/>
-      <c r="G11" s="4"/>
+      <c r="G11" s="11"/>
       <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A12" s="13"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A12" s="14"/>
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
@@ -853,12 +884,15 @@
       <c r="D12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="11"/>
+      <c r="E12" s="13">
+        <v>45729</v>
+      </c>
       <c r="F12" s="11"/>
-      <c r="G12" s="4"/>
+      <c r="G12" s="11"/>
       <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
@@ -871,12 +905,15 @@
       <c r="D13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="11"/>
+      <c r="E13" s="13">
+        <v>45733</v>
+      </c>
       <c r="F13" s="11"/>
-      <c r="G13" s="4"/>
+      <c r="G13" s="11"/>
       <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
@@ -889,60 +926,72 @@
       <c r="D14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="11"/>
+      <c r="E14" s="13">
+        <v>45736</v>
+      </c>
       <c r="F14" s="11"/>
-      <c r="G14" s="4"/>
+      <c r="G14" s="11"/>
       <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A15" s="5"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A15" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="11"/>
+      <c r="E15" s="13">
+        <v>45740</v>
+      </c>
       <c r="F15" s="11"/>
-      <c r="G15" s="4"/>
+      <c r="G15" s="11"/>
       <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="11"/>
+      <c r="E16" s="5"/>
       <c r="F16" s="11"/>
-      <c r="G16" s="4"/>
+      <c r="G16" s="11"/>
       <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="11"/>
+      <c r="E17" s="5"/>
       <c r="F17" s="11"/>
-      <c r="G17" s="4"/>
+      <c r="G17" s="11"/>
       <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="11"/>
+      <c r="E18" s="5"/>
       <c r="F18" s="11"/>
-      <c r="G18" s="4"/>
+      <c r="G18" s="11"/>
       <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="11"/>
+      <c r="E19" s="5"/>
       <c r="F19" s="11"/>
-      <c r="G19" s="4"/>
+      <c r="G19" s="11"/>
       <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
feat: update configuration options, add signal buffering and filtering functionality
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811234ED-F132-4A62-88DC-009272E902E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916527DA-6A01-4CA0-9A75-65DEB69E547A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10620" yWindow="-13826" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="16311" yWindow="-13723" windowWidth="16458" windowHeight="9454" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>Import file</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Testing and Refactoring</t>
+  </si>
+  <si>
+    <t>ongoing</t>
   </si>
 </sst>
 </file>
@@ -636,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -830,7 +833,9 @@
         <v>45719</v>
       </c>
       <c r="G9" s="11"/>
-      <c r="H9" s="4"/>
+      <c r="H9" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
feat: lowpass filter created ,restructured file sturcture, created signal_buffering.c which buffers through the signal.
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916527DA-6A01-4CA0-9A75-65DEB69E547A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB2B291-C50D-47E5-B1F4-4306D80D4C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16311" yWindow="-13723" windowWidth="16458" windowHeight="9454" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="10620" yWindow="-13826" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -36,8 +36,40 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="2">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="2">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>Import file</t>
   </si>
@@ -180,6 +212,18 @@
   </si>
   <si>
     <t>ongoing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used the coefficient that </t>
+  </si>
+  <si>
+    <t>Low Pass Filtering functionality in C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It took alot of time attempting to understand the filtering logic, especially due to Daryl's MATLAB project used a built in MATLAB lowpass function. It was not clear what coefficient was used in this function, but there was a file called lowpass_coeffs.mat in the root directory of the project, but was not imported in any part of the project code. I assumed somehow it was an extracted coefficient of the whats used in the lowpass function so used is in my C low pass filtering functionality. I got a similar trend of result comparing with the matlab code(shown in diagram, but C showing results of about 150 higher that the MATLAB results. </t>
+  </si>
+  <si>
+    <t>I got it to get similar result but not exactly the same. I think it may be because I am using floats instead of double in my C code, Matlab uses double. Plan to change to double next</t>
   </si>
 </sst>
 </file>
@@ -259,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -302,6 +346,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -318,6 +371,75 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>1</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+  <rel r:id="rId2"/>
+</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -639,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -836,7 +958,9 @@
       <c r="H9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I9" s="4"/>
+      <c r="I9" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A10" s="14"/>
@@ -1012,14 +1136,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.23046875" style="16"/>
+    <col min="2" max="2" width="33.84375" style="15" customWidth="1"/>
+    <col min="3" max="3" width="70.84375" style="17" customWidth="1"/>
+    <col min="4" max="4" width="47.15234375" style="15" customWidth="1"/>
+    <col min="5" max="16384" width="9.23046875" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" ht="116.6" x14ac:dyDescent="0.4">
+      <c r="A2" s="16">
+        <v>45723</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="15" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="C3" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="15" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat:  adjust buffer sizes to align with MATLAB logic, moved signal verification function to data_init.c
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB2B291-C50D-47E5-B1F4-4306D80D4C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5503B0-26F9-433D-9D18-18819EBFE3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10620" yWindow="-13826" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="21840" yWindow="1217" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t>Import file</t>
   </si>
@@ -211,12 +211,6 @@
     <t>Testing and Refactoring</t>
   </si>
   <si>
-    <t>ongoing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Used the coefficient that </t>
-  </si>
-  <si>
     <t>Low Pass Filtering functionality in C</t>
   </si>
   <si>
@@ -224,6 +218,24 @@
   </si>
   <si>
     <t>I got it to get similar result but not exactly the same. I think it may be because I am using floats instead of double in my C code, Matlab uses double. Plan to change to double next</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figured out the problem from deeply investigating the daryl's MATLAB project's lowpass filter logic and reading documentations of how the built in filter() function works. Found out the following.
+1. In Daryl's code layer
+- 60 padding front and back added to signal(first value for front 600 values and end value for back 60 values)
+- then it is passed to built in lowpass function
+- then the paddings are removed front and back from the output signal from the lowpass function
+2. MATLAB Layer
+- built in lowpass function checks the opts variables and runs FIR logic, which firstly adds the the filter delay(filter order * 0.5) amount of zero values(29 in this case) to the end of the padded signal.
+- then it is passed to another builtin filter function with the coeffitcients retrieved from the opts variables
+- the output signal from the builtin filter function then has the filter delay amount of  values removed from the front of the signal
+The logic was implimented in the code exactly as the logic above although was still not showing exact result and the reason was below.
+1. Coefficients used in the builtin MATLAB filter() function was not the same as fir_51.mat file in Daryl's project. I found the actual coefficients used in the opts variable that was used in runtime within the lowpass() builtin function. 59 was the number of coefficients that was actually used and the values were also different. 
+2. The filter order != number of coefficients, but was  filter order == number of coefficients - 1, which was 29 in this case
+3. the buffering logic of Daryl's MATLAB code had a error, because matlab does not use 0 indexing, the buffer size was set to 1000 but the buffer was processing 1001 signals in everytime except the first buffer. </t>
+  </si>
+  <si>
+    <t>May need to adjust later. Currently copied wrong logic in Daryl's project to get same results</t>
   </si>
 </sst>
 </file>
@@ -344,17 +356,17 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -761,7 +773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -775,7 +787,7 @@
     <col min="6" max="6" width="6.3828125" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.23046875" style="9"/>
     <col min="8" max="8" width="9.23046875" style="1"/>
-    <col min="9" max="9" width="60.84375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="60.84375" style="2" customWidth="1"/>
     <col min="10" max="16384" width="9.23046875" style="1"/>
   </cols>
   <sheetData>
@@ -807,7 +819,7 @@
       <c r="H2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>41</v>
       </c>
     </row>
@@ -828,10 +840,10 @@
       <c r="H3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="4"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -849,10 +861,10 @@
       <c r="H4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="4"/>
+      <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="14"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="5" t="s">
         <v>40</v>
       </c>
@@ -868,10 +880,10 @@
       <c r="H5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="4"/>
+      <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="14"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
@@ -887,10 +899,10 @@
       <c r="H6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="4"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -910,10 +922,10 @@
       <c r="H7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A8" s="14"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
@@ -933,10 +945,10 @@
       <c r="H8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="4"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -954,16 +966,18 @@
       <c r="F9" s="13">
         <v>45719</v>
       </c>
-      <c r="G9" s="11"/>
+      <c r="G9" s="11">
+        <v>45737</v>
+      </c>
       <c r="H9" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>45</v>
+        <v>24</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A10" s="14"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
@@ -979,10 +993,10 @@
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1000,10 +1014,10 @@
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A12" s="14"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
@@ -1019,7 +1033,7 @@
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
@@ -1040,7 +1054,7 @@
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
@@ -1061,7 +1075,7 @@
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
@@ -1076,7 +1090,7 @@
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="5"/>
@@ -1087,7 +1101,7 @@
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="5"/>
@@ -1098,7 +1112,7 @@
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+      <c r="I17" s="5"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="5"/>
@@ -1109,7 +1123,7 @@
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="I18" s="5"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="5"/>
@@ -1120,7 +1134,7 @@
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
+      <c r="I19" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1136,41 +1150,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A2:D3"/>
+  <dimension ref="A2:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.23046875" style="16"/>
-    <col min="2" max="2" width="33.84375" style="15" customWidth="1"/>
-    <col min="3" max="3" width="70.84375" style="17" customWidth="1"/>
-    <col min="4" max="4" width="47.15234375" style="15" customWidth="1"/>
-    <col min="5" max="16384" width="9.23046875" style="15"/>
+    <col min="1" max="1" width="33.84375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="9.23046875" style="15"/>
+    <col min="3" max="3" width="70.84375" style="16" customWidth="1"/>
+    <col min="4" max="4" width="47.15234375" style="14" customWidth="1"/>
+    <col min="5" max="16384" width="9.23046875" style="14"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="116.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="16">
+      <c r="A2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="15">
         <v>45723</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="C2" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="14" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="C3" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="D3" s="14" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="409.6" x14ac:dyDescent="0.4">
+      <c r="B4" s="15">
+        <v>45728</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>47</v>
-      </c>
-      <c r="D2" s="15" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="C3" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="15" t="e" vm="2">
-        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: enhance get_sample_data and signal_buffering functions to include channel number, add lpf signal verification functionality
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5503B0-26F9-433D-9D18-18819EBFE3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8131C244-3C50-48BE-AC58-9E05A003DBCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21840" yWindow="1217" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
@@ -235,7 +235,7 @@
 3. the buffering logic of Daryl's MATLAB code had a error, because matlab does not use 0 indexing, the buffer size was set to 1000 but the buffer was processing 1001 signals in everytime except the first buffer. </t>
   </si>
   <si>
-    <t>May need to adjust later. Currently copied wrong logic in Daryl's project to get same results</t>
+    <t>May need to adjust later. Currently copied wrong logic in Daryl's project to get same results. Also the result have a average difference of 3.64e-11 compared to the daryl's results</t>
   </si>
 </sst>
 </file>
@@ -774,7 +774,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -947,7 +947,7 @@
       </c>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A9" s="17" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
feat: improve error messages in highpass_filter and apply_padding functions, and free allocated memory in main
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8131C244-3C50-48BE-AC58-9E05A003DBCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D33B3D38-03A1-4BDD-ACFD-E23FF9212854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21840" yWindow="1217" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
     <sheet name="Journal" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t>Import file</t>
   </si>
@@ -236,6 +237,19 @@
   </si>
   <si>
     <t>May need to adjust later. Currently copied wrong logic in Daryl's project to get same results. Also the result have a average difference of 3.64e-11 compared to the daryl's results</t>
+  </si>
+  <si>
+    <t>high pass filtering functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logic of the high pass filter was not the same with the low pass filter. It was as below.
+1. Daryls code layer
+- padding was 50 front and back, not like 60 in the low pass filter
+- pass on to MATLAB built in conv() function with padded signal and coefficients(which was imported from fir_51.mat file in the project)
+2. Matlab Layer
+- the conv function just did a 1d convolution with the signal samples and coeffs.
+Logic was simple so was easy and straight forward so simple to recreate.
+Although I am curious on why the logic was different in both filterings. According to the full report, both just used fir filtering and didnt mention different paddings and post signal zero padding and pre removal were used. I wonder if this is why some misdetections and </t>
   </si>
 </sst>
 </file>
@@ -773,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1150,10 +1164,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A2:D4"/>
+  <dimension ref="A2:D5"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1195,6 +1209,17 @@
         <v>47</v>
       </c>
     </row>
+    <row r="5" spans="1:4" ht="189.45" x14ac:dyDescent="0.4">
+      <c r="A5" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="15">
+        <v>45730</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
start artifact detection functionailtiy.
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D33B3D38-03A1-4BDD-ACFD-E23FF9212854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349665CA-AA9A-4191-99D8-163199440E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
     <sheet name="Journal" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -787,7 +786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1166,7 +1165,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
   <dimension ref="A2:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed high pass filtering conv wrong implementation.
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349665CA-AA9A-4191-99D8-163199440E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0FB725-B0CE-40AD-B15C-ABB404A2DD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>Import file</t>
   </si>
@@ -241,14 +241,17 @@
     <t>high pass filtering functionality</t>
   </si>
   <si>
-    <t xml:space="preserve">logic of the high pass filter was not the same with the low pass filter. It was as below.
+    <t>logic of the high pass filter was not the same with the low pass filter. It was as below.
 1. Daryls code layer
 - padding was 50 front and back, not like 60 in the low pass filter
 - pass on to MATLAB built in conv() function with padded signal and coefficients(which was imported from fir_51.mat file in the project)
 2. Matlab Layer
-- the conv function just did a 1d convolution with the signal samples and coeffs.
+- the conv function just did a 1d convolution with the signal samples and coeffs. The conv function adds 50 samples to the signal length, which seems to be how convolution works.
 Logic was simple so was easy and straight forward so simple to recreate.
-Although I am curious on why the logic was different in both filterings. According to the full report, both just used fir filtering and didnt mention different paddings and post signal zero padding and pre removal were used. I wonder if this is why some misdetections and </t>
+Although I am curious on why the logic was different in both filterings. According to the full report, both just used fir filtering and didnt mention different paddings and post signal zero padding and pre removal were used. I wonder if this is why some misdetections and glitches</t>
+  </si>
+  <si>
+    <t>Artifact Detection</t>
   </si>
 </sst>
 </file>
@@ -787,7 +790,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -797,7 +800,7 @@
     <col min="3" max="3" width="22.4609375" style="2" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="72.23046875" style="2" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="6.4609375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="6.3828125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.53515625" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.23046875" style="9"/>
     <col min="8" max="8" width="9.23046875" style="1"/>
     <col min="9" max="9" width="60.84375" style="2" customWidth="1"/>
@@ -980,7 +983,7 @@
         <v>45719</v>
       </c>
       <c r="G9" s="11">
-        <v>45737</v>
+        <v>45730</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>24</v>
@@ -1003,7 +1006,9 @@
       <c r="E10" s="13">
         <v>45722</v>
       </c>
-      <c r="F10" s="11"/>
+      <c r="F10" s="11">
+        <v>45730</v>
+      </c>
       <c r="G10" s="11"/>
       <c r="H10" s="4"/>
       <c r="I10" s="5"/>
@@ -1163,10 +1168,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A2:D5"/>
+  <dimension ref="A2:D6"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1208,7 +1213,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="189.45" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="218.6" x14ac:dyDescent="0.4">
       <c r="A5" s="14" t="s">
         <v>49</v>
       </c>
@@ -1217,6 +1222,14 @@
       </c>
       <c r="C5" s="16" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="15">
+        <v>45733</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: enhance artifact detection and removal functionality, update Makefile for cross-platform compatibility, and improve result checking output
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0FB725-B0CE-40AD-B15C-ABB404A2DD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF51440-2B30-4621-A4F6-9EFDE5098C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="2066" yWindow="-12189" windowWidth="8931" windowHeight="9455" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
   <si>
     <t>Import file</t>
   </si>
@@ -251,7 +251,13 @@
 Although I am curious on why the logic was different in both filterings. According to the full report, both just used fir filtering and didnt mention different paddings and post signal zero padding and pre removal were used. I wonder if this is why some misdetections and glitches</t>
   </si>
   <si>
-    <t>Artifact Detection</t>
+    <t>The detecting artifact logic is simple, just getting the highest value that is over the threashold, which is a static value. This is concerning. Larrisa's full report mentiones(page9) that the threshold must be manually tuned for each patients as the amplitude of the pacing artifacts varied in defferent datasets.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artifact Detection </t>
+  </si>
+  <si>
+    <t>ongoing</t>
   </si>
 </sst>
 </file>
@@ -789,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1009,8 +1015,12 @@
       <c r="F10" s="11">
         <v>45730</v>
       </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="4"/>
+      <c r="G10" s="11">
+        <v>45734</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
@@ -1029,9 +1039,13 @@
       <c r="E11" s="13">
         <v>45726</v>
       </c>
-      <c r="F11" s="11"/>
+      <c r="F11" s="11">
+        <v>45734</v>
+      </c>
       <c r="G11" s="11"/>
-      <c r="H11" s="4"/>
+      <c r="H11" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
@@ -1170,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
   <dimension ref="A2:D6"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1224,12 +1238,15 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A6" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B6" s="15">
         <v>45733</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: finish neo_transform function and adjust artifact removal verification
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF51440-2B30-4621-A4F6-9EFDE5098C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5291854-379A-4906-8771-6CBBE37D2FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2066" yWindow="-12189" windowWidth="8931" windowHeight="9455" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
   <si>
     <t>Import file</t>
   </si>
@@ -235,9 +235,6 @@
 3. the buffering logic of Daryl's MATLAB code had a error, because matlab does not use 0 indexing, the buffer size was set to 1000 but the buffer was processing 1001 signals in everytime except the first buffer. </t>
   </si>
   <si>
-    <t>May need to adjust later. Currently copied wrong logic in Daryl's project to get same results. Also the result have a average difference of 3.64e-11 compared to the daryl's results</t>
-  </si>
-  <si>
     <t>high pass filtering functionality</t>
   </si>
   <si>
@@ -257,7 +254,25 @@
     <t xml:space="preserve">Artifact Detection </t>
   </si>
   <si>
-    <t>ongoing</t>
+    <t>NEO Transform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The NEO transform in the MATLAB code works as follows.
+- creates a array of 1s
+- assigns the Neo transform output value starting the 2nd index of the array(which means the 1st index is still 1)
+While recreating the NEO transform functionality, ran in to memory errors. Found out that the MATLAB's NEO transform function output [input -1] values. Investigated this and look like it is common in NEO transforms due to how it is calculated. The values that was removed in the output was the last value, which is 1. </t>
+  </si>
+  <si>
+    <t>May need to adjust later. Currently copied wrong logic in Daryl's project to get same results. Also the result have a average difference of 3.64e-11 compared to the daryl's results. Largest diffence was 1e-8. PERCISION constant of PRECISION to 1e-8</t>
+  </si>
+  <si>
+    <t>Changed PRECISION to 1e-7 because the max diff between matlab and C increased</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changed PRECISION to 1e-6 because the max diff between matlab and C increased. </t>
+  </si>
+  <si>
+    <t>Max Average Filtering</t>
   </si>
 </sst>
 </file>
@@ -793,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -969,7 +984,7 @@
       </c>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
@@ -995,7 +1010,7 @@
         <v>24</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
@@ -1021,7 +1036,9 @@
       <c r="H10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A11" s="17" t="s">
@@ -1042,67 +1059,65 @@
       <c r="F11" s="11">
         <v>45734</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G11" s="11">
+        <v>45734</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="17"/>
       <c r="B12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="13">
-        <v>45729</v>
-      </c>
-      <c r="F12" s="11"/>
+        <v>57</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="11">
+        <v>45734</v>
+      </c>
       <c r="G12" s="11"/>
       <c r="H12" s="4"/>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A13" s="5" t="s">
-        <v>12</v>
-      </c>
+    <row r="13" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A13" s="17"/>
       <c r="B13" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E13" s="13">
-        <v>45733</v>
+        <v>45729</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="4"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E14" s="13">
-        <v>45736</v>
+        <v>45733</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
@@ -1111,25 +1126,35 @@
     </row>
     <row r="15" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="E15" s="13">
-        <v>45740</v>
+        <v>45736</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="4"/>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A16" s="5"/>
+    <row r="16" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A16" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="E16" s="13">
+        <v>45740</v>
+      </c>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="4"/>
@@ -1168,11 +1193,22 @@
       <c r="H19" s="4"/>
       <c r="I19" s="5"/>
     </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A11:A13"/>
     <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1182,10 +1218,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A2:D6"/>
+  <dimension ref="A2:D7"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1229,24 +1265,35 @@
     </row>
     <row r="5" spans="1:4" ht="218.6" x14ac:dyDescent="0.4">
       <c r="A5" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="15">
         <v>45730</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A6" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="15">
         <v>45733</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="116.6" x14ac:dyDescent="0.4">
+      <c r="A7" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="15">
+        <v>45734</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: implement moving average filtering function and update NEO transform documentation
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5291854-379A-4906-8771-6CBBE37D2FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0646CAC-AAE3-4349-AD86-D342F626EFC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
   <si>
     <t>Import file</t>
   </si>
@@ -273,6 +273,12 @@
   </si>
   <si>
     <t>Max Average Filtering</t>
+  </si>
+  <si>
+    <t>Moving Average Filtering</t>
+  </si>
+  <si>
+    <t>Incountered unmatching result while creating this, where the reason was due to skiping of 1st index value during the calculation. This is connected to The adding of 1 in front of the output signals in NEO transform. If NEO transform later gets rid of the 1 value in the front of the signal, this may need to be fixed with it.(moving_average_filtering function in activation_detection.c)</t>
   </si>
 </sst>
 </file>
@@ -811,7 +817,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1080,8 +1086,12 @@
       <c r="F12" s="11">
         <v>45734</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="4"/>
+      <c r="G12" s="11">
+        <v>45734</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>24</v>
+      </c>
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
@@ -1218,10 +1228,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A2:D7"/>
+  <dimension ref="A2:D8"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1296,6 +1306,17 @@
         <v>53</v>
       </c>
     </row>
+    <row r="8" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A8" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="15">
+        <v>45734</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: update comments in moving average filtering function for clarity and future refactoring
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0646CAC-AAE3-4349-AD86-D342F626EFC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B105590A-5889-4DFA-9861-BA195A39F709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="1800" yWindow="-13817" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
   <si>
     <t>Import file</t>
   </si>
@@ -220,9 +220,52 @@
     <t>I got it to get similar result but not exactly the same. I think it may be because I am using floats instead of double in my C code, Matlab uses double. Plan to change to double next</t>
   </si>
   <si>
-    <t xml:space="preserve">Figured out the problem from deeply investigating the daryl's MATLAB project's lowpass filter logic and reading documentations of how the built in filter() function works. Found out the following.
+    <t>high pass filtering functionality</t>
+  </si>
+  <si>
+    <t>logic of the high pass filter was not the same with the low pass filter. It was as below.
+1. Daryls code layer
+- padding was 50 front and back, not like 60 in the low pass filter
+- pass on to MATLAB built in conv() function with padded signal and coefficients(which was imported from fir_51.mat file in the project)
+2. Matlab Layer
+- the conv function just did a 1d convolution with the signal samples and coeffs. The conv function adds 50 samples to the signal length, which seems to be how convolution works.
+Logic was simple so was easy and straight forward so simple to recreate.
+Although I am curious on why the logic was different in both filterings. According to the full report, both just used fir filtering and didnt mention different paddings and post signal zero padding and pre removal were used. I wonder if this is why some misdetections and glitches</t>
+  </si>
+  <si>
+    <t>The detecting artifact logic is simple, just getting the highest value that is over the threashold, which is a static value. This is concerning. Larrisa's full report mentiones(page9) that the threshold must be manually tuned for each patients as the amplitude of the pacing artifacts varied in defferent datasets.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artifact Detection </t>
+  </si>
+  <si>
+    <t>NEO Transform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The NEO transform in the MATLAB code works as follows.
+- creates a array of 1s
+- assigns the Neo transform output value starting the 2nd index of the array(which means the 1st index is still 1)
+While recreating the NEO transform functionality, ran in to memory errors. Found out that the MATLAB's NEO transform function output [input -1] values. Investigated this and look like it is common in NEO transforms due to how it is calculated. The values that was removed in the output was the last value, which is 1. </t>
+  </si>
+  <si>
+    <t>Changed PRECISION to 1e-7 because the max diff between matlab and C increased</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changed PRECISION to 1e-6 because the max diff between matlab and C increased. </t>
+  </si>
+  <si>
+    <t>Max Average Filtering</t>
+  </si>
+  <si>
+    <t>Moving Average Filtering</t>
+  </si>
+  <si>
+    <t>May need to adjust later. Currently copied wrong logic in Daryl's project to get same results. Also the result have a average difference of 3.64e-11 compared to the daryl's results. Largest diffence was 1e-8. PERCISION constant of PRECISION to 1e-8 was set to check the difference of MATLAB and C output. if difference is greated that PRECISION, error will occur</t>
+  </si>
+  <si>
+    <t>Figured out the problem from deeply investigating the daryl's MATLAB project's lowpass filter logic and reading documentations of how the built in filter() function works. Found out the following.
 1. In Daryl's code layer
-- 60 padding front and back added to signal(first value for front 600 values and end value for back 60 values)
+- 60 padding front and back added to signal(first value for front 60 values and end value for back 60 values)
 - then it is passed to built in lowpass function
 - then the paddings are removed front and back from the output signal from the lowpass function
 2. MATLAB Layer
@@ -232,53 +275,27 @@
 The logic was implimented in the code exactly as the logic above although was still not showing exact result and the reason was below.
 1. Coefficients used in the builtin MATLAB filter() function was not the same as fir_51.mat file in Daryl's project. I found the actual coefficients used in the opts variable that was used in runtime within the lowpass() builtin function. 59 was the number of coefficients that was actually used and the values were also different. 
 2. The filter order != number of coefficients, but was  filter order == number of coefficients - 1, which was 29 in this case
-3. the buffering logic of Daryl's MATLAB code had a error, because matlab does not use 0 indexing, the buffer size was set to 1000 but the buffer was processing 1001 signals in everytime except the first buffer. </t>
-  </si>
-  <si>
-    <t>high pass filtering functionality</t>
-  </si>
-  <si>
-    <t>logic of the high pass filter was not the same with the low pass filter. It was as below.
-1. Daryls code layer
-- padding was 50 front and back, not like 60 in the low pass filter
-- pass on to MATLAB built in conv() function with padded signal and coefficients(which was imported from fir_51.mat file in the project)
-2. Matlab Layer
-- the conv function just did a 1d convolution with the signal samples and coeffs. The conv function adds 50 samples to the signal length, which seems to be how convolution works.
-Logic was simple so was easy and straight forward so simple to recreate.
-Although I am curious on why the logic was different in both filterings. According to the full report, both just used fir filtering and didnt mention different paddings and post signal zero padding and pre removal were used. I wonder if this is why some misdetections and glitches</t>
-  </si>
-  <si>
-    <t>The detecting artifact logic is simple, just getting the highest value that is over the threashold, which is a static value. This is concerning. Larrisa's full report mentiones(page9) that the threshold must be manually tuned for each patients as the amplitude of the pacing artifacts varied in defferent datasets.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Artifact Detection </t>
-  </si>
-  <si>
-    <t>NEO Transform</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The NEO transform in the MATLAB code works as follows.
-- creates a array of 1s
-- assigns the Neo transform output value starting the 2nd index of the array(which means the 1st index is still 1)
-While recreating the NEO transform functionality, ran in to memory errors. Found out that the MATLAB's NEO transform function output [input -1] values. Investigated this and look like it is common in NEO transforms due to how it is calculated. The values that was removed in the output was the last value, which is 1. </t>
-  </si>
-  <si>
-    <t>May need to adjust later. Currently copied wrong logic in Daryl's project to get same results. Also the result have a average difference of 3.64e-11 compared to the daryl's results. Largest diffence was 1e-8. PERCISION constant of PRECISION to 1e-8</t>
-  </si>
-  <si>
-    <t>Changed PRECISION to 1e-7 because the max diff between matlab and C increased</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Changed PRECISION to 1e-6 because the max diff between matlab and C increased. </t>
-  </si>
-  <si>
-    <t>Max Average Filtering</t>
-  </si>
-  <si>
-    <t>Moving Average Filtering</t>
-  </si>
-  <si>
-    <t>Incountered unmatching result while creating this, where the reason was due to skiping of 1st index value during the calculation. This is connected to The adding of 1 in front of the output signals in NEO transform. If NEO transform later gets rid of the 1 value in the front of the signal, this may need to be fixed with it.(moving_average_filtering function in activation_detection.c)</t>
+3. the buffering logic of Daryl's MATLAB code had a error, because matlab does not use 0 indexing, the buffer size was set to 1000 but the buffer was processing 1001 signals in everytime except the first buffer. I have set the BUFFER_SIZE constant to 1001 in the C program to mirror the outcome.</t>
+  </si>
+  <si>
+    <t>ongoing</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Incountered unmatching result while creating this, where the reason was due to skiping of 1st index value during the calculation. This is connected to The adding of one value of 1 in front of the output signals in NEO transform. If NEO transform later gets rid of the 1 value in the front of the signal post its operations before it outputs result, this may need to be fixed with it.(moving_average_filtering function in activation_detection.c).
+The full reports didnot specifically mention what the moving average filtering was for and how the calculations were done so solely relied of mirroring the moving_average_1s_window function that was used in the MATLAB project. Therefore, I am not sure if there was a mistake in the logic or everything was intentional.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="3" tint="9.9978637043366805E-2"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mentions of it in Daryl's report page 15 and Larissa's report page10.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -288,7 +305,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,6 +316,13 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="9.9978637043366805E-2"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -814,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -990,7 +1014,7 @@
       </c>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:9" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
@@ -1016,7 +1040,7 @@
         <v>24</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
@@ -1043,7 +1067,7 @@
         <v>24</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
@@ -1072,13 +1096,13 @@
         <v>24</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="17"/>
       <c r="B12" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1108,9 +1132,13 @@
       <c r="E13" s="13">
         <v>45729</v>
       </c>
-      <c r="F13" s="11"/>
+      <c r="F13" s="11">
+        <v>45734</v>
+      </c>
       <c r="G13" s="11"/>
-      <c r="H13" s="4"/>
+      <c r="H13" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
@@ -1180,39 +1208,6 @@
       <c r="G17" s="11"/>
       <c r="H17" s="4"/>
       <c r="I17" s="5"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1230,8 +1225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
   <dimension ref="A2:D8"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1270,51 +1265,51 @@
         <v>45728</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="218.6" x14ac:dyDescent="0.4">
       <c r="A5" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="15">
         <v>45730</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A6" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="15">
         <v>45733</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A7" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="15">
         <v>45734</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A8" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B8" s="15">
         <v>45734</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: enhance edge detection functionality and add 1D convolution helper
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B105590A-5889-4DFA-9861-BA195A39F709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED7AF8C-5D8C-46B8-B872-0DB9E62FF0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1800" yWindow="-13817" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="63">
   <si>
     <t>Import file</t>
   </si>
@@ -296,6 +296,12 @@
       </rPr>
       <t>Mentions of it in Daryl's report page 15 and Larissa's report page10.</t>
     </r>
+  </si>
+  <si>
+    <t>Preprocessing</t>
+  </si>
+  <si>
+    <t>Detection</t>
   </si>
 </sst>
 </file>
@@ -838,310 +844,327 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.23046875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.4609375" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="72.23046875" style="2" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="6.4609375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="6.53515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.23046875" style="9"/>
-    <col min="8" max="8" width="9.23046875" style="1"/>
-    <col min="9" max="9" width="60.84375" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="9.23046875" style="1"/>
+    <col min="1" max="2" width="15.23046875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.4609375" style="2" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="72.23046875" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="6.4609375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="6.53515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.23046875" style="9"/>
+    <col min="9" max="9" width="9.23046875" style="1"/>
+    <col min="10" max="10" width="60.84375" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="9.23046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="26.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="8"/>
-    </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" ht="31.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" s="3" customFormat="1" ht="31.3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
-      <c r="F3" s="11">
-        <v>45708</v>
-      </c>
+      <c r="F3" s="5"/>
       <c r="G3" s="11">
         <v>45708</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="11">
+        <v>45708</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="11">
+      <c r="F4" s="5"/>
+      <c r="G4" s="11">
         <v>45708</v>
       </c>
-      <c r="G4" s="11">
+      <c r="H4" s="11">
         <v>45709</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="17"/>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="11">
-        <v>45716</v>
-      </c>
+      <c r="F5" s="5"/>
       <c r="G5" s="11">
         <v>45716</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="11">
+        <v>45716</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="17"/>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="11">
+      <c r="F6" s="5"/>
+      <c r="G6" s="11">
         <v>45709</v>
       </c>
-      <c r="G6" s="11">
+      <c r="H6" s="11">
         <v>45718</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="11">
-        <v>45709</v>
-      </c>
+      <c r="F7" s="5"/>
       <c r="G7" s="11">
         <v>45709</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="11">
+        <v>45709</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A8" s="17"/>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="11">
-        <v>45709</v>
-      </c>
+      <c r="F8" s="5"/>
       <c r="G8" s="11">
         <v>45709</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="11">
+        <v>45709</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="E9" s="13">
-        <v>45719</v>
       </c>
       <c r="F9" s="13">
         <v>45719</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="13">
+        <v>45719</v>
+      </c>
+      <c r="H9" s="11">
         <v>45730</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="I9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="J9" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A10" s="17"/>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="13">
+      <c r="F10" s="13">
         <v>45722</v>
       </c>
-      <c r="F10" s="11">
+      <c r="G10" s="11">
         <v>45730</v>
       </c>
-      <c r="G10" s="11">
+      <c r="H10" s="11">
         <v>45734</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A11" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="13">
+      <c r="F11" s="13">
         <v>45726</v>
-      </c>
-      <c r="F11" s="11">
-        <v>45734</v>
       </c>
       <c r="G11" s="11">
         <v>45734</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="11">
+        <v>45734</v>
+      </c>
+      <c r="I11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="J11" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="17"/>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="11">
-        <v>45734</v>
-      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="11">
         <v>45734</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="11">
+        <v>45734</v>
+      </c>
+      <c r="I12" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A13" s="17"/>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="13">
+      <c r="F13" s="13">
         <v>45729</v>
       </c>
-      <c r="F13" s="11">
+      <c r="G13" s="11">
         <v>45734</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="11"/>
+      <c r="I13" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
@@ -1149,65 +1172,71 @@
         <v>13</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="13">
+      <c r="F14" s="13">
         <v>45733</v>
       </c>
-      <c r="F14" s="11"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="H14" s="11"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="13">
+      <c r="F15" s="13">
         <v>45736</v>
       </c>
-      <c r="F15" s="11"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="H15" s="11"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="13">
+      <c r="E16" s="5"/>
+      <c r="F16" s="13">
         <v>45740</v>
       </c>
-      <c r="F16" s="11"/>
       <c r="G16" s="11"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H16" s="11"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="11"/>
+      <c r="F17" s="5"/>
       <c r="G17" s="11"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="5"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1225,7 +1254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
   <dimension ref="A2:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix: update comments and clean up edge detection code for clarity
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED7AF8C-5D8C-46B8-B872-0DB9E62FF0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650CC239-D4EE-4CBC-A171-D3DA706125A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="-13817" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
   <si>
     <t>Import file</t>
   </si>
@@ -302,6 +302,17 @@
   </si>
   <si>
     <t>Detection</t>
+  </si>
+  <si>
+    <t>Odd implimentations of skiping the first sample of the filtered signal during conv encountered in the MATLAB code</t>
+  </si>
+  <si>
+    <t>Logic of alg of edge detection is as below.
+1. convolve the artifact removed(before neo transformed) signal and kernel of [-1, 0, 1]
+2. convolve the output of step 1 and the neo filtered(after maf) signal
+3. negative values in the output of step 2, is set to 0, and all the positive values are set to the squared value of itself 
+4. get the mean of output of step 3 and set all the values of output of 3, that are less than the mean value to 0
+Ran into some issues during creating this in C due to step 2. In this stage the output of step one is 1 signal larger that the neo filtered signal which seems to be a connected issue from the neo transfrom stage. In the matlab code to solve this, it seems the first value of the convolved signal is skipped the conv of step 2. These signals maybe not relevant since they are few values that are in the front and end of the buffer, but I worry these small differences building up create bigger issue in the activation detection.</t>
   </si>
 </sst>
 </file>
@@ -388,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -439,6 +450,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -846,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1158,11 +1172,15 @@
       <c r="G13" s="11">
         <v>45734</v>
       </c>
-      <c r="H13" s="11"/>
+      <c r="H13" s="11">
+        <v>45736</v>
+      </c>
       <c r="I13" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="J13" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
@@ -1183,9 +1201,13 @@
       <c r="F14" s="13">
         <v>45733</v>
       </c>
-      <c r="G14" s="11"/>
+      <c r="G14" s="11">
+        <v>45736</v>
+      </c>
       <c r="H14" s="11"/>
-      <c r="I14" s="4"/>
+      <c r="I14" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
@@ -1252,23 +1274,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A2:D8"/>
+  <dimension ref="A2:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="33.84375" style="14" customWidth="1"/>
+    <col min="1" max="1" width="14.4609375" style="16" customWidth="1"/>
     <col min="2" max="2" width="9.23046875" style="15"/>
-    <col min="3" max="3" width="70.84375" style="16" customWidth="1"/>
+    <col min="3" max="3" width="114.23046875" style="16" customWidth="1"/>
     <col min="4" max="4" width="47.15234375" style="14" customWidth="1"/>
     <col min="5" max="16384" width="9.23046875" style="14"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="116.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="18" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="15">
@@ -1282,6 +1304,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A3" s="18"/>
       <c r="C3" s="16" t="s">
         <v>46</v>
       </c>
@@ -1289,7 +1312,8 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="409.6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="306" x14ac:dyDescent="0.4">
+      <c r="A4" s="18"/>
       <c r="B4" s="15">
         <v>45728</v>
       </c>
@@ -1297,8 +1321,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="218.6" x14ac:dyDescent="0.4">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:4" ht="160.30000000000001" x14ac:dyDescent="0.4">
+      <c r="A5" s="16" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="15">
@@ -1308,8 +1332,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:4" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A6" s="16" t="s">
         <v>50</v>
       </c>
       <c r="B6" s="15">
@@ -1319,8 +1343,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="116.6" x14ac:dyDescent="0.4">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:4" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A7" s="16" t="s">
         <v>51</v>
       </c>
       <c r="B7" s="15">
@@ -1330,8 +1354,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="160.30000000000001" x14ac:dyDescent="0.4">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:4" ht="116.6" x14ac:dyDescent="0.4">
+      <c r="A8" s="16" t="s">
         <v>56</v>
       </c>
       <c r="B8" s="15">
@@ -1341,7 +1365,21 @@
         <v>60</v>
       </c>
     </row>
+    <row r="9" spans="1:4" ht="145.75" x14ac:dyDescent="0.4">
+      <c r="A9" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="15">
+        <v>45736</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: adjust variable types and improve comments for clarity in signal processing functions
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650CC239-D4EE-4CBC-A171-D3DA706125A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A592C8-7C70-4CB8-9A63-55A498732F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -242,16 +242,7 @@
     <t>NEO Transform</t>
   </si>
   <si>
-    <t xml:space="preserve">The NEO transform in the MATLAB code works as follows.
-- creates a array of 1s
-- assigns the Neo transform output value starting the 2nd index of the array(which means the 1st index is still 1)
-While recreating the NEO transform functionality, ran in to memory errors. Found out that the MATLAB's NEO transform function output [input -1] values. Investigated this and look like it is common in NEO transforms due to how it is calculated. The values that was removed in the output was the last value, which is 1. </t>
-  </si>
-  <si>
     <t>Changed PRECISION to 1e-7 because the max diff between matlab and C increased</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Changed PRECISION to 1e-6 because the max diff between matlab and C increased. </t>
   </si>
   <si>
     <t>Max Average Filtering</t>
@@ -281,6 +272,49 @@
     <t>ongoing</t>
   </si>
   <si>
+    <t>Preprocessing</t>
+  </si>
+  <si>
+    <t>Detection</t>
+  </si>
+  <si>
+    <t>Logic of alg of edge detection is as below.
+1. convolve the artifact removed(before neo transformed) signal and kernel of [-1, 0, 1]
+2. convolve the output of step 1 and the neo filtered(after maf) signal
+3. negative values in the output of step 2, is set to 0, and all the positive values are set to the squared value of itself 
+4. get the mean of output of step 3 and set all the values of output of 3, that are less than the mean value to 0
+Ran into some issues during creating this in C due to step 2. In this stage the output of step one is 1 signal larger that the neo filtered signal which seems to be a connected issue from the neo transfrom stage. In the matlab code to solve this, it seems the first value of the convolved signal is skipped the conv of step 2. These signals maybe not relevant since they are few values that are in the front and end of the buffer, but I worry these small differences building up create bigger issue in the activation detection.</t>
+  </si>
+  <si>
+    <r>
+      <t>The NEO transform in the MATLAB code works as follows.
+- creates a array of 1s
+- assigns the Neo transform output value starting the 2nd index of the array(which means the 1st index is still 1)
+While recreating the NEO transform functionality, ran in to memory errors. Found out that the MATLAB's NEO transform function output [input -1] values. Investigated this and look like it is common in NEO transforms due to how it is calculated. The values that was removed in the output was the last value, which is 1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>refer to  neo_transform function in detection.c</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Incountered unmatching result while creating this, where the reason was due to skiping of 1st index value during the calculation. This is connected to The adding of one value of 1 in front of the output signals in NEO transform. If NEO transform later gets rid of the 1 value in the front of the signal post its operations before it outputs result, this may need to be fixed with it.(moving_average_filtering function in activation_detection.c).
 The full reports didnot specifically mention what the moving average filtering was for and how the calculations were done so solely relied of mirroring the moving_average_1s_window function that was used in the MATLAB project. Therefore, I am not sure if there was a mistake in the logic or everything was intentional.
@@ -288,6 +322,7 @@
     </r>
     <r>
       <rPr>
+        <i/>
         <sz val="11"/>
         <color theme="3" tint="9.9978637043366805E-2"/>
         <rFont val="Aptos Narrow"/>
@@ -298,21 +333,10 @@
     </r>
   </si>
   <si>
-    <t>Preprocessing</t>
-  </si>
-  <si>
-    <t>Detection</t>
-  </si>
-  <si>
-    <t>Odd implimentations of skiping the first sample of the filtered signal during conv encountered in the MATLAB code</t>
-  </si>
-  <si>
-    <t>Logic of alg of edge detection is as below.
-1. convolve the artifact removed(before neo transformed) signal and kernel of [-1, 0, 1]
-2. convolve the output of step 1 and the neo filtered(after maf) signal
-3. negative values in the output of step 2, is set to 0, and all the positive values are set to the squared value of itself 
-4. get the mean of output of step 3 and set all the values of output of 3, that are less than the mean value to 0
-Ran into some issues during creating this in C due to step 2. In this stage the output of step one is 1 signal larger that the neo filtered signal which seems to be a connected issue from the neo transfrom stage. In the matlab code to solve this, it seems the first value of the convolved signal is skipped the conv of step 2. These signals maybe not relevant since they are few values that are in the front and end of the buffer, but I worry these small differences building up create bigger issue in the activation detection.</t>
+    <t>Changed PRECISION to 1e-6 because the max diff between matlab and C increased.  Odd implimentations in MATLAB code which was mirrored in the C code</t>
+  </si>
+  <si>
+    <t>Odd implimentations of skiping the first sample of the filtered signal during conv encountered in the MATLAB code. Seems to be connected with the odd implimentation in the neo transform</t>
   </si>
 </sst>
 </file>
@@ -322,7 +346,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,6 +362,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="3" tint="9.9978637043366805E-2"/>
       <name val="Aptos Narrow"/>
@@ -860,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1047,7 +1087,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>3</v>
@@ -1071,7 +1111,7 @@
         <v>24</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="43.75" x14ac:dyDescent="0.4">
@@ -1099,15 +1139,15 @@
         <v>24</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A11" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>8</v>
@@ -1131,14 +1171,14 @@
         <v>24</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="17"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1154,7 +1194,7 @@
       </c>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A13" s="17"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
@@ -1179,7 +1219,7 @@
         <v>24</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="43.75" x14ac:dyDescent="0.4">
@@ -1206,7 +1246,7 @@
       </c>
       <c r="H14" s="11"/>
       <c r="I14" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J14" s="5"/>
     </row>
@@ -1276,8 +1316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
   <dimension ref="A2:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1289,7 +1329,7 @@
     <col min="5" max="16384" width="9.23046875" style="14"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="116.6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A2" s="18" t="s">
         <v>44</v>
       </c>
@@ -1303,7 +1343,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A3" s="18"/>
       <c r="C3" s="16" t="s">
         <v>46</v>
@@ -1318,7 +1358,7 @@
         <v>45728</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="160.30000000000001" x14ac:dyDescent="0.4">
@@ -1351,18 +1391,18 @@
         <v>45734</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A8" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8" s="15">
         <v>45734</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="145.75" x14ac:dyDescent="0.4">
@@ -1373,7 +1413,7 @@
         <v>45736</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: enhance activation checking and verification processes; update function signatures and improve memory management
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A592C8-7C70-4CB8-9A63-55A498732F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3277A3-D867-4349-8848-9CFE4040C1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="38280" yWindow="-2910" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
   <si>
     <t>Import file</t>
   </si>
@@ -267,9 +267,6 @@
 1. Coefficients used in the builtin MATLAB filter() function was not the same as fir_51.mat file in Daryl's project. I found the actual coefficients used in the opts variable that was used in runtime within the lowpass() builtin function. 59 was the number of coefficients that was actually used and the values were also different. 
 2. The filter order != number of coefficients, but was  filter order == number of coefficients - 1, which was 29 in this case
 3. the buffering logic of Daryl's MATLAB code had a error, because matlab does not use 0 indexing, the buffer size was set to 1000 but the buffer was processing 1001 signals in everytime except the first buffer. I have set the BUFFER_SIZE constant to 1001 in the C program to mirror the outcome.</t>
-  </si>
-  <si>
-    <t>ongoing</t>
   </si>
   <si>
     <t>Preprocessing</t>
@@ -315,28 +312,27 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Incountered unmatching result while creating this, where the reason was due to skiping of 1st index value during the calculation. This is connected to The adding of one value of 1 in front of the output signals in NEO transform. If NEO transform later gets rid of the 1 value in the front of the signal post its operations before it outputs result, this may need to be fixed with it.(moving_average_filtering function in activation_detection.c).
-The full reports didnot specifically mention what the moving average filtering was for and how the calculations were done so solely relied of mirroring the moving_average_1s_window function that was used in the MATLAB project. Therefore, I am not sure if there was a mistake in the logic or everything was intentional.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="3" tint="9.9978637043366805E-2"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Mentions of it in Daryl's report page 15 and Larissa's report page10.</t>
-    </r>
-  </si>
-  <si>
     <t>Changed PRECISION to 1e-6 because the max diff between matlab and C increased.  Odd implimentations in MATLAB code which was mirrored in the C code</t>
   </si>
   <si>
     <t>Odd implimentations of skiping the first sample of the filtered signal during conv encountered in the MATLAB code. Seems to be connected with the odd implimentation in the neo transform</t>
+  </si>
+  <si>
+    <t>Refatoring</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After finishing activation detection functionality, I've encountered that the good signal datasets were not outputting same results as the MATLAB project. I've been testing with the bad signal datasets only to check the c program outputs during the recreation process. After long investigation, I found the below was the issue.
+1. Good signal datasets had opposite orientation(channel = row, samples=col) 
+2. The MATLAB's built-in lowpass function used in the MATLAB project was dynamically creating the coefficents used in the filtering process
+This means that the C lowpass functionality also needs to create coeffs dynamically too. I still have to analyse how it does it and what component is uses for the calulations(sample freq, signal length, etc).  </t>
+  </si>
+  <si>
+    <t>Encountered unmatching result while creating this, where the reason was due to skipping of 1st index value during the calculation. This is connected to The adding of one value of 1 in front of the output signals in NEO transform. If NEO transform later gets rid of the 1 value in the front of the signal post its operations before it outputs result, this may need to be fixed with it.(moving_average_filtering function in activation_detection.c).
+The full reports did not specifically mention what the moving average filtering was for and how the calculations were done so solely relied of mirroring the moving_average_1s_window function that was used in the MATLAB project. Therefore, I am not sure if there was a mistake in the logic or everything was intentional.
+Mentions of it in Daryl's report page 15 and Larissa's report page10.</t>
   </si>
 </sst>
 </file>
@@ -346,7 +342,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,14 +368,6 @@
       <i/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="3" tint="9.9978637043366805E-2"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -900,8 +888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1087,7 +1075,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>3</v>
@@ -1147,7 +1135,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>8</v>
@@ -1171,7 +1159,7 @@
         <v>24</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
@@ -1219,7 +1207,7 @@
         <v>24</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="43.75" x14ac:dyDescent="0.4">
@@ -1244,9 +1232,11 @@
       <c r="G14" s="11">
         <v>45736</v>
       </c>
-      <c r="H14" s="11"/>
+      <c r="H14" s="11">
+        <v>45736</v>
+      </c>
       <c r="I14" s="4" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="J14" s="5"/>
     </row>
@@ -1267,25 +1257,39 @@
       <c r="F15" s="13">
         <v>45736</v>
       </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="4"/>
+      <c r="G15" s="11">
+        <v>45740</v>
+      </c>
+      <c r="H15" s="11">
+        <v>45740</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="5"/>
+      <c r="B16" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="13">
         <v>45740</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="4"/>
+      <c r="G16" s="11">
+        <v>45740</v>
+      </c>
+      <c r="H16" s="11">
+        <v>45742</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.4">
@@ -1314,10 +1318,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A2:D9"/>
+  <dimension ref="A2:D10"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1391,7 +1395,7 @@
         <v>45734</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="116.6" x14ac:dyDescent="0.4">
@@ -1402,7 +1406,7 @@
         <v>45734</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="145.75" x14ac:dyDescent="0.4">
@@ -1413,7 +1417,18 @@
         <v>45736</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="102" x14ac:dyDescent="0.4">
+      <c r="A10" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="15">
+        <v>45742</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: update verification flags and improve logging in signal processing functions
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3277A3-D867-4349-8848-9CFE4040C1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA995CB-957A-441B-956C-78613A8422ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-2910" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="38280" yWindow="-2910" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
     <sheet name="Journal" sheetId="3" r:id="rId2"/>
+    <sheet name="Results" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1320,7 +1321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
   <dimension ref="A2:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1437,4 +1438,18 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69446ECF-727C-4A2E-AB35-11AEE6EEA4B3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add data feeder implementation for signal processing
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333A2824-4515-4875-8BC3-ADB1588F796D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BC404D-85E0-4083-B1DC-2698EE36F5FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-77" yWindow="-77" windowWidth="22097" windowHeight="13148" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
     <sheet name="Journal" sheetId="3" r:id="rId2"/>
-    <sheet name="Results" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -70,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
   <si>
     <t>Import file</t>
   </si>
@@ -268,6 +267,9 @@
 1. Coefficients used in the builtin MATLAB filter() function was not the same as fir_51.mat file in Daryl's project. I found the actual coefficients used in the opts variable that was used in runtime within the lowpass() builtin function. 59 was the number of coefficients that was actually used and the values were also different. 
 2. The filter order != number of coefficients, but was  filter order == number of coefficients - 1, which was 29 in this case
 3. the buffering logic of Daryl's MATLAB code had a error, because matlab does not use 0 indexing, the buffer size was set to 1000 but the buffer was processing 1001 signals in everytime except the first buffer. I have set the BUFFER_SIZE constant to 1001 in the C program to mirror the outcome.</t>
+  </si>
+  <si>
+    <t>ongoing</t>
   </si>
   <si>
     <t>Preprocessing</t>
@@ -313,117 +315,46 @@
     </r>
   </si>
   <si>
-    <t>Changed PRECISION to 1e-6 because the max diff between matlab and C increased.  Odd implimentations in MATLAB code which was mirrored in the C code</t>
-  </si>
-  <si>
-    <t>Odd implimentations of skiping the first sample of the filtered signal during conv encountered in the MATLAB code. Seems to be connected with the odd implimentation in the neo transform</t>
-  </si>
-  <si>
-    <t xml:space="preserve">After finishing activation detection functionality, I've encountered that the good signal datasets were not outputting same results as the MATLAB project. I've been testing with the bad signal datasets only to check the c program outputs during the recreation process. After long investigation, I found the below was the issue.
-1. Good signal datasets had opposite orientation(channel = row, samples=col) 
-2. The MATLAB's built-in lowpass function used in the MATLAB project was dynamically creating the coefficents used in the filtering process
-This means that the C lowpass functionality also needs to create coeffs dynamically too. I still have to analyse how it does it and what component is uses for the calulations(sample freq, signal length, etc).  </t>
-  </si>
-  <si>
-    <t>Encountered unmatching result while creating this, where the reason was due to skipping of 1st index value during the calculation. This is connected to The adding of one value of 1 in front of the output signals in NEO transform. If NEO transform later gets rid of the 1 value in the front of the signal post its operations before it outputs result, this may need to be fixed with it.(moving_average_filtering function in activation_detection.c).
-The full reports did not specifically mention what the moving average filtering was for and how the calculations were done so solely relied of mirroring the moving_average_1s_window function that was used in the MATLAB project. Therefore, I am not sure if there was a mistake in the logic or everything was intentional.
-Mentions of it in Daryl's report page 15 and Larissa's report page10.</t>
-  </si>
-  <si>
-    <t>Luman Wang's Thesis Chap 5 Review</t>
-  </si>
-  <si>
-    <t>Testing and Refatoring</t>
-  </si>
-  <si>
-    <t>C Program Recreation</t>
-  </si>
-  <si>
-    <t>Pacing Feature Implementation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implement pacing according to state's real time change </t>
-  </si>
-  <si>
-    <t>Implement real time state handling post each activation detection</t>
-  </si>
-  <si>
-    <t>Step 3 - Recreate the MATLAB project with C without using any libraries as possible and run it on desktop(goal is to make it run on a PIC or similar level real time processor so need to be as light and simple as possible)</t>
-  </si>
-  <si>
-    <t>Step 4 - Run program in a microprocessor</t>
-  </si>
-  <si>
-    <t>Modify dataset samples to transmit signals in a set freq</t>
-  </si>
-  <si>
-    <t>Data Initialization</t>
-  </si>
-  <si>
-    <t>Testing &amp; Refactoring</t>
-  </si>
-  <si>
-    <t>I realized after reviewing the pacing algorithm in Dr. Wang's thesis. The MATLAB program was designed to just verify that it filters the data well enough to detect activations from the datasets, which is why it just import the whole dataset file, then buffering through it, then showing result of all the detected activations, then program ends. In order to implement the pacing correction features to the program, it needs process the signals in a frequency as it would in real life, so that I can eventually test the pacing feature if it reacts well according to the state changes. 
-But then again, I may be thinking too much like a industry software engineer. Thinking that the goal of this research is to validate that this program is a valid method, this means that showing results via diagrams and graphs as evidence that this method is valid is the goal here. Maybe modifying the code to actually work in real time is like it would in a real environment is for future work? Then if so, to think like a researcher, the main question I should be asking is, How can the pacing functionality be created for the purpose to validate it is correctly working, not to pace the actual GI track?</t>
-  </si>
-  <si>
-    <t>There was another possible flaw with the signal processing of Daryl and Larissa's project that I realized after realizing the above. From what I understand, the signal processes in buffers of 1000 samples, which is 31.25 seconds at 32 Hz, and slides forward by 500 samples each time, giving a 50% overlap.
-Here's my concern:
-Let’s say the real-time gut signal is coming in continuously. 
-Firstly, 31.25 seconds over the normal activation time of 3cpm(every 20 secs), meaning that, in normal activation scenario, the program will detect an activation after at least 11.25 secs after the next activation of the the actual activation has occurs. Is this right...?
-More over, when processing Buffer A, it takes 31.25 seconds to fill it. We have the 50%(500 samples) overlap, to validate activations near the end of Buffer A which I understand. That means we’re effectively delaying reliable detection of Buffer A’s end activations until Buffer B completes — another 31.25 seconds later.
-So overall, wouldn’t this introduce a minimum latency of over 60 seconds (31.25 + 31.25) before we can respond to certain activation events? A abnormal activation will be detected over a minute later then start pacing. A corrected activation will only be detected after over a minute later, then the pacing will stop. Is that or isn't that too slow real time closed-loop GES? Has this been considered in Daryl's and Larissa's project? I will need to clarify this with Daryl if I have correctly understood it am not missing anything, after clarify with Dr Malik and Dr Wang about it. If this is an issue, i may need to lower buffer to a realistic value, but I am not sure how much process I may need to go through to validate the results, which I personally am not exited about.
-In the mean time, I will start with the next stage.</t>
-  </si>
-  <si>
-    <t>This should be created in a way that it can drive the whole program's timing. For example, if turned off it will run the like it is before, and turned on, operate in a set frequency. This will make test while development much more time efficient.</t>
-  </si>
-  <si>
     <r>
-      <t>I realized that the worst case senario of the above mentioned is wrong. If you think about it, all initial activations detections will be in the last half of the buffer. For example, if there was a activation detections in the first half of the buffer, it means that, that half's samples were already transmitted in to the past buffer, meaning it as already been detected. So taking only the last buffer in to account, worst case senario would be if the activations was in the first sample of the last half of the buffer. For it to be initially detected, it would take half the buffer length samples to be transmitted(31.25/2 secs) to start processing the buffer. And the activation detection feature detects it to be a possible detection and then wait for the next buffer to validate it since it will be in the start of the buffer. (</t>
+      <t xml:space="preserve">Incountered unmatching result while creating this, where the reason was due to skiping of 1st index value during the calculation. This is connected to The adding of one value of 1 in front of the output signals in NEO transform. If NEO transform later gets rid of the 1 value in the front of the signal post its operations before it outputs result, this may need to be fixed with it.(moving_average_filtering function in activation_detection.c).
+The full reports didnot specifically mention what the moving average filtering was for and how the calculations were done so solely relied of mirroring the moving_average_1s_window function that was used in the MATLAB project. Therefore, I am not sure if there was a mistake in the logic or everything was intentional.
+</t>
     </r>
     <r>
       <rPr>
         <i/>
         <sz val="11"/>
-        <color rgb="FFC00000"/>
+        <color theme="3" tint="9.9978637043366805E-2"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Does it have to wait for the next buffer? if it is in the starting edge of the signal, maybe the prior buffer is a more reliable source? Needs to be investigated.</t>
+      <t>Mentions of it in Daryl's report page 15 and Larissa's report page10.</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) The next buffer starts after 500 samples from the prior buffer(another 31.25/2 secs), which means duration of 1000 samples of delay is the worse case.</t>
-    </r>
-  </si>
-  <si>
-    <t>After thinking of the above, I realized the activation state change conditions are not set at the moment, meaning I have to set the conditions. If the conditions of changing to a normal activation is to only change state if activation was detected in the middle 500 samples of the buffer and wait for the next buffer if it was detected in the end of the buffer, this would reduce the worst case delay to about around 23.44 secs, which will be a scenario where activation signal was in the just after the middle 500 samples, or in other words, the start of the last quarter of the buffer.</t>
-  </si>
-  <si>
-    <t>Met with Dr Malik, more confused. I don’t know if my explaination was the issue, but got advice that I might need to modify the algorhythm to a double buffering method, which I have no clue about. I didn’t even know what type of buffering the current method was. Need to do more research about this concepts. 
-Also was told that i donot need to test the datasets on desktop, but just connect it to the gut model instead using simulink. I have to learn what simulink does to understand what this means.</t>
-  </si>
-  <si>
-    <t>What is SIMULINK?</t>
-  </si>
-  <si>
-    <t>Simulink</t>
-  </si>
-  <si>
-    <t>Ive discussed with daryl regarding the buffer window size, the delay and the half buffer sample overlap. I realized that I have been approaching the role of the overlap wrong. I thought for some reason that it was to verify the activation that was in the last half of the buffer. Its partially correct, since if the activation was detected in the last buffer, it wouldnt need verification, it would mean that it detected a activation which needs not verifying. Incase the buffer couldnt detect the activation due to being in the end of the buffer and then it would most definately be detected in the next buffer, since the activation would have been in the end of the first half of the buffer, hence being in the center of the buffer window. 
-Also I now see why the 1000 sample(31.25s) window makes sense. one whole slow wave signal is around 20s. And for the buffers to have the whole signal in it, 1000 samples seem like a good number and the overlap would make it that a slow wave would be within the center of the window if it wasnt on the previous buffer window. And even if the signal was in the edge of the windows, since the part that is essential to activation detection is around only 8s(ave 12 s resting phase), if the first half was is in the buffer window, it will most likely be detected. 
-Thus, the worst case senario would be if the activation occured after #750 sample in the buffer window. that would be (31.25 x 0.25) + (31.25 0.5)s delay since it will be detected in the next buffer window, which is still around 23.44s, but having the activation signal in the start of the slow wave  would make it more likely to be detected in the first buffer window. Hence it would most likely that delay would be less than 20 sec. Although I might have to check if this is okey with Dr. Malik.</t>
-  </si>
-  <si>
-    <t>After some research and asking chatgpt about the current type of processing methodol</t>
+  </si>
+  <si>
+    <t>Changed PRECISION to 1e-6 because the max diff between matlab and C increased.  Odd implimentations in MATLAB code which was mirrored in the C code</t>
+  </si>
+  <si>
+    <t>Odd implimentations of skiping the first sample of the filtered signal during conv encountered in the MATLAB code. Seems to be connected with the odd implimentation in the neo transform</t>
+  </si>
+  <si>
+    <t>Get simulink to communicate with c prog</t>
+  </si>
+  <si>
+    <t>Modify signal processing to work with circular buffering</t>
+  </si>
+  <si>
+    <t>TCP/IP Comm from PC(simulink) to board</t>
+  </si>
+  <si>
+    <t>migrate C prog to arm processor</t>
+  </si>
+  <si>
+    <t>implement pacing algo to C prog in PC the update to ARM processor</t>
+  </si>
+  <si>
+    <t>Migrate to Flexpret</t>
   </si>
 </sst>
 </file>
@@ -433,7 +364,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -466,17 +397,10 @@
     <font>
       <i/>
       <sz val="11"/>
-      <color rgb="FFC00000"/>
+      <color theme="3" tint="9.9978637043366805E-2"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Display"/>
-      <family val="2"/>
-      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="3">
@@ -493,7 +417,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -529,48 +453,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -620,35 +507,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1053,675 +916,444 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView topLeftCell="B15" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.23046875" style="2" customWidth="1"/>
-    <col min="2" max="3" width="10.765625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.23046875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.4609375" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="72.23046875" style="2" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="6.4609375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.53515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.23046875" style="9"/>
-    <col min="11" max="11" width="9.23046875" style="1"/>
-    <col min="12" max="12" width="60.84375" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="9.23046875" style="1"/>
+    <col min="1" max="2" width="15.23046875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.4609375" style="2" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="72.23046875" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="6.4609375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="6.53515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.23046875" style="9"/>
+    <col min="9" max="9" width="9.23046875" style="1"/>
+    <col min="10" max="10" width="60.84375" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="9.23046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="26.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="26.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-    </row>
-    <row r="2" spans="1:12" s="3" customFormat="1" ht="31.3" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:10" s="3" customFormat="1" ht="31.3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="C2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="E2" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="11">
+      <c r="G3" s="11">
         <v>45708</v>
       </c>
-      <c r="J3" s="11">
+      <c r="H3" s="11">
         <v>45708</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="5"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A4" s="24" t="s">
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="s">
         <v>0</v>
       </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="11">
+      <c r="G4" s="11">
         <v>45708</v>
       </c>
-      <c r="J4" s="11">
+      <c r="H4" s="11">
         <v>45709</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="5"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A5" s="24"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="5" t="s">
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A5" s="17"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
         <v>40</v>
       </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="11">
+      <c r="G5" s="11">
         <v>45716</v>
       </c>
-      <c r="J5" s="11">
+      <c r="H5" s="11">
         <v>45716</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="5"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A6" s="24"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="5" t="s">
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A6" s="17"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="11">
+      <c r="G6" s="11">
         <v>45709</v>
       </c>
-      <c r="J6" s="11">
+      <c r="H6" s="11">
         <v>45718</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="5"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A7" s="24" t="s">
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A7" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F7" s="5"/>
-      <c r="G7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="11">
+      <c r="G7" s="11">
         <v>45709</v>
       </c>
-      <c r="J7" s="11">
+      <c r="H7" s="11">
         <v>45709</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="5"/>
-    </row>
-    <row r="8" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A8" s="24"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A8" s="17"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="E8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="11">
+      <c r="F8" s="5"/>
+      <c r="G8" s="11">
         <v>45709</v>
       </c>
-      <c r="J8" s="11">
+      <c r="H8" s="11">
         <v>45709</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L8" s="5"/>
-    </row>
-    <row r="9" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A9" s="24" t="s">
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="18" t="s">
-        <v>57</v>
+      <c r="B9" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="13">
+      <c r="F9" s="13">
         <v>45719</v>
       </c>
-      <c r="I9" s="13">
+      <c r="G9" s="13">
         <v>45719</v>
       </c>
-      <c r="J9" s="11">
+      <c r="H9" s="11">
         <v>45730</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="I9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="J9" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A10" s="24"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
+    <row r="10" spans="1:10" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A10" s="17"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="13">
+      <c r="F10" s="13">
         <v>45722</v>
       </c>
-      <c r="I10" s="11">
+      <c r="G10" s="11">
         <v>45730</v>
       </c>
-      <c r="J10" s="11">
+      <c r="H10" s="11">
         <v>45734</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A11" s="24" t="s">
+    <row r="11" spans="1:10" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A11" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="18" t="s">
-        <v>58</v>
+      <c r="B11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="13">
+      <c r="F11" s="13">
         <v>45726</v>
       </c>
-      <c r="I11" s="11">
+      <c r="G11" s="11">
         <v>45734</v>
       </c>
-      <c r="J11" s="11">
+      <c r="H11" s="11">
         <v>45734</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="I11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A12" s="24"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="5" t="s">
+      <c r="J11" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A12" s="17"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="11">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="11">
         <v>45734</v>
       </c>
-      <c r="J12" s="11">
+      <c r="H12" s="11">
         <v>45734</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="I12" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="L12" s="5"/>
-    </row>
-    <row r="13" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A13" s="24"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A13" s="17"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="13">
+      <c r="F13" s="13">
         <v>45729</v>
       </c>
-      <c r="I13" s="11">
+      <c r="G13" s="11">
         <v>45734</v>
       </c>
-      <c r="J13" s="11">
+      <c r="H13" s="11">
         <v>45736</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L13" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="J13" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="18" t="s">
+      <c r="B14" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="C14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="13">
+      <c r="F14" s="13">
         <v>45733</v>
       </c>
-      <c r="I14" s="11">
+      <c r="G14" s="11">
         <v>45736</v>
       </c>
-      <c r="J14" s="11">
-        <v>45736</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L14" s="5"/>
-    </row>
-    <row r="15" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="H14" s="11"/>
+      <c r="I14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="13">
+      <c r="F15" s="13">
         <v>45736</v>
       </c>
-      <c r="I15" s="11">
-        <v>45740</v>
-      </c>
-      <c r="J15" s="11">
-        <v>45740</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L15" s="5"/>
-    </row>
-    <row r="16" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="5" t="s">
-        <v>66</v>
-      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="13">
+      <c r="F16" s="13">
         <v>45740</v>
       </c>
-      <c r="I16" s="11">
-        <v>45740</v>
-      </c>
-      <c r="J16" s="11">
-        <v>45742</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L16" s="5"/>
-    </row>
-    <row r="17" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A17" s="17"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>73</v>
-      </c>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="13">
-        <v>45744</v>
-      </c>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A18" s="17"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="5" t="s">
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="19" spans="1:10" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A21" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A24" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="13">
-        <v>45748</v>
-      </c>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="5"/>
-    </row>
-    <row r="19" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A19" s="17"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="13">
-        <v>45720</v>
-      </c>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="5"/>
-    </row>
-    <row r="20" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A20" s="17"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="5"/>
-    </row>
-    <row r="21" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A21" s="17"/>
-      <c r="B21" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="5"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A22" s="17"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="5"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A23" s="17"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="5"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="5"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="5"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="5"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="5"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="5"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="5"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="4">
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="C3:C16"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="B3:B20"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D4:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1730,15 +1362,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A2:D18"/>
+  <dimension ref="A2:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.4609375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.4609375" style="16" customWidth="1"/>
     <col min="2" max="2" width="9.23046875" style="15"/>
     <col min="3" max="3" width="114.23046875" style="16" customWidth="1"/>
     <col min="4" max="4" width="47.15234375" style="14" customWidth="1"/>
@@ -1746,7 +1378,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="18" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="15">
@@ -1760,7 +1392,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A3" s="25"/>
+      <c r="A3" s="18"/>
       <c r="C3" s="16" t="s">
         <v>46</v>
       </c>
@@ -1769,7 +1401,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="306" x14ac:dyDescent="0.4">
-      <c r="A4" s="25"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="15">
         <v>45728</v>
       </c>
@@ -1778,7 +1410,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="160.30000000000001" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="16" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="15">
@@ -1789,7 +1421,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="16" t="s">
         <v>50</v>
       </c>
       <c r="B6" s="15">
@@ -1800,134 +1432,42 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="16" t="s">
         <v>51</v>
       </c>
       <c r="B7" s="15">
         <v>45734</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="116.6" x14ac:dyDescent="0.4">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="16" t="s">
         <v>54</v>
       </c>
       <c r="B8" s="15">
         <v>45734</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="145.75" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="16" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="15">
         <v>45736</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="102" x14ac:dyDescent="0.4">
-      <c r="A10" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B10" s="15">
-        <v>45742</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="160.30000000000001" x14ac:dyDescent="0.4">
-      <c r="A11" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" s="15">
-        <v>45743</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="291.45" x14ac:dyDescent="0.4">
-      <c r="A12" s="25"/>
-      <c r="B12" s="15">
-        <v>45743</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="116.6" x14ac:dyDescent="0.4">
-      <c r="B13" s="15">
-        <v>45743</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="B14" s="15">
-        <v>45743</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="233.15" x14ac:dyDescent="0.4">
-      <c r="B15" s="15">
-        <v>45747</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="B16" s="15">
-        <v>45747</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B17" s="15">
-        <v>45748</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A18" s="2" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A11:A12"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69446ECF-727C-4A2E-AB35-11AEE6EEA4B3}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update: modify progress.xlsx with new data
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333A2824-4515-4875-8BC3-ADB1588F796D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F156A8E5-FA91-4ADB-B78A-B97B622222F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-77" yWindow="-77" windowWidth="22097" windowHeight="13148" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="98">
   <si>
     <t>Import file</t>
   </si>
@@ -336,27 +336,6 @@
     <t>Testing and Refatoring</t>
   </si>
   <si>
-    <t>C Program Recreation</t>
-  </si>
-  <si>
-    <t>Pacing Feature Implementation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implement pacing according to state's real time change </t>
-  </si>
-  <si>
-    <t>Implement real time state handling post each activation detection</t>
-  </si>
-  <si>
-    <t>Step 3 - Recreate the MATLAB project with C without using any libraries as possible and run it on desktop(goal is to make it run on a PIC or similar level real time processor so need to be as light and simple as possible)</t>
-  </si>
-  <si>
-    <t>Step 4 - Run program in a microprocessor</t>
-  </si>
-  <si>
-    <t>Modify dataset samples to transmit signals in a set freq</t>
-  </si>
-  <si>
     <t>Data Initialization</t>
   </si>
   <si>
@@ -374,9 +353,6 @@
 More over, when processing Buffer A, it takes 31.25 seconds to fill it. We have the 50%(500 samples) overlap, to validate activations near the end of Buffer A which I understand. That means we’re effectively delaying reliable detection of Buffer A’s end activations until Buffer B completes — another 31.25 seconds later.
 So overall, wouldn’t this introduce a minimum latency of over 60 seconds (31.25 + 31.25) before we can respond to certain activation events? A abnormal activation will be detected over a minute later then start pacing. A corrected activation will only be detected after over a minute later, then the pacing will stop. Is that or isn't that too slow real time closed-loop GES? Has this been considered in Daryl's and Larissa's project? I will need to clarify this with Daryl if I have correctly understood it am not missing anything, after clarify with Dr Malik and Dr Wang about it. If this is an issue, i may need to lower buffer to a realistic value, but I am not sure how much process I may need to go through to validate the results, which I personally am not exited about.
 In the mean time, I will start with the next stage.</t>
-  </si>
-  <si>
-    <t>This should be created in a way that it can drive the whole program's timing. For example, if turned off it will run the like it is before, and turned on, operate in a set frequency. This will make test while development much more time efficient.</t>
   </si>
   <si>
     <r>
@@ -412,9 +388,6 @@
 Also was told that i donot need to test the datasets on desktop, but just connect it to the gut model instead using simulink. I have to learn what simulink does to understand what this means.</t>
   </si>
   <si>
-    <t>What is SIMULINK?</t>
-  </si>
-  <si>
     <t>Simulink</t>
   </si>
   <si>
@@ -424,6 +397,69 @@
   </si>
   <si>
     <t>After some research and asking chatgpt about the current type of processing methodol</t>
+  </si>
+  <si>
+    <t>Step 4 - connect gut model to C Prog</t>
+  </si>
+  <si>
+    <t>Simulink to C</t>
+  </si>
+  <si>
+    <t>Dataset simulation</t>
+  </si>
+  <si>
+    <t>Use gut model</t>
+  </si>
+  <si>
+    <t>Step 5 - Migrate to ARM Processor</t>
+  </si>
+  <si>
+    <t>Migrate C prog to board</t>
+  </si>
+  <si>
+    <t>Link PC(Simulink) to Board(C program)</t>
+  </si>
+  <si>
+    <t>Step 3 - Recreate the MATLAB project with C without using any libraries as possible and run it on desktop(goal is to make it run on a PC or similar level real time processor so need to be as light and simple as possible)</t>
+  </si>
+  <si>
+    <t>Step 5 - Migrate to FlexPRET</t>
+  </si>
+  <si>
+    <t>Implement pacing feature in PC</t>
+  </si>
+  <si>
+    <t>Migrate C prog to FlexPRET env</t>
+  </si>
+  <si>
+    <t>Link PC(Simulink) to FlexPRET</t>
+  </si>
+  <si>
+    <t>Step 6 - Testing and Optimization</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>Initial env prep</t>
+  </si>
+  <si>
+    <t>Initial env prep for DE1-Soc</t>
+  </si>
+  <si>
+    <t>Initial bare metal dev env prep</t>
+  </si>
+  <si>
+    <t>Research &amp; Review</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>ongoing</t>
+  </si>
+  <si>
+    <t>Migrate pacing functionality to board</t>
   </si>
 </sst>
 </file>
@@ -493,7 +529,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -533,19 +569,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -566,11 +589,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -620,35 +661,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1053,675 +1106,688 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="B15" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.23046875" style="2" customWidth="1"/>
-    <col min="2" max="3" width="10.765625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.23046875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.4609375" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="72.23046875" style="2" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="6.4609375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.53515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.23046875" style="9"/>
-    <col min="11" max="11" width="9.23046875" style="1"/>
-    <col min="12" max="12" width="60.84375" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="9.23046875" style="1"/>
+    <col min="1" max="1" width="10.765625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.15234375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.765625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.4609375" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="72.23046875" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="6.765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.765625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.23046875" style="9"/>
+    <col min="10" max="10" width="9.23046875" style="1"/>
+    <col min="11" max="11" width="60.84375" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.23046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="26.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="20.6" x14ac:dyDescent="0.4">
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-    </row>
-    <row r="2" spans="1:12" s="3" customFormat="1" ht="31.3" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:11" s="3" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="7"/>
       <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="D2" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="E2" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="7" t="s">
         <v>42</v>
       </c>
+      <c r="H2" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="I2" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A3" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="12"/>
+      <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="H3" s="11">
+        <v>45708</v>
+      </c>
       <c r="I3" s="11">
         <v>45708</v>
       </c>
-      <c r="J3" s="11">
-        <v>45708</v>
-      </c>
-      <c r="K3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="5"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A4" s="24" t="s">
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A4" s="23"/>
+      <c r="B4" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>0</v>
       </c>
+      <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="H4" s="11">
+        <v>45708</v>
+      </c>
       <c r="I4" s="11">
-        <v>45708</v>
-      </c>
-      <c r="J4" s="11">
         <v>45709</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="5"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A5" s="24"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="5" t="s">
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A5" s="23"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="5" t="s">
         <v>40</v>
       </c>
+      <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="H5" s="11">
+        <v>45716</v>
+      </c>
       <c r="I5" s="11">
         <v>45716</v>
       </c>
-      <c r="J5" s="11">
-        <v>45716</v>
-      </c>
-      <c r="K5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="5"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A6" s="24"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="5" t="s">
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A6" s="23"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="H6" s="11">
+        <v>45709</v>
+      </c>
       <c r="I6" s="11">
+        <v>45718</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A7" s="23"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="11">
         <v>45709</v>
       </c>
-      <c r="J6" s="11">
-        <v>45718</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" s="5"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A7" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="5"/>
       <c r="I7" s="11">
         <v>45709</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A8" s="23"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="11">
         <v>45709</v>
       </c>
-      <c r="K7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L7" s="5"/>
-    </row>
-    <row r="8" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A8" s="24"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" s="5"/>
       <c r="I8" s="11">
         <v>45709</v>
       </c>
-      <c r="J8" s="11">
-        <v>45709</v>
-      </c>
-      <c r="K8" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L8" s="5"/>
-    </row>
-    <row r="9" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A9" s="24" t="s">
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A9" s="23"/>
+      <c r="B9" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="18" t="s">
+      <c r="C9" s="19" t="s">
         <v>57</v>
       </c>
+      <c r="D9" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="E9" s="5" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="5" t="s">
         <v>4</v>
+      </c>
+      <c r="G9" s="13">
+        <v>45719</v>
       </c>
       <c r="H9" s="13">
         <v>45719</v>
       </c>
-      <c r="I9" s="13">
-        <v>45719</v>
-      </c>
-      <c r="J9" s="11">
+      <c r="I9" s="11">
         <v>45730</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="J9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="K9" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A10" s="24"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
+    <row r="10" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A10" s="23"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="E10" s="5" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="13">
+      <c r="G10" s="13">
         <v>45722</v>
       </c>
+      <c r="H10" s="11">
+        <v>45730</v>
+      </c>
       <c r="I10" s="11">
-        <v>45730</v>
-      </c>
-      <c r="J10" s="11">
         <v>45734</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="J10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="K10" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A11" s="24" t="s">
+    <row r="11" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A11" s="23"/>
+      <c r="B11" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="18" t="s">
+      <c r="C11" s="19" t="s">
         <v>58</v>
       </c>
+      <c r="D11" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="E11" s="5" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="13">
+      <c r="G11" s="13">
         <v>45726</v>
+      </c>
+      <c r="H11" s="11">
+        <v>45734</v>
       </c>
       <c r="I11" s="11">
         <v>45734</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A12" s="23"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="11">
         <v>45734</v>
       </c>
-      <c r="K11" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A12" s="24"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="13"/>
       <c r="I12" s="11">
         <v>45734</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A13" s="23"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="13">
+        <v>45729</v>
+      </c>
+      <c r="H13" s="11">
         <v>45734</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="I13" s="11">
+        <v>45736</v>
+      </c>
+      <c r="J13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L12" s="5"/>
-    </row>
-    <row r="13" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A13" s="24"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="13">
-        <v>45729</v>
-      </c>
-      <c r="I13" s="11">
-        <v>45734</v>
-      </c>
-      <c r="J13" s="11">
+      <c r="K13" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A14" s="23"/>
+      <c r="B14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="13">
+        <v>45733</v>
+      </c>
+      <c r="H14" s="11">
         <v>45736</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="13">
-        <v>45733</v>
       </c>
       <c r="I14" s="11">
         <v>45736</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A15" s="23"/>
+      <c r="B15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="21"/>
+      <c r="D15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="13">
         <v>45736</v>
       </c>
-      <c r="K14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L14" s="5"/>
-    </row>
-    <row r="15" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="13">
-        <v>45736</v>
+      <c r="H15" s="11">
+        <v>45740</v>
       </c>
       <c r="I15" s="11">
         <v>45740</v>
       </c>
-      <c r="J15" s="11">
-        <v>45740</v>
-      </c>
-      <c r="K15" s="4" t="s">
+      <c r="J15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L15" s="5"/>
-    </row>
-    <row r="16" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A16" s="5" t="s">
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A16" s="23"/>
+      <c r="B16" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="5" t="s">
+      <c r="C16" s="5" t="s">
         <v>66</v>
       </c>
+      <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="13">
+      <c r="G16" s="13">
         <v>45740</v>
       </c>
+      <c r="H16" s="11">
+        <v>45740</v>
+      </c>
       <c r="I16" s="11">
-        <v>45740</v>
-      </c>
-      <c r="J16" s="11">
         <v>45742</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="J16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L16" s="5"/>
-    </row>
-    <row r="17" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A17" s="17"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>73</v>
-      </c>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A17" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="13">
-        <v>45744</v>
-      </c>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A18" s="17"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="5" t="s">
-        <v>70</v>
-      </c>
+      <c r="G17" s="11">
+        <v>45778</v>
+      </c>
+      <c r="H17" s="11">
+        <v>45778</v>
+      </c>
+      <c r="I17" s="11">
+        <v>45779</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A18" s="26"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="13">
-        <v>45748</v>
-      </c>
+      <c r="G18" s="11">
+        <v>45779</v>
+      </c>
+      <c r="H18" s="11"/>
       <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="5"/>
-    </row>
-    <row r="19" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A19" s="17"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="5" t="s">
-        <v>69</v>
-      </c>
+      <c r="J18" s="4"/>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A19" s="26"/>
+      <c r="B19" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="13">
-        <v>45720</v>
-      </c>
+      <c r="G19" s="11">
+        <v>45783</v>
+      </c>
+      <c r="H19" s="11"/>
       <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="5"/>
-    </row>
-    <row r="20" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A20" s="17"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="5" t="s">
-        <v>66</v>
-      </c>
+      <c r="J19" s="4"/>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A20" s="27"/>
+      <c r="B20" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="13"/>
+      <c r="G20" s="11">
+        <v>45784</v>
+      </c>
+      <c r="H20" s="11"/>
       <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="5"/>
-    </row>
-    <row r="21" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A21" s="17"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A21" s="19" t="s">
+        <v>81</v>
+      </c>
       <c r="B21" s="5" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="11">
+        <v>45792</v>
+      </c>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A22" s="20"/>
+      <c r="B22" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="5"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A22" s="17"/>
-      <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="13"/>
+      <c r="G22" s="11">
+        <v>45796</v>
+      </c>
+      <c r="H22" s="11"/>
       <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="5"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A23" s="17"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A23" s="20"/>
+      <c r="B23" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="13"/>
+      <c r="G23" s="11">
+        <v>45803</v>
+      </c>
+      <c r="H23" s="11"/>
       <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="5"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B24" s="5"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="5"/>
+    </row>
+    <row r="24" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A24" s="20"/>
+      <c r="B24" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="13"/>
+      <c r="G24" s="11">
+        <v>45810</v>
+      </c>
+      <c r="H24" s="11"/>
       <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="5"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B25" s="5"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A25" s="21"/>
+      <c r="B25" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="13"/>
+      <c r="G25" s="11">
+        <v>45817</v>
+      </c>
+      <c r="H25" s="11"/>
       <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="5"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B26" s="5"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="5"/>
+    </row>
+    <row r="26" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A26" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="13"/>
+      <c r="G26" s="11">
+        <v>45824</v>
+      </c>
+      <c r="H26" s="11"/>
       <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="5"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B27" s="5"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="5"/>
+    </row>
+    <row r="27" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A27" s="20"/>
+      <c r="B27" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="13"/>
+      <c r="G27" s="11">
+        <v>45831</v>
+      </c>
+      <c r="H27" s="11"/>
       <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="5"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B28" s="5"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="5"/>
+    </row>
+    <row r="28" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A28" s="20"/>
+      <c r="B28" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="13"/>
+      <c r="G28" s="11">
+        <v>45838</v>
+      </c>
+      <c r="H28" s="11"/>
       <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="5"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="J28" s="4"/>
+      <c r="K28" s="5"/>
+    </row>
+    <row r="29" spans="1:11" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A29" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="13"/>
+      <c r="G29" s="11">
+        <v>45845</v>
+      </c>
+      <c r="H29" s="11"/>
       <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="5"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="5"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="C3:C16"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="B3:B20"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D4:D8"/>
+  <mergeCells count="13">
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A3:A16"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C7:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1732,7 +1798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
   <dimension ref="A2:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1746,7 +1812,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="15">
@@ -1760,7 +1826,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A3" s="25"/>
+      <c r="A3" s="24"/>
       <c r="C3" s="16" t="s">
         <v>46</v>
       </c>
@@ -1769,7 +1835,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="306" x14ac:dyDescent="0.4">
-      <c r="A4" s="25"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="15">
         <v>45728</v>
       </c>
@@ -1834,7 +1900,7 @@
     </row>
     <row r="10" spans="1:4" ht="102" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B10" s="15">
         <v>45742</v>
@@ -1844,23 +1910,23 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="160.30000000000001" x14ac:dyDescent="0.4">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>65</v>
       </c>
       <c r="B11" s="15">
         <v>45743</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="291.45" x14ac:dyDescent="0.4">
-      <c r="A12" s="25"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="15">
         <v>45743</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="116.6" x14ac:dyDescent="0.4">
@@ -1868,7 +1934,7 @@
         <v>45743</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
@@ -1876,7 +1942,7 @@
         <v>45743</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="233.15" x14ac:dyDescent="0.4">
@@ -1884,15 +1950,15 @@
         <v>45747</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="B16" s="15">
         <v>45747</v>
       </c>
-      <c r="C16" s="26" t="s">
-        <v>81</v>
+      <c r="C16" s="17" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
@@ -1900,12 +1966,12 @@
         <v>45748</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add TCP server implementation including necessary includes for socket programming.
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F156A8E5-FA91-4ADB-B78A-B97B622222F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A6808A-DBC0-45A6-A844-ABFA7034031C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="102">
   <si>
     <t>Import file</t>
   </si>
@@ -460,6 +460,18 @@
   </si>
   <si>
     <t>Migrate pacing functionality to board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a simulink model that sends samples from dataset file in a set frequency via TCP/IP to C TCP server </t>
+  </si>
+  <si>
+    <t>Implemented TCP server in C program</t>
+  </si>
+  <si>
+    <t>Dataset simulink model</t>
+  </si>
+  <si>
+    <t>Circular buffer implementation</t>
   </si>
 </sst>
 </file>
@@ -611,7 +623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -664,13 +676,31 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -685,23 +715,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1106,10 +1124,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1137,7 +1155,7 @@
       <c r="A2" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="18" t="s">
         <v>35</v>
       </c>
       <c r="C2" s="7"/>
@@ -1167,7 +1185,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="28" t="s">
         <v>84</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1192,11 +1210,11 @@
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A4" s="23"/>
-      <c r="B4" s="18" t="s">
+      <c r="A4" s="29"/>
+      <c r="B4" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="21" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -1217,9 +1235,9 @@
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A5" s="23"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
       <c r="D5" s="5" t="s">
         <v>40</v>
       </c>
@@ -1238,9 +1256,9 @@
       <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A6" s="23"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
       <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1259,9 +1277,9 @@
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A7" s="23"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18" t="s">
+      <c r="A7" s="29"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1284,9 +1302,9 @@
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A8" s="23"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1309,8 +1327,8 @@
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A9" s="23"/>
-      <c r="B9" s="18" t="s">
+      <c r="A9" s="29"/>
+      <c r="B9" s="21" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="19" t="s">
@@ -1342,9 +1360,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A10" s="23"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="21"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1371,8 +1389,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A11" s="23"/>
-      <c r="B11" s="18" t="s">
+      <c r="A11" s="29"/>
+      <c r="B11" s="21" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="19" t="s">
@@ -1404,8 +1422,8 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A12" s="23"/>
-      <c r="B12" s="18"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="21"/>
       <c r="C12" s="20"/>
       <c r="D12" s="5" t="s">
         <v>53</v>
@@ -1425,9 +1443,9 @@
       <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A13" s="23"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="21"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
@@ -1454,7 +1472,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A14" s="23"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
@@ -1485,11 +1503,11 @@
       <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A15" s="23"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="21"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1514,7 +1532,7 @@
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A16" s="23"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="5" t="s">
         <v>43</v>
       </c>
@@ -1539,10 +1557,10 @@
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="22" t="s">
         <v>78</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -1561,13 +1579,13 @@
         <v>45779</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A18" s="26"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="5" t="s">
         <v>95</v>
       </c>
@@ -1577,58 +1595,78 @@
       <c r="G18" s="11">
         <v>45779</v>
       </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="5"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A19" s="26"/>
-      <c r="B19" s="5" t="s">
+      <c r="H18" s="11">
+        <v>45779</v>
+      </c>
+      <c r="I18" s="11">
+        <v>45779</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A19" s="25"/>
+      <c r="B19" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="11">
         <v>45783</v>
       </c>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="5"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A20" s="27"/>
-      <c r="B20" s="5" t="s">
-        <v>80</v>
+      <c r="H19" s="11">
+        <v>45780</v>
+      </c>
+      <c r="I19" s="11">
+        <v>45781</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A20" s="25"/>
+      <c r="B20" s="32" t="s">
+        <v>101</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="11">
-        <v>45784</v>
-      </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="4"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11">
+        <v>45782</v>
+      </c>
+      <c r="I20" s="11">
+        <v>45782</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A21" s="19" t="s">
-        <v>81</v>
-      </c>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A21" s="26"/>
       <c r="B21" s="5" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="11">
-        <v>45792</v>
+        <v>45784</v>
       </c>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
@@ -1636,16 +1674,18 @@
       <c r="K21" s="5"/>
     </row>
     <row r="22" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A22" s="20"/>
+      <c r="A22" s="19" t="s">
+        <v>81</v>
+      </c>
       <c r="B22" s="5" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="11">
-        <v>45796</v>
+        <v>45792</v>
       </c>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
@@ -1655,14 +1695,14 @@
     <row r="23" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A23" s="20"/>
       <c r="B23" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="11">
-        <v>45803</v>
+        <v>45796</v>
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
@@ -1672,50 +1712,48 @@
     <row r="24" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A24" s="20"/>
       <c r="B24" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="11">
-        <v>45810</v>
+        <v>45803</v>
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="4"/>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A25" s="21"/>
+    <row r="25" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A25" s="20"/>
       <c r="B25" s="5" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="11">
-        <v>45817</v>
+        <v>45810</v>
       </c>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
       <c r="J25" s="4"/>
       <c r="K25" s="5"/>
     </row>
-    <row r="26" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A26" s="19" t="s">
-        <v>85</v>
-      </c>
+    <row r="26" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A26" s="27"/>
       <c r="B26" s="5" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="11">
-        <v>45824</v>
+        <v>45817</v>
       </c>
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
@@ -1723,16 +1761,18 @@
       <c r="K26" s="5"/>
     </row>
     <row r="27" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A27" s="20"/>
+      <c r="A27" s="19" t="s">
+        <v>85</v>
+      </c>
       <c r="B27" s="5" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="11">
-        <v>45831</v>
+        <v>45824</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
@@ -1742,45 +1782,56 @@
     <row r="28" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A28" s="20"/>
       <c r="B28" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="11">
-        <v>45838</v>
+        <v>45831</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
       <c r="J28" s="4"/>
       <c r="K28" s="5"/>
     </row>
-    <row r="29" spans="1:11" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A29" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B29" s="5"/>
+    <row r="29" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A29" s="20"/>
+      <c r="B29" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="11">
-        <v>45845</v>
+        <v>45838</v>
       </c>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
       <c r="J29" s="4"/>
       <c r="K29" s="5"/>
     </row>
+    <row r="30" spans="1:11" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A30" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="11">
+        <v>45845</v>
+      </c>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="A3:A16"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C15"/>
@@ -1788,6 +1839,12 @@
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A3:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1812,7 +1869,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="30" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="15">
@@ -1826,7 +1883,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A3" s="24"/>
+      <c r="A3" s="30"/>
       <c r="C3" s="16" t="s">
         <v>46</v>
       </c>
@@ -1835,7 +1892,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="306" x14ac:dyDescent="0.4">
-      <c r="A4" s="24"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="15">
         <v>45728</v>
       </c>
@@ -1910,7 +1967,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="160.30000000000001" x14ac:dyDescent="0.4">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="30" t="s">
         <v>65</v>
       </c>
       <c r="B11" s="15">
@@ -1921,7 +1978,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="291.45" x14ac:dyDescent="0.4">
-      <c r="A12" s="24"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="15">
         <v>45743</v>
       </c>

</xml_diff>

<commit_message>
Add mode selection functionality and moved features accordingly
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A6808A-DBC0-45A6-A844-ABFA7034031C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2AA541-0673-455E-9FDE-E411E4B26189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
     <sheet name="Journal" sheetId="3" r:id="rId2"/>
-    <sheet name="Results" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -70,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="104">
   <si>
     <t>Import file</t>
   </si>
@@ -388,9 +387,6 @@
 Also was told that i donot need to test the datasets on desktop, but just connect it to the gut model instead using simulink. I have to learn what simulink does to understand what this means.</t>
   </si>
   <si>
-    <t>Simulink</t>
-  </si>
-  <si>
     <t>Ive discussed with daryl regarding the buffer window size, the delay and the half buffer sample overlap. I realized that I have been approaching the role of the overlap wrong. I thought for some reason that it was to verify the activation that was in the last half of the buffer. Its partially correct, since if the activation was detected in the last buffer, it wouldnt need verification, it would mean that it detected a activation which needs not verifying. Incase the buffer couldnt detect the activation due to being in the end of the buffer and then it would most definately be detected in the next buffer, since the activation would have been in the end of the first half of the buffer, hence being in the center of the buffer window. 
 Also I now see why the 1000 sample(31.25s) window makes sense. one whole slow wave signal is around 20s. And for the buffers to have the whole signal in it, 1000 samples seem like a good number and the overlap would make it that a slow wave would be within the center of the window if it wasnt on the previous buffer window. And even if the signal was in the edge of the windows, since the part that is essential to activation detection is around only 8s(ave 12 s resting phase), if the first half was is in the buffer window, it will most likely be detected. 
 Thus, the worst case senario would be if the activation occured after #750 sample in the buffer window. that would be (31.25 x 0.25) + (31.25 0.5)s delay since it will be detected in the next buffer window, which is still around 23.44s, but having the activation signal in the start of the slow wave  would make it more likely to be detected in the first buffer window. Hence it would most likely that delay would be less than 20 sec. Although I might have to check if this is okey with Dr. Malik.</t>
@@ -456,15 +452,9 @@
     <t>Implementation</t>
   </si>
   <si>
-    <t>ongoing</t>
-  </si>
-  <si>
     <t>Migrate pacing functionality to board</t>
   </si>
   <si>
-    <t xml:space="preserve">Create a simulink model that sends samples from dataset file in a set frequency via TCP/IP to C TCP server </t>
-  </si>
-  <si>
     <t>Implemented TCP server in C program</t>
   </si>
   <si>
@@ -472,6 +462,21 @@
   </si>
   <si>
     <t>Circular buffer implementation</t>
+  </si>
+  <si>
+    <t>Create circular buffer</t>
+  </si>
+  <si>
+    <t>Apply circular buffer into c program</t>
+  </si>
+  <si>
+    <t>Create a Simulink model that sends samples from a dataset file to a C TCP server via TCP/IP at the original (real-time) sampling rate.</t>
+  </si>
+  <si>
+    <t>Need to implement concurrency. Signal reception and signal processing should be executed in separate threads to ensure that incoming samples are not missed during processing.</t>
+  </si>
+  <si>
+    <t>Upon doing this, I realized that without concurrency implemented here, if the activation detection pipeline process takes longer than the interval between each sample being sent from Simulink, incoming samples will not be received in time, or the server would miss incoming samples due to blocking, leading to data loss. So to address this, the receiving(reception, and the processing task must be decoupled and executed concurrently. The reception of signal will be handled in the main thread and the pipeline in the second thread.</t>
   </si>
 </sst>
 </file>
@@ -623,7 +628,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -680,6 +685,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -703,9 +714,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -714,12 +722,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1124,10 +1126,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1153,7 +1155,7 @@
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>35</v>
@@ -1185,11 +1187,11 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A3" s="28" t="s">
-        <v>84</v>
+      <c r="A3" s="29" t="s">
+        <v>83</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>37</v>
@@ -1210,11 +1212,11 @@
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A4" s="29"/>
-      <c r="B4" s="21" t="s">
+      <c r="A4" s="30"/>
+      <c r="B4" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="23" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -1235,9 +1237,9 @@
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A5" s="29"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="5" t="s">
         <v>40</v>
       </c>
@@ -1256,9 +1258,9 @@
       <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A6" s="29"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1277,9 +1279,9 @@
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A7" s="29"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21" t="s">
+      <c r="A7" s="30"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1302,9 +1304,9 @@
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A8" s="29"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
       <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1327,11 +1329,11 @@
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A9" s="29"/>
-      <c r="B9" s="21" t="s">
+      <c r="A9" s="30"/>
+      <c r="B9" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="20" t="s">
         <v>57</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1360,9 +1362,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A10" s="29"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="27"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1389,11 +1391,11 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A11" s="29"/>
-      <c r="B11" s="21" t="s">
+      <c r="A11" s="30"/>
+      <c r="B11" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="20" t="s">
         <v>58</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1422,9 +1424,9 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A12" s="29"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="20"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="5" t="s">
         <v>53</v>
       </c>
@@ -1443,9 +1445,9 @@
       <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A13" s="29"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="27"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="21"/>
       <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
@@ -1472,11 +1474,11 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A14" s="29"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="20" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -1503,11 +1505,11 @@
       <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A15" s="29"/>
+      <c r="A15" s="30"/>
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="27"/>
+      <c r="C15" s="21"/>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1532,7 +1534,7 @@
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A16" s="29"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="5" t="s">
         <v>43</v>
       </c>
@@ -1557,14 +1559,14 @@
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="22" t="s">
-        <v>78</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1584,10 +1586,10 @@
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A18" s="25"/>
-      <c r="B18" s="23"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1605,16 +1607,16 @@
         <v>24</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A19" s="25"/>
-      <c r="B19" s="31" t="s">
-        <v>79</v>
+      <c r="A19" s="27"/>
+      <c r="B19" s="19" t="s">
+        <v>78</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1632,15 +1634,17 @@
         <v>24</v>
       </c>
       <c r="K19" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A20" s="27"/>
+      <c r="B20" s="24" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A20" s="25"/>
-      <c r="B20" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="C20" s="5"/>
+      <c r="C20" s="5" t="s">
+        <v>99</v>
+      </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -1652,40 +1656,40 @@
         <v>45782</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A21" s="26"/>
-      <c r="B21" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="5"/>
+    <row r="21" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A21" s="27"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="11">
-        <v>45784</v>
-      </c>
-      <c r="H21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11">
+        <v>45783</v>
+      </c>
       <c r="I21" s="11"/>
       <c r="J21" s="4"/>
-      <c r="K21" s="5"/>
-    </row>
-    <row r="22" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A22" s="19" t="s">
-        <v>81</v>
-      </c>
+      <c r="K21" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A22" s="28"/>
       <c r="B22" s="5" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="11">
-        <v>45792</v>
+        <v>45784</v>
       </c>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
@@ -1693,16 +1697,18 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A23" s="20"/>
+      <c r="A23" s="20" t="s">
+        <v>80</v>
+      </c>
       <c r="B23" s="5" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="11">
-        <v>45796</v>
+        <v>45792</v>
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
@@ -1710,16 +1716,16 @@
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A24" s="20"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="11">
-        <v>45803</v>
+        <v>45796</v>
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
@@ -1727,52 +1733,50 @@
       <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A25" s="20"/>
+      <c r="A25" s="22"/>
       <c r="B25" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="11">
-        <v>45810</v>
+        <v>45803</v>
       </c>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
       <c r="J25" s="4"/>
       <c r="K25" s="5"/>
     </row>
-    <row r="26" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A26" s="27"/>
+    <row r="26" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A26" s="22"/>
       <c r="B26" s="5" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="11">
-        <v>45817</v>
+        <v>45810</v>
       </c>
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
       <c r="J26" s="4"/>
       <c r="K26" s="5"/>
     </row>
-    <row r="27" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A27" s="19" t="s">
-        <v>85</v>
-      </c>
+    <row r="27" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A27" s="21"/>
       <c r="B27" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="11">
-        <v>45824</v>
+        <v>45817</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
@@ -1780,16 +1784,18 @@
       <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A28" s="20"/>
+      <c r="A28" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="B28" s="5" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="11">
-        <v>45831</v>
+        <v>45824</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
@@ -1797,41 +1803,65 @@
       <c r="K28" s="5"/>
     </row>
     <row r="29" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A29" s="20"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="11">
-        <v>45838</v>
+        <v>45831</v>
       </c>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
       <c r="J29" s="4"/>
       <c r="K29" s="5"/>
     </row>
-    <row r="30" spans="1:11" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A30" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B30" s="5"/>
+    <row r="30" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A30" s="22"/>
+      <c r="B30" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="11">
-        <v>45845</v>
+        <v>45838</v>
       </c>
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
       <c r="J30" s="4"/>
       <c r="K30" s="5"/>
     </row>
+    <row r="31" spans="1:11" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A31" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="11">
+        <v>45845</v>
+      </c>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="A3:A16"/>
+    <mergeCell ref="B20:B21"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C15"/>
@@ -1839,12 +1869,6 @@
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C7:C8"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A3:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1855,8 +1879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
   <dimension ref="A2:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1869,7 +1893,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="31" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="15">
@@ -1883,7 +1907,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A3" s="30"/>
+      <c r="A3" s="31"/>
       <c r="C3" s="16" t="s">
         <v>46</v>
       </c>
@@ -1892,7 +1916,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="306" x14ac:dyDescent="0.4">
-      <c r="A4" s="30"/>
+      <c r="A4" s="31"/>
       <c r="B4" s="15">
         <v>45728</v>
       </c>
@@ -1967,7 +1991,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="160.30000000000001" x14ac:dyDescent="0.4">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="31" t="s">
         <v>65</v>
       </c>
       <c r="B11" s="15">
@@ -1978,7 +2002,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="291.45" x14ac:dyDescent="0.4">
-      <c r="A12" s="30"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="15">
         <v>45743</v>
       </c>
@@ -2007,7 +2031,7 @@
         <v>45747</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
@@ -2023,12 +2047,18 @@
         <v>45748</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>74</v>
+        <v>100</v>
+      </c>
+      <c r="B18" s="15">
+        <v>45783</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2039,18 +2069,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69446ECF-727C-4A2E-AB35-11AEE6EEA4B3}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Enhance timing logic in TCP server receive function and add timer to signal buffering process
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2AA541-0673-455E-9FDE-E411E4B26189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969BA251-CD50-41E8-B878-753241BEE0C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
@@ -476,7 +476,9 @@
     <t>Need to implement concurrency. Signal reception and signal processing should be executed in separate threads to ensure that incoming samples are not missed during processing.</t>
   </si>
   <si>
-    <t>Upon doing this, I realized that without concurrency implemented here, if the activation detection pipeline process takes longer than the interval between each sample being sent from Simulink, incoming samples will not be received in time, or the server would miss incoming samples due to blocking, leading to data loss. So to address this, the receiving(reception, and the processing task must be decoupled and executed concurrently. The reception of signal will be handled in the main thread and the pipeline in the second thread.</t>
+    <t>Upon doing this, I realized that without concurrency implemented here, if the activation detection pipeline process takes longer than the interval between each sample being sent from Simulink, incoming samples will not be received in time, or the server would miss incoming samples due to blocking, leading to data loss. So to address this, the receiving(reception, and the processing task must be decoupled and executed concurrently. The reception of signal will be handled in the main thread and the pipeline in the second thread.
+Although, the signal processing pipeline only takes about 0.15ms to complete and assuming the samples are transmitting in around 32 hz, which is about 30ms interval for each transmission, the processing complete within the before the next transmission where the server can start waiting for the next sample before the next transmission.
+But Im not sure how long the pipeline would take in a restricted environment, thus feel that it is better to implement this now than later.</t>
   </si>
 </sst>
 </file>
@@ -690,9 +692,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -712,6 +711,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1213,10 +1215,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="30"/>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -1238,8 +1240,8 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="30"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="5" t="s">
         <v>40</v>
       </c>
@@ -1259,8 +1261,8 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="30"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
       <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1280,8 +1282,8 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" s="30"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1305,8 +1307,8 @@
     </row>
     <row r="8" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A8" s="30"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1330,7 +1332,7 @@
     </row>
     <row r="9" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A9" s="30"/>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="20" t="s">
@@ -1363,8 +1365,8 @@
     </row>
     <row r="10" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A10" s="30"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1392,7 +1394,7 @@
     </row>
     <row r="11" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A11" s="30"/>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="20" t="s">
@@ -1425,8 +1427,8 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="30"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="5" t="s">
         <v>53</v>
       </c>
@@ -1446,8 +1448,8 @@
     </row>
     <row r="13" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A13" s="30"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="21"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
@@ -1509,7 +1511,7 @@
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="21"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1559,10 +1561,10 @@
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="23" t="s">
         <v>77</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -1586,8 +1588,8 @@
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A18" s="27"/>
-      <c r="B18" s="25"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="5" t="s">
         <v>94</v>
       </c>
@@ -1611,7 +1613,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A19" s="27"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="19" t="s">
         <v>78</v>
       </c>
@@ -1638,8 +1640,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A20" s="27"/>
-      <c r="B20" s="24" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="23" t="s">
         <v>98</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -1661,8 +1663,8 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A21" s="27"/>
-      <c r="B21" s="25"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="5" t="s">
         <v>100</v>
       </c>
@@ -1680,7 +1682,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A22" s="28"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="5" t="s">
         <v>79</v>
       </c>
@@ -1716,7 +1718,7 @@
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A24" s="22"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="5" t="s">
         <v>81</v>
       </c>
@@ -1733,7 +1735,7 @@
       <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A25" s="22"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="5" t="s">
         <v>82</v>
       </c>
@@ -1750,7 +1752,7 @@
       <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A26" s="22"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="5" t="s">
         <v>85</v>
       </c>
@@ -1767,7 +1769,7 @@
       <c r="K26" s="5"/>
     </row>
     <row r="27" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A27" s="21"/>
+      <c r="A27" s="28"/>
       <c r="B27" s="5" t="s">
         <v>95</v>
       </c>
@@ -1803,7 +1805,7 @@
       <c r="K28" s="5"/>
     </row>
     <row r="29" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A29" s="22"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="5" t="s">
         <v>86</v>
       </c>
@@ -1820,7 +1822,7 @@
       <c r="K29" s="5"/>
     </row>
     <row r="30" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A30" s="22"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="5" t="s">
         <v>87</v>
       </c>
@@ -1855,6 +1857,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C7:C8"/>
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="B4:B8"/>
     <mergeCell ref="B17:B18"/>
@@ -1862,13 +1871,6 @@
     <mergeCell ref="A23:A27"/>
     <mergeCell ref="A3:A16"/>
     <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C7:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1879,8 +1881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
   <dimension ref="A2:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2050,7 +2052,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
Refactor mode selection and integrate dataset modes into main application
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969BA251-CD50-41E8-B878-753241BEE0C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB2B228-79B9-485E-B698-E4012D8CFFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="-103" yWindow="-13817" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="105">
   <si>
     <t>Import file</t>
   </si>
@@ -392,9 +392,6 @@
 Thus, the worst case senario would be if the activation occured after #750 sample in the buffer window. that would be (31.25 x 0.25) + (31.25 0.5)s delay since it will be detected in the next buffer window, which is still around 23.44s, but having the activation signal in the start of the slow wave  would make it more likely to be detected in the first buffer window. Hence it would most likely that delay would be less than 20 sec. Although I might have to check if this is okey with Dr. Malik.</t>
   </si>
   <si>
-    <t>After some research and asking chatgpt about the current type of processing methodol</t>
-  </si>
-  <si>
     <t>Step 4 - connect gut model to C Prog</t>
   </si>
   <si>
@@ -479,6 +476,13 @@
     <t>Upon doing this, I realized that without concurrency implemented here, if the activation detection pipeline process takes longer than the interval between each sample being sent from Simulink, incoming samples will not be received in time, or the server would miss incoming samples due to blocking, leading to data loss. So to address this, the receiving(reception, and the processing task must be decoupled and executed concurrently. The reception of signal will be handled in the main thread and the pipeline in the second thread.
 Although, the signal processing pipeline only takes about 0.15ms to complete and assuming the samples are transmitting in around 32 hz, which is about 30ms interval for each transmission, the processing complete within the before the next transmission where the server can start waiting for the next sample before the next transmission.
 But Im not sure how long the pipeline would take in a restricted environment, thus feel that it is better to implement this now than later.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Due to mid sem break, and personal matters, and Luman's delay in sharing gut model, pacing alg, was not able to make any progress. Also, I found out that the part 4 students project was not producing same outputs as the algorithm results they have provided in their compendium. I communicated with Daryl and he said the thresholds and some other components were asjusted for the good datasets and bad datasets, which seems to be an unfinished version of the algorithm. I get into a delema about if I should spend time fixing the alg, so requested to meet with my supervisor to get some advice.
+</t>
+  </si>
+  <si>
+    <t>Meeting with the supervisor certainly cleared my mind. I was worried that I would not get to the hardware implementation part of the research if I had to work on the signal processing alg. But Dr Malik has advised that my research focus should be on the hardware implemenatation since it is a embedded system research topic, not a signal processing for gut pacemaker. My goal should be implementing the alg into to a embedded system, even though the alg doesnt work perfectly. The optimization for gut signal processing can be part of another project, but doesnt nessesarily have to be part of this one. This definately cleared my mind and a clear pathway. Will proceed to next step.</t>
   </si>
 </sst>
 </file>
@@ -692,6 +696,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -711,9 +718,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1157,7 +1161,7 @@
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>35</v>
@@ -1190,10 +1194,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>37</v>
@@ -1215,10 +1219,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="30"/>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="23" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -1240,8 +1244,8 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="30"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="5" t="s">
         <v>40</v>
       </c>
@@ -1261,8 +1265,8 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="30"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1282,8 +1286,8 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" s="30"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="23"/>
+      <c r="C7" s="23" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1307,8 +1311,8 @@
     </row>
     <row r="8" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A8" s="30"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
       <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1332,7 +1336,7 @@
     </row>
     <row r="9" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A9" s="30"/>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="23" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="20" t="s">
@@ -1365,8 +1369,8 @@
     </row>
     <row r="10" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A10" s="30"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="28"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1394,7 +1398,7 @@
     </row>
     <row r="11" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A11" s="30"/>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="23" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="20" t="s">
@@ -1427,8 +1431,8 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="30"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="21"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="5" t="s">
         <v>53</v>
       </c>
@@ -1448,8 +1452,8 @@
     </row>
     <row r="13" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A13" s="30"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="28"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="21"/>
       <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
@@ -1511,7 +1515,7 @@
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="28"/>
+      <c r="C15" s="21"/>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1561,14 +1565,14 @@
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="23" t="s">
-        <v>77</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1588,10 +1592,10 @@
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A18" s="26"/>
-      <c r="B18" s="24"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1609,16 +1613,16 @@
         <v>24</v>
       </c>
       <c r="K18" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A19" s="27"/>
+      <c r="B19" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A19" s="26"/>
-      <c r="B19" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1636,16 +1640,16 @@
         <v>24</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A20" s="26"/>
-      <c r="B20" s="23" t="s">
+      <c r="A20" s="27"/>
+      <c r="B20" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -1663,10 +1667,10 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A21" s="26"/>
-      <c r="B21" s="24"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -1678,13 +1682,13 @@
       <c r="I21" s="11"/>
       <c r="J21" s="4"/>
       <c r="K21" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A22" s="27"/>
+      <c r="A22" s="28"/>
       <c r="B22" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -1700,10 +1704,10 @@
     </row>
     <row r="23" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A23" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -1718,9 +1722,9 @@
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A24" s="21"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -1735,9 +1739,9 @@
       <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A25" s="21"/>
+      <c r="A25" s="22"/>
       <c r="B25" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -1752,9 +1756,9 @@
       <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A26" s="21"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -1769,9 +1773,9 @@
       <c r="K26" s="5"/>
     </row>
     <row r="27" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A27" s="28"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -1787,10 +1791,10 @@
     </row>
     <row r="28" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A28" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -1805,9 +1809,9 @@
       <c r="K28" s="5"/>
     </row>
     <row r="29" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A29" s="21"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -1822,9 +1826,9 @@
       <c r="K29" s="5"/>
     </row>
     <row r="30" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A30" s="21"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -1840,7 +1844,7 @@
     </row>
     <row r="31" spans="1:11" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A31" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1857,6 +1861,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="A3:A16"/>
+    <mergeCell ref="B20:B21"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C15"/>
@@ -1864,13 +1875,6 @@
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C7:C8"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A17:A22"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="A3:A16"/>
-    <mergeCell ref="B20:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1879,10 +1883,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A2:D18"/>
+  <dimension ref="A2:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2044,23 +2048,31 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" ht="87.45" x14ac:dyDescent="0.4">
       <c r="B17" s="15">
-        <v>45748</v>
+        <v>45765</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="145.75" x14ac:dyDescent="0.4">
-      <c r="A18" s="2" t="s">
-        <v>100</v>
-      </c>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="87.45" x14ac:dyDescent="0.4">
       <c r="B18" s="15">
+        <v>45770</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="145.75" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="15">
         <v>45783</v>
       </c>
-      <c r="C18" s="16" t="s">
-        <v>103</v>
+      <c r="C19" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor buffer handling: update buffer size definitions, add overlap count to SharedData, and enhance TCP server signal processing logic.
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB2B228-79B9-485E-B698-E4012D8CFFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52BCCE9-D92D-47B1-8B5C-5CE4A46B935A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-13817" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="113">
   <si>
     <t>Import file</t>
   </si>
@@ -483,6 +483,33 @@
   </si>
   <si>
     <t>Meeting with the supervisor certainly cleared my mind. I was worried that I would not get to the hardware implementation part of the research if I had to work on the signal processing alg. But Dr Malik has advised that my research focus should be on the hardware implemenatation since it is a embedded system research topic, not a signal processing for gut pacemaker. My goal should be implementing the alg into to a embedded system, even though the alg doesnt work perfectly. The optimization for gut signal processing can be part of another project, but doesnt nessesarily have to be part of this one. This definately cleared my mind and a clear pathway. Will proceed to next step.</t>
+  </si>
+  <si>
+    <t>Multithreading for signal reception and detection pipeline</t>
+  </si>
+  <si>
+    <t>Implement threads</t>
+  </si>
+  <si>
+    <t>Condition vars implementation for process thread</t>
+  </si>
+  <si>
+    <t>Pipeline modification for new implementation</t>
+  </si>
+  <si>
+    <t>refactoring</t>
+  </si>
+  <si>
+    <t>Simulink to C Communication Implementation &amp; Multithreading</t>
+  </si>
+  <si>
+    <t>After completing the multithreading implementation for signal reception and the activation detection (signal processing) pipeline, a few concerns came to mind:
+1. pthread cannot be used for multitasking in bare-metal programming environments.
+2. TCP/IP is also unavailable in bare-metal environments.
+To make future transitions smoother—particularly toward embedded platforms and eventually FlexPRET—I decided to abstract both the multithreading and communication interfaces. This way, I can adapt the underlying implementation for each new environment without changing the core application logic.</t>
+  </si>
+  <si>
+    <t>ongoing</t>
   </si>
 </sst>
 </file>
@@ -634,7 +661,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -696,30 +723,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -727,6 +754,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1132,10 +1162,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="B14" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1219,10 +1249,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="30"/>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -1244,8 +1274,8 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="30"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="5" t="s">
         <v>40</v>
       </c>
@@ -1265,8 +1295,8 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="30"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
       <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1286,8 +1316,8 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" s="30"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1311,8 +1341,8 @@
     </row>
     <row r="8" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A8" s="30"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1336,7 +1366,7 @@
     </row>
     <row r="9" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A9" s="30"/>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="20" t="s">
@@ -1369,8 +1399,8 @@
     </row>
     <row r="10" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A10" s="30"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1398,7 +1428,7 @@
     </row>
     <row r="11" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A11" s="30"/>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="20" t="s">
@@ -1431,8 +1461,8 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="30"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="5" t="s">
         <v>53</v>
       </c>
@@ -1452,8 +1482,8 @@
     </row>
     <row r="13" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A13" s="30"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="21"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
@@ -1515,7 +1545,7 @@
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="21"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1565,10 +1595,10 @@
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="23" t="s">
         <v>76</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -1592,8 +1622,8 @@
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A18" s="27"/>
-      <c r="B18" s="25"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="5" t="s">
         <v>93</v>
       </c>
@@ -1617,7 +1647,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A19" s="27"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="19" t="s">
         <v>77</v>
       </c>
@@ -1644,8 +1674,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A20" s="27"/>
-      <c r="B20" s="24" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="22" t="s">
         <v>97</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -1667,8 +1697,8 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A21" s="27"/>
-      <c r="B21" s="25"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="22"/>
       <c r="C21" s="5" t="s">
         <v>99</v>
       </c>
@@ -1679,110 +1709,126 @@
       <c r="H21" s="11">
         <v>45783</v>
       </c>
-      <c r="I21" s="11"/>
-      <c r="J21" s="4"/>
+      <c r="I21" s="11">
+        <v>45791</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="K21" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A22" s="28"/>
-      <c r="B22" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" s="5"/>
+    <row r="22" spans="1:11" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="26"/>
+      <c r="B22" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>106</v>
+      </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="11">
-        <v>45784</v>
-      </c>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="4"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11">
+        <v>45791</v>
+      </c>
+      <c r="I22" s="11">
+        <v>45791</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="K22" s="5"/>
     </row>
-    <row r="23" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A23" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C23" s="5"/>
+    <row r="23" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A23" s="26"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="11">
-        <v>45792</v>
-      </c>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="4"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11">
+        <v>45791</v>
+      </c>
+      <c r="I23" s="11">
+        <v>45793</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="K23" s="5"/>
     </row>
-    <row r="24" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A24" s="22"/>
-      <c r="B24" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C24" s="5"/>
+    <row r="24" spans="1:11" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A24" s="26"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="11">
         <v>45796</v>
       </c>
-      <c r="H24" s="11"/>
+      <c r="H24" s="11">
+        <v>45796</v>
+      </c>
       <c r="I24" s="11"/>
-      <c r="J24" s="4"/>
+      <c r="J24" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A25" s="22"/>
-      <c r="B25" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="5"/>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A25" s="26"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="5" t="s">
+        <v>109</v>
+      </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="11">
-        <v>45803</v>
-      </c>
+      <c r="G25" s="11"/>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
       <c r="J25" s="4"/>
       <c r="K25" s="5"/>
     </row>
-    <row r="26" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A26" s="22"/>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A26" s="27"/>
       <c r="B26" s="5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="11">
-        <v>45810</v>
+        <v>45784</v>
       </c>
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
       <c r="J26" s="4"/>
       <c r="K26" s="5"/>
     </row>
-    <row r="27" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A27" s="21"/>
+    <row r="27" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A27" s="20" t="s">
+        <v>79</v>
+      </c>
       <c r="B27" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="11">
-        <v>45817</v>
+        <v>45792</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
@@ -1790,18 +1836,16 @@
       <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A28" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="A28" s="21"/>
       <c r="B28" s="5" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="11">
-        <v>45824</v>
+        <v>45796</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
@@ -1809,16 +1853,16 @@
       <c r="K28" s="5"/>
     </row>
     <row r="29" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A29" s="22"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="11">
-        <v>45831</v>
+        <v>45803</v>
       </c>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
@@ -1826,48 +1870,111 @@
       <c r="K29" s="5"/>
     </row>
     <row r="30" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A30" s="22"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="11">
-        <v>45838</v>
+        <v>45810</v>
       </c>
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
       <c r="J30" s="4"/>
       <c r="K30" s="5"/>
     </row>
-    <row r="31" spans="1:11" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A31" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B31" s="5"/>
+    <row r="31" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A31" s="28"/>
+      <c r="B31" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="11">
-        <v>45845</v>
+        <v>45817</v>
       </c>
       <c r="H31" s="11"/>
       <c r="I31" s="11"/>
       <c r="J31" s="4"/>
       <c r="K31" s="5"/>
     </row>
+    <row r="32" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A32" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="11">
+        <v>45824</v>
+      </c>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="5"/>
+    </row>
+    <row r="33" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A33" s="21"/>
+      <c r="B33" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="11">
+        <v>45831</v>
+      </c>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="5"/>
+    </row>
+    <row r="34" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A34" s="21"/>
+      <c r="B34" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="11">
+        <v>45838</v>
+      </c>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="5"/>
+    </row>
+    <row r="35" spans="1:11" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A35" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="11">
+        <v>45845</v>
+      </c>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A17:A22"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="A3:A16"/>
-    <mergeCell ref="B20:B21"/>
+  <mergeCells count="15">
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C15"/>
@@ -1875,6 +1982,14 @@
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A17:A26"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A3:A16"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1883,10 +1998,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A2:D19"/>
+  <dimension ref="A2:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2075,6 +2190,17 @@
         <v>102</v>
       </c>
     </row>
+    <row r="20" spans="1:3" ht="102" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" s="15">
+        <v>45794</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:A4"/>

</xml_diff>

<commit_message>
Refactor ring buffer and shared data structures: update signal count handling, improve initialization logic, and enhance buffer processing in TCP server.
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52BCCE9-D92D-47B1-8B5C-5CE4A46B935A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE3D430-8CF7-49BD-9937-0652E838CEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="114">
   <si>
     <t>Import file</t>
   </si>
@@ -510,6 +510,12 @@
   </si>
   <si>
     <t>ongoing</t>
+  </si>
+  <si>
+    <t>There is a condition check for removing artifact when calling remove_artifact fucntion in the c program where I commented out better implementation and just used a Matlab prog mimiced one. 
+if (x2 &lt; ARTIFACT_DETECT_WINDOW_WIDTH &amp;&amp; x1 &gt;= 0) // this make sence but it is not the same as MATLAB logic
+// if (x2 &lt; ARTIFACT_DETECT_WINDOW_WIDTH &amp;&amp; x1 &gt;= 2) // this mimics the MATLAB logic
+Need to change in the future if need to refactor</t>
   </si>
 </sst>
 </file>
@@ -723,6 +729,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -744,19 +753,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1164,7 +1170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -1249,10 +1255,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="30"/>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="23" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -1274,8 +1280,8 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="30"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="5" t="s">
         <v>40</v>
       </c>
@@ -1295,8 +1301,8 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="30"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1316,8 +1322,8 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" s="30"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="23"/>
+      <c r="C7" s="23" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1341,8 +1347,8 @@
     </row>
     <row r="8" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A8" s="30"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
       <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1366,7 +1372,7 @@
     </row>
     <row r="9" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A9" s="30"/>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="23" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="20" t="s">
@@ -1399,8 +1405,8 @@
     </row>
     <row r="10" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A10" s="30"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="28"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1428,7 +1434,7 @@
     </row>
     <row r="11" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A11" s="30"/>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="23" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="20" t="s">
@@ -1461,8 +1467,8 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="30"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="21"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="5" t="s">
         <v>53</v>
       </c>
@@ -1482,8 +1488,8 @@
     </row>
     <row r="13" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A13" s="30"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="28"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="21"/>
       <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
@@ -1545,7 +1551,7 @@
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="28"/>
+      <c r="C15" s="21"/>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1595,10 +1601,10 @@
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="24" t="s">
         <v>76</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -1622,8 +1628,8 @@
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A18" s="26"/>
-      <c r="B18" s="24"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="5" t="s">
         <v>93</v>
       </c>
@@ -1647,7 +1653,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A19" s="26"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="19" t="s">
         <v>77</v>
       </c>
@@ -1674,8 +1680,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A20" s="26"/>
-      <c r="B20" s="22" t="s">
+      <c r="A20" s="27"/>
+      <c r="B20" s="23" t="s">
         <v>97</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -1697,8 +1703,8 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A21" s="26"/>
-      <c r="B21" s="22"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="23"/>
       <c r="C21" s="5" t="s">
         <v>99</v>
       </c>
@@ -1720,8 +1726,8 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="26"/>
-      <c r="B22" s="23" t="s">
+      <c r="A22" s="27"/>
+      <c r="B22" s="24" t="s">
         <v>105</v>
       </c>
       <c r="C22" s="5" t="s">
@@ -1743,8 +1749,8 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A23" s="26"/>
-      <c r="B23" s="32"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="31"/>
       <c r="C23" s="5" t="s">
         <v>107</v>
       </c>
@@ -1764,8 +1770,8 @@
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:11" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A24" s="26"/>
-      <c r="B24" s="32"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="31"/>
       <c r="C24" s="5" t="s">
         <v>108</v>
       </c>
@@ -1785,8 +1791,8 @@
       <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A25" s="26"/>
-      <c r="B25" s="24"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="25"/>
       <c r="C25" s="5" t="s">
         <v>109</v>
       </c>
@@ -1800,7 +1806,7 @@
       <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A26" s="27"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="5" t="s">
         <v>78</v>
       </c>
@@ -1836,7 +1842,7 @@
       <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A28" s="21"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="5" t="s">
         <v>80</v>
       </c>
@@ -1853,7 +1859,7 @@
       <c r="K28" s="5"/>
     </row>
     <row r="29" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A29" s="21"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="5" t="s">
         <v>81</v>
       </c>
@@ -1870,7 +1876,7 @@
       <c r="K29" s="5"/>
     </row>
     <row r="30" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A30" s="21"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="5" t="s">
         <v>84</v>
       </c>
@@ -1887,7 +1893,7 @@
       <c r="K30" s="5"/>
     </row>
     <row r="31" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A31" s="28"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="5" t="s">
         <v>94</v>
       </c>
@@ -1923,7 +1929,7 @@
       <c r="K32" s="5"/>
     </row>
     <row r="33" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A33" s="21"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="5" t="s">
         <v>85</v>
       </c>
@@ -1940,7 +1946,7 @@
       <c r="K33" s="5"/>
     </row>
     <row r="34" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A34" s="21"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="5" t="s">
         <v>86</v>
       </c>
@@ -1975,13 +1981,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C7:C8"/>
     <mergeCell ref="A32:A34"/>
     <mergeCell ref="B4:B8"/>
     <mergeCell ref="B17:B18"/>
@@ -1990,6 +1989,13 @@
     <mergeCell ref="A3:A16"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C7:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1998,10 +2004,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A2:D20"/>
+  <dimension ref="A2:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2014,7 +2020,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="32" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="15">
@@ -2028,7 +2034,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A3" s="31"/>
+      <c r="A3" s="32"/>
       <c r="C3" s="16" t="s">
         <v>46</v>
       </c>
@@ -2037,7 +2043,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="306" x14ac:dyDescent="0.4">
-      <c r="A4" s="31"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="15">
         <v>45728</v>
       </c>
@@ -2057,7 +2063,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="32" t="s">
         <v>50</v>
       </c>
       <c r="B6" s="15">
@@ -2067,144 +2073,154 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A7" s="32"/>
+      <c r="B7" s="15">
+        <v>45798</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B7" s="15">
-        <v>45734</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="116.6" x14ac:dyDescent="0.4">
-      <c r="A8" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="B8" s="15">
         <v>45734</v>
       </c>
       <c r="C8" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="116.6" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="15">
+        <v>45734</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="145.75" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:4" ht="145.75" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B10" s="15">
         <v>45736</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C10" s="16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="102" x14ac:dyDescent="0.4">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:4" ht="102" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B11" s="15">
         <v>45742</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C11" s="16" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="160.30000000000001" x14ac:dyDescent="0.4">
-      <c r="A11" s="31" t="s">
+    <row r="12" spans="1:4" ht="160.30000000000001" x14ac:dyDescent="0.4">
+      <c r="A12" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="15">
-        <v>45743</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="291.45" x14ac:dyDescent="0.4">
-      <c r="A12" s="31"/>
       <c r="B12" s="15">
         <v>45743</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="116.6" x14ac:dyDescent="0.4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="291.45" x14ac:dyDescent="0.4">
+      <c r="A13" s="32"/>
       <c r="B13" s="15">
         <v>45743</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="116.6" x14ac:dyDescent="0.4">
       <c r="B14" s="15">
         <v>45743</v>
       </c>
       <c r="C14" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="B15" s="15">
+        <v>45743</v>
+      </c>
+      <c r="C15" s="16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="233.15" x14ac:dyDescent="0.4">
-      <c r="B15" s="15">
-        <v>45747</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" ht="233.15" x14ac:dyDescent="0.4">
       <c r="B16" s="15">
         <v>45747</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="B17" s="15">
+        <v>45747</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="B17" s="15">
-        <v>45765</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="87.45" x14ac:dyDescent="0.4">
       <c r="B18" s="15">
+        <v>45765</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="B19" s="15">
         <v>45770</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C19" s="16" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="145.75" x14ac:dyDescent="0.4">
-      <c r="A19" s="2" t="s">
+    <row r="20" spans="1:3" ht="145.75" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B20" s="15">
         <v>45783</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C20" s="16" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="102" x14ac:dyDescent="0.4">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:3" ht="102" x14ac:dyDescent="0.4">
+      <c r="A21" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B21" s="15">
         <v>45794</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C21" s="16" t="s">
         <v>111</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
chore: update execution to p.o
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE3D430-8CF7-49BD-9937-0652E838CEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236C8ED2-5B80-4327-A544-4DDD0E2FF5FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="117">
   <si>
     <t>Import file</t>
   </si>
@@ -516,6 +516,16 @@
 if (x2 &lt; ARTIFACT_DETECT_WINDOW_WIDTH &amp;&amp; x1 &gt;= 0) // this make sence but it is not the same as MATLAB logic
 // if (x2 &lt; ARTIFACT_DETECT_WINDOW_WIDTH &amp;&amp; x1 &gt;= 2) // this mimics the MATLAB logic
 Need to change in the future if need to refactor</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>Gut Model connection to C program</t>
+  </si>
+  <si>
+    <t>While analysing Luman's repo that she shared, I found that the gut model was not modularised and just in the simulink file with pacing blocks and other components. I'm having difficulty understanding and analysing it, since the implementations in it are not really clear. I requested to meet Luman again to get her to explain what each block is in the simulink model, so that I can just extract the actual gut model and modularize it. So this part will be pending until I meet Luman.
+In the meantime, I will just go on and start the migration process to the DE1 SoC board.</t>
   </si>
 </sst>
 </file>
@@ -1170,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1786,7 +1796,7 @@
       </c>
       <c r="I24" s="11"/>
       <c r="J24" s="4" t="s">
-        <v>112</v>
+        <v>24</v>
       </c>
       <c r="K24" s="5"/>
     </row>
@@ -1801,8 +1811,12 @@
       <c r="F25" s="5"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="4"/>
+      <c r="I25" s="11">
+        <v>45805</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.4">
@@ -1817,9 +1831,13 @@
       <c r="G26" s="11">
         <v>45784</v>
       </c>
-      <c r="H26" s="11"/>
+      <c r="H26" s="11">
+        <v>45805</v>
+      </c>
       <c r="I26" s="11"/>
-      <c r="J26" s="4"/>
+      <c r="J26" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="K26" s="5"/>
     </row>
     <row r="27" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
@@ -1836,9 +1854,13 @@
       <c r="G27" s="11">
         <v>45792</v>
       </c>
-      <c r="H27" s="11"/>
+      <c r="H27" s="11">
+        <v>45805</v>
+      </c>
       <c r="I27" s="11"/>
-      <c r="J27" s="4"/>
+      <c r="J27" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
@@ -2004,10 +2026,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A2:D21"/>
+  <dimension ref="A2:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2216,6 +2238,17 @@
         <v>111</v>
       </c>
     </row>
+    <row r="22" spans="1:3" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" s="15">
+        <v>45805</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:A4"/>

</xml_diff>

<commit_message>
docs: update progress and journal
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236C8ED2-5B80-4327-A544-4DDD0E2FF5FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3F8C5C-7957-42DF-8997-128C052260B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="14777" yWindow="-11074" windowWidth="16457" windowHeight="9454" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
     <sheet name="Journal" sheetId="3" r:id="rId2"/>
+    <sheet name="README" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="121">
   <si>
     <t>Import file</t>
   </si>
@@ -509,9 +510,6 @@
 To make future transitions smoother—particularly toward embedded platforms and eventually FlexPRET—I decided to abstract both the multithreading and communication interfaces. This way, I can adapt the underlying implementation for each new environment without changing the core application logic.</t>
   </si>
   <si>
-    <t>ongoing</t>
-  </si>
-  <si>
     <t>There is a condition check for removing artifact when calling remove_artifact fucntion in the c program where I commented out better implementation and just used a Matlab prog mimiced one. 
 if (x2 &lt; ARTIFACT_DETECT_WINDOW_WIDTH &amp;&amp; x1 &gt;= 0) // this make sence but it is not the same as MATLAB logic
 // if (x2 &lt; ARTIFACT_DETECT_WINDOW_WIDTH &amp;&amp; x1 &gt;= 2) // this mimics the MATLAB logic
@@ -526,6 +524,25 @@
   <si>
     <t>While analysing Luman's repo that she shared, I found that the gut model was not modularised and just in the simulink file with pacing blocks and other components. I'm having difficulty understanding and analysing it, since the implementations in it are not really clear. I requested to meet Luman again to get her to explain what each block is in the simulink model, so that I can just extract the actual gut model and modularize it. So this part will be pending until I meet Luman.
 In the meantime, I will just go on and start the migration process to the DE1 SoC board.</t>
+  </si>
+  <si>
+    <t>in notion</t>
+  </si>
+  <si>
+    <t>Pacemaker Dev Notes: Cross-Compiling for DE1-SoC ARM Linux</t>
+  </si>
+  <si>
+    <t>how to configure the makefile for de1-soc ARM Linux compiler</t>
+  </si>
+  <si>
+    <t>Migrate C prog to DE1SoC board</t>
+  </si>
+  <si>
+    <t>I had trouble getting the crosscompiled file to run successfully on the board. I needed extensive assistance from chatGPT to figure out how to solve the issue. Basically it was 3 things.
+1. version of the toolchain, where I handled by extracting the root file system fromthe board and recomplied with --sysroot pointing to the rootfs
+2. Then i found that the there were missing headers and libs in this root file system so copied the missing files from the compiler to the root file 
+3. and there was linker error for pthead functions so added -lpthread to the compile command which caused /lib/libc.so.6: version `GLIBC_2.17' not found and solved that my adding --static to the comple command
+this took a long time with chatgpt and without it, im not sure how long it would have taken. I found that there is a rootsys that I can download from the site i downloaded the toolchain. I wil try to complile again with that instead.</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
@@ -1836,7 +1853,7 @@
       </c>
       <c r="I26" s="11"/>
       <c r="J26" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K26" s="5"/>
     </row>
@@ -1857,9 +1874,11 @@
       <c r="H27" s="11">
         <v>45805</v>
       </c>
-      <c r="I27" s="11"/>
+      <c r="I27" s="11">
+        <v>45806</v>
+      </c>
       <c r="J27" s="4" t="s">
-        <v>112</v>
+        <v>24</v>
       </c>
       <c r="K27" s="5"/>
     </row>
@@ -1875,9 +1894,15 @@
       <c r="G28" s="11">
         <v>45796</v>
       </c>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="4"/>
+      <c r="H28" s="11">
+        <v>45806</v>
+      </c>
+      <c r="I28" s="11">
+        <v>45806</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="K28" s="5"/>
     </row>
     <row r="29" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
@@ -2026,10 +2051,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A2:D22"/>
+  <dimension ref="A2:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2101,7 +2126,7 @@
         <v>45798</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="87.45" x14ac:dyDescent="0.4">
@@ -2240,13 +2265,24 @@
     </row>
     <row r="22" spans="1:3" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B22" s="15">
         <v>45805</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="174.9" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B23" s="15">
+        <v>45806</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2258,4 +2294,33 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D394CF-E473-41AA-B964-15AB3737F01C}">
+  <dimension ref="A2:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="54.23046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor: Move large pipeline buffers to static storage to prevent stack overflow
- Moved all large buffer variables in processing_pipeline() to file-scoped static
storage to avoid stack overflow on DE1-SoC during real-time mode execution.
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3F8C5C-7957-42DF-8997-128C052260B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B8257D-184E-42AE-894F-3451F4EA5B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14777" yWindow="-11074" windowWidth="16457" windowHeight="9454" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="122">
   <si>
     <t>Import file</t>
   </si>
@@ -543,6 +543,12 @@
 2. Then i found that the there were missing headers and libs in this root file system so copied the missing files from the compiler to the root file 
 3. and there was linker error for pthead functions so added -lpthread to the compile command which caused /lib/libc.so.6: version `GLIBC_2.17' not found and solved that my adding --static to the comple command
 this took a long time with chatgpt and without it, im not sure how long it would have taken. I found that there is a rootsys that I can download from the site i downloaded the toolchain. I wil try to complile again with that instead.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linking the board went smoothly; I connected it via Ethernet using the eth0 interface, brought it up with ifconfig eth0 up, and obtained an IP address through DHCP using udhcpc -i eth0. I then connected to the assigned IP from the MATLAB dataset interface for data transmission.
+While testing Realtime Dataset Mode on the DE1-SoC board using the setup described above, a segmentation fault occurred. The root cause was likely a stack overflow due to oversized buffers declared within the processing_pipeline function.
+On many embedded Linux systems, including DE1-SoC, the default pthread stack size is often only 64 KB or 128 KB(I tried confirming this from the board terminal, I couldnt). Although I could have increased it using pthread_attr_setstacksize(), I decided against it since future implementations will run on memory-constrained environments like bare-metal systems. 
+Instead, I refactored all large buffer variables inside the pipeline to be file-scoped static variables, allowing them to reside in the .bss segment (static memory) instead of the thread’s stack. This fixed the issue. </t>
   </si>
 </sst>
 </file>
@@ -756,9 +762,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -778,6 +781,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1197,8 +1203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1282,10 +1288,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="30"/>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -1307,8 +1313,8 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="30"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="5" t="s">
         <v>40</v>
       </c>
@@ -1328,8 +1334,8 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="30"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
       <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1349,8 +1355,8 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" s="30"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1374,8 +1380,8 @@
     </row>
     <row r="8" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A8" s="30"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1399,7 +1405,7 @@
     </row>
     <row r="9" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A9" s="30"/>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="20" t="s">
@@ -1432,8 +1438,8 @@
     </row>
     <row r="10" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A10" s="30"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1461,7 +1467,7 @@
     </row>
     <row r="11" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A11" s="30"/>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="20" t="s">
@@ -1494,8 +1500,8 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="30"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="5" t="s">
         <v>53</v>
       </c>
@@ -1515,8 +1521,8 @@
     </row>
     <row r="13" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A13" s="30"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="21"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
@@ -1578,7 +1584,7 @@
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="21"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1628,10 +1634,10 @@
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="23" t="s">
         <v>76</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -1655,8 +1661,8 @@
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A18" s="27"/>
-      <c r="B18" s="25"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="5" t="s">
         <v>93</v>
       </c>
@@ -1680,7 +1686,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A19" s="27"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="19" t="s">
         <v>77</v>
       </c>
@@ -1707,8 +1713,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A20" s="27"/>
-      <c r="B20" s="23" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="22" t="s">
         <v>97</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -1730,8 +1736,8 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A21" s="27"/>
-      <c r="B21" s="23"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="22"/>
       <c r="C21" s="5" t="s">
         <v>99</v>
       </c>
@@ -1753,8 +1759,8 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="27"/>
-      <c r="B22" s="24" t="s">
+      <c r="A22" s="26"/>
+      <c r="B22" s="23" t="s">
         <v>105</v>
       </c>
       <c r="C22" s="5" t="s">
@@ -1776,7 +1782,7 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A23" s="27"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="31"/>
       <c r="C23" s="5" t="s">
         <v>107</v>
@@ -1797,7 +1803,7 @@
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:11" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A24" s="27"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="31"/>
       <c r="C24" s="5" t="s">
         <v>108</v>
@@ -1818,8 +1824,8 @@
       <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A25" s="27"/>
-      <c r="B25" s="25"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="24"/>
       <c r="C25" s="5" t="s">
         <v>109</v>
       </c>
@@ -1837,7 +1843,7 @@
       <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A26" s="28"/>
+      <c r="A26" s="27"/>
       <c r="B26" s="5" t="s">
         <v>78</v>
       </c>
@@ -1883,7 +1889,7 @@
       <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A28" s="22"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="5" t="s">
         <v>80</v>
       </c>
@@ -1906,7 +1912,7 @@
       <c r="K28" s="5"/>
     </row>
     <row r="29" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A29" s="22"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="5" t="s">
         <v>81</v>
       </c>
@@ -1917,13 +1923,19 @@
       <c r="G29" s="11">
         <v>45803</v>
       </c>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="4"/>
+      <c r="H29" s="11">
+        <v>45806</v>
+      </c>
+      <c r="I29" s="11">
+        <v>45814</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="K29" s="5"/>
     </row>
     <row r="30" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A30" s="22"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="5" t="s">
         <v>84</v>
       </c>
@@ -1940,7 +1952,7 @@
       <c r="K30" s="5"/>
     </row>
     <row r="31" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A31" s="21"/>
+      <c r="A31" s="28"/>
       <c r="B31" s="5" t="s">
         <v>94</v>
       </c>
@@ -1976,7 +1988,7 @@
       <c r="K32" s="5"/>
     </row>
     <row r="33" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A33" s="22"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="5" t="s">
         <v>85</v>
       </c>
@@ -1993,7 +2005,7 @@
       <c r="K33" s="5"/>
     </row>
     <row r="34" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A34" s="22"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="5" t="s">
         <v>86</v>
       </c>
@@ -2028,6 +2040,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C7:C8"/>
     <mergeCell ref="A32:A34"/>
     <mergeCell ref="B4:B8"/>
     <mergeCell ref="B17:B18"/>
@@ -2036,13 +2055,6 @@
     <mergeCell ref="A3:A16"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C7:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2051,10 +2063,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A2:D23"/>
+  <dimension ref="A2:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2283,6 +2295,17 @@
       </c>
       <c r="C23" s="16" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="145.75" x14ac:dyDescent="0.4">
+      <c r="A24" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="15">
+        <v>45814</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: change internal fucntions to static in detection.c and preprocessing.c
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B8257D-184E-42AE-894F-3451F4EA5B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214B8DA5-87D7-4F8A-8544-8EE607CB7309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="123">
   <si>
     <t>Import file</t>
   </si>
@@ -516,9 +516,6 @@
 Need to change in the future if need to refactor</t>
   </si>
   <si>
-    <t>pending</t>
-  </si>
-  <si>
     <t>Gut Model connection to C program</t>
   </si>
   <si>
@@ -549,6 +546,12 @@
 While testing Realtime Dataset Mode on the DE1-SoC board using the setup described above, a segmentation fault occurred. The root cause was likely a stack overflow due to oversized buffers declared within the processing_pipeline function.
 On many embedded Linux systems, including DE1-SoC, the default pthread stack size is often only 64 KB or 128 KB(I tried confirming this from the board terminal, I couldnt). Although I could have increased it using pthread_attr_setstacksize(), I decided against it since future implementations will run on memory-constrained environments like bare-metal systems. 
 Instead, I refactored all large buffer variables inside the pipeline to be file-scoped static variables, allowing them to reside in the .bss segment (static memory) instead of the thread’s stack. This fixed the issue. </t>
+  </si>
+  <si>
+    <t>ongoing</t>
+  </si>
+  <si>
+    <t>Hard to understand Luman's repo so pending to meet with Luman.</t>
   </si>
 </sst>
 </file>
@@ -762,6 +765,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -781,9 +787,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1203,8 +1206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1288,10 +1291,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="30"/>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="23" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -1313,8 +1316,8 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="30"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="5" t="s">
         <v>40</v>
       </c>
@@ -1334,8 +1337,8 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="30"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1355,8 +1358,8 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" s="30"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="23"/>
+      <c r="C7" s="23" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1380,8 +1383,8 @@
     </row>
     <row r="8" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A8" s="30"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
       <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1405,7 +1408,7 @@
     </row>
     <row r="9" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A9" s="30"/>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="23" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="20" t="s">
@@ -1438,8 +1441,8 @@
     </row>
     <row r="10" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A10" s="30"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="28"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1467,7 +1470,7 @@
     </row>
     <row r="11" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A11" s="30"/>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="23" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="20" t="s">
@@ -1500,8 +1503,8 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="30"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="21"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="5" t="s">
         <v>53</v>
       </c>
@@ -1521,8 +1524,8 @@
     </row>
     <row r="13" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A13" s="30"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="28"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="21"/>
       <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
@@ -1584,7 +1587,7 @@
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="28"/>
+      <c r="C15" s="21"/>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1634,10 +1637,10 @@
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="24" t="s">
         <v>76</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -1661,8 +1664,8 @@
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A18" s="26"/>
-      <c r="B18" s="24"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="5" t="s">
         <v>93</v>
       </c>
@@ -1686,7 +1689,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A19" s="26"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="19" t="s">
         <v>77</v>
       </c>
@@ -1713,8 +1716,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A20" s="26"/>
-      <c r="B20" s="22" t="s">
+      <c r="A20" s="27"/>
+      <c r="B20" s="23" t="s">
         <v>97</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -1736,8 +1739,8 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A21" s="26"/>
-      <c r="B21" s="22"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="23"/>
       <c r="C21" s="5" t="s">
         <v>99</v>
       </c>
@@ -1759,8 +1762,8 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="26"/>
-      <c r="B22" s="23" t="s">
+      <c r="A22" s="27"/>
+      <c r="B22" s="24" t="s">
         <v>105</v>
       </c>
       <c r="C22" s="5" t="s">
@@ -1782,7 +1785,7 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A23" s="26"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="31"/>
       <c r="C23" s="5" t="s">
         <v>107</v>
@@ -1803,7 +1806,7 @@
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:11" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A24" s="26"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="31"/>
       <c r="C24" s="5" t="s">
         <v>108</v>
@@ -1824,8 +1827,8 @@
       <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A25" s="26"/>
-      <c r="B25" s="24"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="25"/>
       <c r="C25" s="5" t="s">
         <v>109</v>
       </c>
@@ -1843,7 +1846,7 @@
       <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A26" s="27"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="5" t="s">
         <v>78</v>
       </c>
@@ -1859,9 +1862,11 @@
       </c>
       <c r="I26" s="11"/>
       <c r="J26" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="K26" s="5"/>
+        <v>121</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="27" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A27" s="20" t="s">
@@ -1889,7 +1894,7 @@
       <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A28" s="21"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="5" t="s">
         <v>80</v>
       </c>
@@ -1912,7 +1917,7 @@
       <c r="K28" s="5"/>
     </row>
     <row r="29" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A29" s="21"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="5" t="s">
         <v>81</v>
       </c>
@@ -1935,7 +1940,7 @@
       <c r="K29" s="5"/>
     </row>
     <row r="30" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A30" s="21"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="5" t="s">
         <v>84</v>
       </c>
@@ -1952,7 +1957,7 @@
       <c r="K30" s="5"/>
     </row>
     <row r="31" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A31" s="28"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="5" t="s">
         <v>94</v>
       </c>
@@ -1988,7 +1993,7 @@
       <c r="K32" s="5"/>
     </row>
     <row r="33" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A33" s="21"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="5" t="s">
         <v>85</v>
       </c>
@@ -2005,7 +2010,7 @@
       <c r="K33" s="5"/>
     </row>
     <row r="34" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A34" s="21"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="5" t="s">
         <v>86</v>
       </c>
@@ -2040,13 +2045,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C7:C8"/>
     <mergeCell ref="A32:A34"/>
     <mergeCell ref="B4:B8"/>
     <mergeCell ref="B17:B18"/>
@@ -2055,6 +2053,13 @@
     <mergeCell ref="A3:A16"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C7:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2065,8 +2070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
   <dimension ref="A2:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2277,24 +2282,24 @@
     </row>
     <row r="22" spans="1:3" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B22" s="15">
         <v>45805</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="174.9" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B23" s="15">
         <v>45806</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="145.75" x14ac:dyDescent="0.4">
@@ -2305,7 +2310,7 @@
         <v>45814</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2334,13 +2339,13 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" t="s">
         <v>116</v>
-      </c>
-      <c r="C2" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: add recieving and sending logic to gut model mode(prototype) and updated progress.xlsx
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214B8DA5-87D7-4F8A-8544-8EE607CB7309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24EBF88-2459-49BA-9845-55014156878F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="124">
   <si>
     <t>Import file</t>
   </si>
@@ -552,6 +552,10 @@
   </si>
   <si>
     <t>Hard to understand Luman's repo so pending to meet with Luman.</t>
+  </si>
+  <si>
+    <t>I talked to Luman and got some insight of her repo. Basically all the pacemaker was in a block inside the simulink model and the gut model was a set of several ICC blocks. There were t types of pacemaker blocks, which seem like one just close loop with in cell, others with several cells()channels. I got advised that it might be easier to just work with on cell for now, and move on to more.
+I started back to designing the architecture of how I will connect my C program to the Simulink model. I decided to make some changes from mode 2 (having the TCP server in the C program side). I created a relay server in MATLAB, which is just a layer that relays the signals from the gut model to the program, and the pacing signal from the program to the gut model. It was easier and cleaner that way since I can have the plotting of relayed signals within this layer to visualize signals and pacing. Also, I can keep the functionality separate and modular, the gut model, pacemaker logic, and visualization/relay are decoupled from each other, making debugging and future upgrades much easier. This architecture also allows for better monitoring during experiments and opens the door for future features like logging, signal analysis, or feedback visualization without touching the core pacemaker logic.</t>
   </si>
 </sst>
 </file>
@@ -765,9 +769,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -787,6 +788,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1206,7 +1210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
       <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
@@ -1291,10 +1295,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="30"/>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -1316,8 +1320,8 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="30"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="5" t="s">
         <v>40</v>
       </c>
@@ -1337,8 +1341,8 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="30"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
       <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1358,8 +1362,8 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" s="30"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1383,8 +1387,8 @@
     </row>
     <row r="8" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A8" s="30"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1408,7 +1412,7 @@
     </row>
     <row r="9" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A9" s="30"/>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="20" t="s">
@@ -1441,8 +1445,8 @@
     </row>
     <row r="10" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A10" s="30"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1470,7 +1474,7 @@
     </row>
     <row r="11" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A11" s="30"/>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="20" t="s">
@@ -1503,8 +1507,8 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="30"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="5" t="s">
         <v>53</v>
       </c>
@@ -1524,8 +1528,8 @@
     </row>
     <row r="13" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A13" s="30"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="21"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
@@ -1587,7 +1591,7 @@
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="21"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1637,10 +1641,10 @@
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="23" t="s">
         <v>76</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -1664,8 +1668,8 @@
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A18" s="27"/>
-      <c r="B18" s="25"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="5" t="s">
         <v>93</v>
       </c>
@@ -1689,7 +1693,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A19" s="27"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="19" t="s">
         <v>77</v>
       </c>
@@ -1716,8 +1720,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A20" s="27"/>
-      <c r="B20" s="23" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="22" t="s">
         <v>97</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -1739,8 +1743,8 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A21" s="27"/>
-      <c r="B21" s="23"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="22"/>
       <c r="C21" s="5" t="s">
         <v>99</v>
       </c>
@@ -1762,8 +1766,8 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="27"/>
-      <c r="B22" s="24" t="s">
+      <c r="A22" s="26"/>
+      <c r="B22" s="23" t="s">
         <v>105</v>
       </c>
       <c r="C22" s="5" t="s">
@@ -1785,7 +1789,7 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A23" s="27"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="31"/>
       <c r="C23" s="5" t="s">
         <v>107</v>
@@ -1806,7 +1810,7 @@
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:11" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A24" s="27"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="31"/>
       <c r="C24" s="5" t="s">
         <v>108</v>
@@ -1827,8 +1831,8 @@
       <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A25" s="27"/>
-      <c r="B25" s="25"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="24"/>
       <c r="C25" s="5" t="s">
         <v>109</v>
       </c>
@@ -1846,7 +1850,7 @@
       <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A26" s="28"/>
+      <c r="A26" s="27"/>
       <c r="B26" s="5" t="s">
         <v>78</v>
       </c>
@@ -1894,7 +1898,7 @@
       <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A28" s="22"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="5" t="s">
         <v>80</v>
       </c>
@@ -1917,7 +1921,7 @@
       <c r="K28" s="5"/>
     </row>
     <row r="29" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A29" s="22"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="5" t="s">
         <v>81</v>
       </c>
@@ -1940,7 +1944,7 @@
       <c r="K29" s="5"/>
     </row>
     <row r="30" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A30" s="22"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="5" t="s">
         <v>84</v>
       </c>
@@ -1957,7 +1961,7 @@
       <c r="K30" s="5"/>
     </row>
     <row r="31" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A31" s="21"/>
+      <c r="A31" s="28"/>
       <c r="B31" s="5" t="s">
         <v>94</v>
       </c>
@@ -1993,7 +1997,7 @@
       <c r="K32" s="5"/>
     </row>
     <row r="33" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A33" s="22"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="5" t="s">
         <v>85</v>
       </c>
@@ -2010,7 +2014,7 @@
       <c r="K33" s="5"/>
     </row>
     <row r="34" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A34" s="22"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="5" t="s">
         <v>86</v>
       </c>
@@ -2045,6 +2049,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C7:C8"/>
     <mergeCell ref="A32:A34"/>
     <mergeCell ref="B4:B8"/>
     <mergeCell ref="B17:B18"/>
@@ -2053,13 +2064,6 @@
     <mergeCell ref="A3:A16"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C7:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2068,10 +2072,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A2:D24"/>
+  <dimension ref="A2:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2291,25 +2295,33 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="174.9" x14ac:dyDescent="0.4">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:3" ht="160.30000000000001" x14ac:dyDescent="0.4">
+      <c r="B23" s="15">
+        <v>45815</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="174.9" x14ac:dyDescent="0.4">
+      <c r="A24" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B24" s="15">
         <v>45806</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C24" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="145.75" x14ac:dyDescent="0.4">
-      <c r="A24" s="2" t="s">
+    <row r="25" spans="1:3" ht="145.75" x14ac:dyDescent="0.4">
+      <c r="A25" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B24" s="15">
+      <c r="B25" s="15">
         <v>45814</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C25" s="16" t="s">
         <v>120</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: reintroduced Gut Model Mode and tcp server implementaions within it
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24EBF88-2459-49BA-9845-55014156878F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8CDB71-9AF0-40CE-9405-496A54043A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="20205" yWindow="1320" windowWidth="16455" windowHeight="9458" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="132">
   <si>
     <t>Import file</t>
   </si>
@@ -556,6 +556,37 @@
   <si>
     <t>I talked to Luman and got some insight of her repo. Basically all the pacemaker was in a block inside the simulink model and the gut model was a set of several ICC blocks. There were t types of pacemaker blocks, which seem like one just close loop with in cell, others with several cells()channels. I got advised that it might be easier to just work with on cell for now, and move on to more.
 I started back to designing the architecture of how I will connect my C program to the Simulink model. I decided to make some changes from mode 2 (having the TCP server in the C program side). I created a relay server in MATLAB, which is just a layer that relays the signals from the gut model to the program, and the pacing signal from the program to the gut model. It was easier and cleaner that way since I can have the plotting of relayed signals within this layer to visualize signals and pacing. Also, I can keep the functionality separate and modular, the gut model, pacemaker logic, and visualization/relay are decoupled from each other, making debugging and future upgrades much easier. This architecture also allows for better monitoring during experiments and opens the door for future features like logging, signal analysis, or feedback visualization without touching the core pacemaker logic.</t>
+  </si>
+  <si>
+    <t>need to test</t>
+  </si>
+  <si>
+    <t>Relay Server</t>
+  </si>
+  <si>
+    <t>Luman's repo analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After analysing Luman's repo again, I found that connection to the gut model and applying the pacemaker algorithm post the current processing pipeline(Part4 algorithm) is more complex that I thought due to below.
+1. The shape of the activation signals from Luman's gut model is not shaped like the activation signals in the datasets(recorded signals used by the part 4s)
+2. Luman's activation detection algorithm relies on a threshold that was calculated using 60 to 120 seconds of the initial signal, forming an adaptive baseline, whereas the Part 4 students' detection method used edge detection with a static threshold applied to a fixed window, without adapting to long-term signal trends.
+3. </t>
+  </si>
+  <si>
+    <t>need to complete</t>
+  </si>
+  <si>
+    <t>Relay server implementations above, I though it was working great. But after more testing,  I found that some samples were lost during the signal relay(the pacemaker was not receiving all samples), I think due to timing issues. There things wer going on,
+1. relay signals
+2. relay pacing
+3. plot signals and pacing
+Im not 100% sure this is the problem so will do some testing to confirm. I tried using multithreading to solve this but MATLAB's multithreading interface does not have data sharing, which made things complex</t>
+  </si>
+  <si>
+    <t>Another problem is that when run simulink and a separate matlab instance with the relay server, seems to be a lag in the gutmodels side sending the signal. The task manager show about 90% of RAM memory usage(32GB RAM) which i think is not sustainable. I Think I will try just implementing a server in a simulink block instead.</t>
+  </si>
+  <si>
+    <t>I attempted this, I was not able to find a simple way todo this and the overhead of learning simulink is too big. I decieded to go back to the old implementation of having the server in the c pacemaker program instead.</t>
   </si>
 </sst>
 </file>
@@ -611,7 +642,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -621,6 +652,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -707,7 +744,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -769,6 +806,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -790,9 +830,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -804,6 +841,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1210,7 +1253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
@@ -1295,10 +1338,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="30"/>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="23" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -1320,8 +1363,8 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="30"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="5" t="s">
         <v>40</v>
       </c>
@@ -1341,8 +1384,8 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="30"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1362,8 +1405,8 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" s="30"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="23"/>
+      <c r="C7" s="23" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1387,8 +1430,8 @@
     </row>
     <row r="8" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A8" s="30"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
       <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1412,7 +1455,7 @@
     </row>
     <row r="9" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A9" s="30"/>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="23" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="20" t="s">
@@ -1445,8 +1488,8 @@
     </row>
     <row r="10" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A10" s="30"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="28"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1474,7 +1517,7 @@
     </row>
     <row r="11" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A11" s="30"/>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="23" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="20" t="s">
@@ -1507,8 +1550,8 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="30"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="21"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="5" t="s">
         <v>53</v>
       </c>
@@ -1528,8 +1571,8 @@
     </row>
     <row r="13" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A13" s="30"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="28"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="21"/>
       <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
@@ -1591,7 +1634,7 @@
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="28"/>
+      <c r="C15" s="21"/>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1641,10 +1684,10 @@
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="24" t="s">
         <v>76</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -1668,8 +1711,8 @@
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A18" s="26"/>
-      <c r="B18" s="24"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="5" t="s">
         <v>93</v>
       </c>
@@ -1693,7 +1736,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A19" s="26"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="19" t="s">
         <v>77</v>
       </c>
@@ -1720,8 +1763,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A20" s="26"/>
-      <c r="B20" s="22" t="s">
+      <c r="A20" s="27"/>
+      <c r="B20" s="23" t="s">
         <v>97</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -1743,8 +1786,8 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A21" s="26"/>
-      <c r="B21" s="22"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="23"/>
       <c r="C21" s="5" t="s">
         <v>99</v>
       </c>
@@ -1766,8 +1809,8 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="26"/>
-      <c r="B22" s="23" t="s">
+      <c r="A22" s="27"/>
+      <c r="B22" s="24" t="s">
         <v>105</v>
       </c>
       <c r="C22" s="5" t="s">
@@ -1789,7 +1832,7 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A23" s="26"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="31"/>
       <c r="C23" s="5" t="s">
         <v>107</v>
@@ -1810,7 +1853,7 @@
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:11" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A24" s="26"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="31"/>
       <c r="C24" s="5" t="s">
         <v>108</v>
@@ -1831,8 +1874,8 @@
       <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A25" s="26"/>
-      <c r="B25" s="24"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="25"/>
       <c r="C25" s="5" t="s">
         <v>109</v>
       </c>
@@ -1850,7 +1893,7 @@
       <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A26" s="27"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="5" t="s">
         <v>78</v>
       </c>
@@ -1898,7 +1941,7 @@
       <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A28" s="21"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="5" t="s">
         <v>80</v>
       </c>
@@ -1921,7 +1964,7 @@
       <c r="K28" s="5"/>
     </row>
     <row r="29" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A29" s="21"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="5" t="s">
         <v>81</v>
       </c>
@@ -1944,7 +1987,7 @@
       <c r="K29" s="5"/>
     </row>
     <row r="30" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A30" s="21"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="5" t="s">
         <v>84</v>
       </c>
@@ -1961,7 +2004,7 @@
       <c r="K30" s="5"/>
     </row>
     <row r="31" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A31" s="28"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="5" t="s">
         <v>94</v>
       </c>
@@ -1997,7 +2040,7 @@
       <c r="K32" s="5"/>
     </row>
     <row r="33" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A33" s="21"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="5" t="s">
         <v>85</v>
       </c>
@@ -2014,7 +2057,7 @@
       <c r="K33" s="5"/>
     </row>
     <row r="34" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A34" s="21"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="5" t="s">
         <v>86</v>
       </c>
@@ -2049,13 +2092,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C7:C8"/>
     <mergeCell ref="A32:A34"/>
     <mergeCell ref="B4:B8"/>
     <mergeCell ref="B17:B18"/>
@@ -2064,6 +2100,13 @@
     <mergeCell ref="A3:A16"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C7:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2072,264 +2115,324 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A2:D25"/>
+  <dimension ref="A2:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="14.4609375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.23046875" style="15"/>
-    <col min="3" max="3" width="114.23046875" style="16" customWidth="1"/>
-    <col min="4" max="4" width="47.15234375" style="14" customWidth="1"/>
-    <col min="5" max="16384" width="9.23046875" style="14"/>
+    <col min="2" max="2" width="10.07421875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.23046875" style="15"/>
+    <col min="4" max="4" width="114.23046875" style="16" customWidth="1"/>
+    <col min="5" max="5" width="47.15234375" style="14" customWidth="1"/>
+    <col min="6" max="16384" width="9.23046875" style="14"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A2" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="15">
+      <c r="C2" s="15">
         <v>45723</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="D2" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="14" t="e" vm="1">
+      <c r="E2" s="14" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A3" s="32"/>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="14" t="e" vm="2">
+      <c r="E3" s="14" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="306" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="306" x14ac:dyDescent="0.4">
       <c r="A4" s="32"/>
-      <c r="B4" s="15">
+      <c r="C4" s="15">
         <v>45728</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="D4" s="16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="160.30000000000001" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="15">
+      <c r="C5" s="15">
         <v>45730</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="D5" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A6" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="15">
+      <c r="C6" s="15">
         <v>45733</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="D6" s="16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A7" s="32"/>
-      <c r="B7" s="15">
+      <c r="C7" s="15">
         <v>45798</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="D7" s="16" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="15">
+      <c r="C8" s="15">
         <v>45734</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="D8" s="16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="116.6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="15">
+      <c r="C9" s="15">
         <v>45734</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="D9" s="16" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="145.75" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="15">
+      <c r="C10" s="15">
         <v>45736</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="D10" s="16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="102" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" ht="102" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="15">
+      <c r="C11" s="15">
         <v>45742</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="D11" s="16" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="160.30000000000001" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A12" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="15">
+      <c r="C12" s="15">
         <v>45743</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="D12" s="16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="291.45" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" ht="291.45" x14ac:dyDescent="0.4">
       <c r="A13" s="32"/>
-      <c r="B13" s="15">
+      <c r="C13" s="15">
         <v>45743</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="D13" s="16" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="116.6" x14ac:dyDescent="0.4">
-      <c r="B14" s="15">
+    <row r="14" spans="1:5" ht="116.6" x14ac:dyDescent="0.4">
+      <c r="C14" s="15">
         <v>45743</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="D14" s="16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="B15" s="15">
+    <row r="15" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="C15" s="15">
         <v>45743</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="D15" s="16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="233.15" x14ac:dyDescent="0.4">
-      <c r="B16" s="15">
+    <row r="16" spans="1:5" ht="233.15" x14ac:dyDescent="0.4">
+      <c r="C16" s="15">
         <v>45747</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="D16" s="16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="B17" s="15">
+    <row r="17" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="C17" s="15">
         <v>45747</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="D17" s="17" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="B18" s="15">
+    <row r="18" spans="1:5" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="C18" s="15">
         <v>45765</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="D18" s="16" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="B19" s="15">
+    <row r="19" spans="1:5" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="C19" s="15">
         <v>45770</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="D19" s="16" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="145.75" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B20" s="15">
+      <c r="C20" s="15">
         <v>45783</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="D20" s="16" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="102" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" ht="102" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B21" s="15">
+      <c r="C21" s="15">
         <v>45794</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="D21" s="16" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:5" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A22" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" s="15">
         <v>45805</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="D22" s="16" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="160.30000000000001" x14ac:dyDescent="0.4">
-      <c r="B23" s="15">
+    <row r="23" spans="1:5" ht="160.30000000000001" x14ac:dyDescent="0.4">
+      <c r="A23" s="27"/>
+      <c r="B23" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C23" s="15">
         <v>45815</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="D23" s="16" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="174.9" x14ac:dyDescent="0.4">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:5" ht="102" x14ac:dyDescent="0.4">
+      <c r="A24" s="27"/>
+      <c r="B24" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="15">
+        <v>45817</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A25" s="27"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="15">
+        <v>45820</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="15">
+        <v>45820</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="116.6" x14ac:dyDescent="0.4">
+      <c r="A27" s="27"/>
+      <c r="B27" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="15">
+        <v>45819</v>
+      </c>
+      <c r="D27" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="174.9" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B24" s="15">
+      <c r="C28" s="15">
         <v>45806</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="D28" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="145.75" x14ac:dyDescent="0.4">
-      <c r="A25" s="2" t="s">
+    <row r="29" spans="1:5" ht="145.75" x14ac:dyDescent="0.4">
+      <c r="A29" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B25" s="15">
+      <c r="C29" s="15">
         <v>45814</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="D29" s="16" t="s">
         <v>120</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="B24:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
chore : update progress.xlsx and rename constant vars
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8CDB71-9AF0-40CE-9405-496A54043A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F94236-8382-4F50-9BF9-98A87D1401A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20205" yWindow="1320" windowWidth="16455" windowHeight="9458" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="133">
   <si>
     <t>Import file</t>
   </si>
@@ -558,19 +558,10 @@
 I started back to designing the architecture of how I will connect my C program to the Simulink model. I decided to make some changes from mode 2 (having the TCP server in the C program side). I created a relay server in MATLAB, which is just a layer that relays the signals from the gut model to the program, and the pacing signal from the program to the gut model. It was easier and cleaner that way since I can have the plotting of relayed signals within this layer to visualize signals and pacing. Also, I can keep the functionality separate and modular, the gut model, pacemaker logic, and visualization/relay are decoupled from each other, making debugging and future upgrades much easier. This architecture also allows for better monitoring during experiments and opens the door for future features like logging, signal analysis, or feedback visualization without touching the core pacemaker logic.</t>
   </si>
   <si>
-    <t>need to test</t>
-  </si>
-  <si>
     <t>Relay Server</t>
   </si>
   <si>
     <t>Luman's repo analysis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">After analysing Luman's repo again, I found that connection to the gut model and applying the pacemaker algorithm post the current processing pipeline(Part4 algorithm) is more complex that I thought due to below.
-1. The shape of the activation signals from Luman's gut model is not shaped like the activation signals in the datasets(recorded signals used by the part 4s)
-2. Luman's activation detection algorithm relies on a threshold that was calculated using 60 to 120 seconds of the initial signal, forming an adaptive baseline, whereas the Part 4 students' detection method used edge detection with a static threshold applied to a fixed window, without adapting to long-term signal trends.
-3. </t>
   </si>
   <si>
     <t>need to complete</t>
@@ -587,6 +578,34 @@
   </si>
   <si>
     <t>I attempted this, I was not able to find a simple way todo this and the overhead of learning simulink is too big. I decieded to go back to the old implementation of having the server in the c pacemaker program instead.</t>
+  </si>
+  <si>
+    <t>After analysing Luman's repo again, I found that connection to the gut model and applying the pacemaker algorithm post the current processing pipeline(Part4 algorithm) is more complex that I thought due to below.
+1. The shape of the activation signals from Luman's gut model is not shaped like the activation signals in the datasets(recorded signals used by the part 4s). Not just that, dataset and the signals produced by Luman's gut model are too different.
+2. Luman's activation detection algorithm relies on a threshold that was calculated using 60 to 120 seconds of the initial signal, forming an adaptive baseline, whereas the Part 4 students' detection method used edge detection with a static threshold applied to a fixed window, without adapting to long-term signal trends.
+3. I tried processing the gut model's signals with the part 4's processing alg and the activations detection implementations removes the activation signals, and no activations is detected, I assume since the activations are removed(the Cprogram doesnot have a scope to see whats going on so not sure)
+The delema here is, part4's signal processing and activation detection pipeline does not work with the gut model, and to make it work there are sereral options.
+1. Modify the pipeline to use the part4's signal processing with Luman's activation detection
+       - this is a really messy and a headache, since the basic buffering and threshold calculation is very different
+2. Fix the part4's pipeline to work with the gut model.
+3. Throw away the part4's pipeline that I created and recreate Luman's 
+And I realized that I went down this rabbit hole last time and the focus of my reseach was hardware implementation not optimizing a pacemaker algorithm.
+So I decided that,
+1. Dispite the result of the part4s pipeline when connected to the gut model, just append Luman's pacing algorythm and continue the hardware implementation.</t>
+  </si>
+  <si>
+    <t>not using this method anymore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have a few thing from further analyse of Luman's simulink project.
+1. Why does the activation signal wave from the gut model not look like the activations in the datasets?
+2. Why is the EGM1_2 not showing any signal? Isnt the 1st cell suppose to have a signal since it drives the other cells?
+3. What do I set in param2_n2.m to simulate...
+     - a cell with no activation
+     - slow activation 
+     - what is the defination of "block case" in the file?
+4. Which channel should I hook up to just connect to single channel?(input and output)
+</t>
   </si>
 </sst>
 </file>
@@ -744,7 +763,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -803,33 +822,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -841,9 +866,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1253,32 +1275,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.765625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.15234375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.765625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="25.921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.4609375" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="72.23046875" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="6.765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.765625" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.23046875" style="9"/>
-    <col min="10" max="10" width="9.23046875" style="1"/>
-    <col min="11" max="11" width="60.84375" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.23046875" style="1"/>
+    <col min="1" max="1" width="10.7265625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.7265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.453125" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="72.26953125" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.26953125" style="9"/>
+    <col min="10" max="10" width="9.26953125" style="1"/>
+    <col min="11" max="11" width="60.81640625" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.26953125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
     </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>88</v>
       </c>
@@ -1311,8 +1333,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A3" s="29" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="31" t="s">
         <v>82</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1336,12 +1358,12 @@
       </c>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A4" s="30"/>
-      <c r="B4" s="23" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="32"/>
+      <c r="B4" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="24" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -1361,10 +1383,10 @@
       </c>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A5" s="30"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="32"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="5" t="s">
         <v>40</v>
       </c>
@@ -1382,10 +1404,10 @@
       </c>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A6" s="30"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="32"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1403,10 +1425,10 @@
       </c>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A7" s="30"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="32"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1428,10 +1450,10 @@
       </c>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A8" s="30"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
+    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="32"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1453,12 +1475,12 @@
       </c>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:11" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A9" s="30"/>
-      <c r="B9" s="23" t="s">
+    <row r="9" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="32"/>
+      <c r="B9" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="22" t="s">
         <v>57</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1486,10 +1508,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A10" s="30"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="21"/>
+    <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="32"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1515,12 +1537,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A11" s="30"/>
-      <c r="B11" s="23" t="s">
+    <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="32"/>
+      <c r="B11" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="22" t="s">
         <v>58</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1548,10 +1570,10 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A12" s="30"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="22"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="32"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="23"/>
       <c r="D12" s="5" t="s">
         <v>53</v>
       </c>
@@ -1569,10 +1591,10 @@
       </c>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A13" s="30"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="21"/>
+    <row r="13" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="32"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
@@ -1598,12 +1620,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A14" s="30"/>
+    <row r="14" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="32"/>
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="22" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -1629,12 +1651,12 @@
       </c>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A15" s="30"/>
+    <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="32"/>
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="21"/>
+      <c r="C15" s="30"/>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1658,8 +1680,8 @@
       </c>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A16" s="30"/>
+    <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="32"/>
       <c r="B16" s="5" t="s">
         <v>43</v>
       </c>
@@ -1683,11 +1705,11 @@
       </c>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A17" s="26" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="25" t="s">
         <v>76</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -1710,9 +1732,9 @@
       </c>
       <c r="K17" s="5"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A18" s="27"/>
-      <c r="B18" s="25"/>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="28"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="5" t="s">
         <v>93</v>
       </c>
@@ -1735,8 +1757,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A19" s="27"/>
+    <row r="19" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="28"/>
       <c r="B19" s="19" t="s">
         <v>77</v>
       </c>
@@ -1762,9 +1784,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A20" s="27"/>
-      <c r="B20" s="23" t="s">
+    <row r="20" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="28"/>
+      <c r="B20" s="24" t="s">
         <v>97</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -1785,9 +1807,9 @@
       </c>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A21" s="27"/>
-      <c r="B21" s="23"/>
+    <row r="21" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="28"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="5" t="s">
         <v>99</v>
       </c>
@@ -1808,9 +1830,9 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="27"/>
-      <c r="B22" s="24" t="s">
+    <row r="22" spans="1:11" ht="14.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="28"/>
+      <c r="B22" s="25" t="s">
         <v>105</v>
       </c>
       <c r="C22" s="5" t="s">
@@ -1831,9 +1853,9 @@
       </c>
       <c r="K22" s="5"/>
     </row>
-    <row r="23" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A23" s="27"/>
-      <c r="B23" s="31"/>
+    <row r="23" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="28"/>
+      <c r="B23" s="33"/>
       <c r="C23" s="5" t="s">
         <v>107</v>
       </c>
@@ -1852,9 +1874,9 @@
       </c>
       <c r="K23" s="5"/>
     </row>
-    <row r="24" spans="1:11" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A24" s="27"/>
-      <c r="B24" s="31"/>
+    <row r="24" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A24" s="28"/>
+      <c r="B24" s="33"/>
       <c r="C24" s="5" t="s">
         <v>108</v>
       </c>
@@ -1873,9 +1895,9 @@
       </c>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A25" s="27"/>
-      <c r="B25" s="25"/>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" s="28"/>
+      <c r="B25" s="26"/>
       <c r="C25" s="5" t="s">
         <v>109</v>
       </c>
@@ -1892,8 +1914,8 @@
       </c>
       <c r="K25" s="5"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A26" s="28"/>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26" s="29"/>
       <c r="B26" s="5" t="s">
         <v>78</v>
       </c>
@@ -1907,7 +1929,9 @@
       <c r="H26" s="11">
         <v>45805</v>
       </c>
-      <c r="I26" s="11"/>
+      <c r="I26" s="11">
+        <v>45820</v>
+      </c>
       <c r="J26" s="4" t="s">
         <v>121</v>
       </c>
@@ -1915,8 +1939,8 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A27" s="20" t="s">
+    <row r="27" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="22" t="s">
         <v>79</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -1940,8 +1964,8 @@
       </c>
       <c r="K27" s="5"/>
     </row>
-    <row r="28" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A28" s="22"/>
+    <row r="28" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="23"/>
       <c r="B28" s="5" t="s">
         <v>80</v>
       </c>
@@ -1963,8 +1987,8 @@
       </c>
       <c r="K28" s="5"/>
     </row>
-    <row r="29" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A29" s="22"/>
+    <row r="29" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="23"/>
       <c r="B29" s="5" t="s">
         <v>81</v>
       </c>
@@ -1986,8 +2010,8 @@
       </c>
       <c r="K29" s="5"/>
     </row>
-    <row r="30" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A30" s="22"/>
+    <row r="30" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="23"/>
       <c r="B30" s="5" t="s">
         <v>84</v>
       </c>
@@ -2003,8 +2027,8 @@
       <c r="J30" s="4"/>
       <c r="K30" s="5"/>
     </row>
-    <row r="31" spans="1:11" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A31" s="21"/>
+    <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="30"/>
       <c r="B31" s="5" t="s">
         <v>94</v>
       </c>
@@ -2020,8 +2044,8 @@
       <c r="J31" s="4"/>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A32" s="20" t="s">
+    <row r="32" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="22" t="s">
         <v>83</v>
       </c>
       <c r="B32" s="5" t="s">
@@ -2039,8 +2063,8 @@
       <c r="J32" s="4"/>
       <c r="K32" s="5"/>
     </row>
-    <row r="33" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A33" s="22"/>
+    <row r="33" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33" s="23"/>
       <c r="B33" s="5" t="s">
         <v>85</v>
       </c>
@@ -2056,8 +2080,8 @@
       <c r="J33" s="4"/>
       <c r="K33" s="5"/>
     </row>
-    <row r="34" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A34" s="22"/>
+    <row r="34" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="23"/>
       <c r="B34" s="5" t="s">
         <v>86</v>
       </c>
@@ -2073,7 +2097,7 @@
       <c r="J34" s="4"/>
       <c r="K34" s="5"/>
     </row>
-    <row r="35" spans="1:11" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>87</v>
       </c>
@@ -2092,6 +2116,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C7:C8"/>
     <mergeCell ref="A32:A34"/>
     <mergeCell ref="B4:B8"/>
     <mergeCell ref="B17:B18"/>
@@ -2100,13 +2131,6 @@
     <mergeCell ref="A3:A16"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C7:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2115,24 +2139,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A2:E29"/>
+  <dimension ref="A2:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.4609375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.07421875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.23046875" style="15"/>
-    <col min="4" max="4" width="114.23046875" style="16" customWidth="1"/>
-    <col min="5" max="5" width="47.15234375" style="14" customWidth="1"/>
-    <col min="6" max="16384" width="9.23046875" style="14"/>
+    <col min="1" max="1" width="14.453125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.26953125" style="15"/>
+    <col min="4" max="4" width="114.26953125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="47.1796875" style="14" customWidth="1"/>
+    <col min="6" max="16384" width="9.26953125" style="14"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="34" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="15">
@@ -2145,8 +2169,8 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A3" s="32"/>
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="34"/>
       <c r="D3" s="16" t="s">
         <v>46</v>
       </c>
@@ -2154,8 +2178,8 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="306" x14ac:dyDescent="0.4">
-      <c r="A4" s="32"/>
+    <row r="4" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="34"/>
       <c r="C4" s="15">
         <v>45728</v>
       </c>
@@ -2163,7 +2187,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="160.30000000000001" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>47</v>
       </c>
@@ -2174,8 +2198,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A6" s="32" t="s">
+    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="34" t="s">
         <v>50</v>
       </c>
       <c r="C6" s="15">
@@ -2185,8 +2209,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A7" s="32"/>
+    <row r="7" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="34"/>
       <c r="C7" s="15">
         <v>45798</v>
       </c>
@@ -2194,7 +2218,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>51</v>
       </c>
@@ -2205,7 +2229,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="116.6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>54</v>
       </c>
@@ -2216,7 +2240,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="145.75" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -2227,7 +2251,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="102" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>68</v>
       </c>
@@ -2238,8 +2262,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="160.30000000000001" x14ac:dyDescent="0.4">
-      <c r="A12" s="32" t="s">
+    <row r="12" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="34" t="s">
         <v>65</v>
       </c>
       <c r="C12" s="15">
@@ -2249,8 +2273,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="291.45" x14ac:dyDescent="0.4">
-      <c r="A13" s="32"/>
+    <row r="13" spans="1:5" ht="290" x14ac:dyDescent="0.35">
+      <c r="A13" s="34"/>
       <c r="C13" s="15">
         <v>45743</v>
       </c>
@@ -2258,7 +2282,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="116.6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="C14" s="15">
         <v>45743</v>
       </c>
@@ -2266,7 +2290,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C15" s="15">
         <v>45743</v>
       </c>
@@ -2274,7 +2298,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="233.15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="C16" s="15">
         <v>45747</v>
       </c>
@@ -2282,7 +2306,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C17" s="15">
         <v>45747</v>
       </c>
@@ -2290,7 +2314,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="C18" s="15">
         <v>45765</v>
       </c>
@@ -2298,7 +2322,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="C19" s="15">
         <v>45770</v>
       </c>
@@ -2306,7 +2330,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="145.75" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>99</v>
       </c>
@@ -2317,7 +2341,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="102" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>110</v>
       </c>
@@ -2328,12 +2352,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="A22" s="27" t="s">
+    <row r="22" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A22" s="28" t="s">
         <v>113</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C22" s="15">
         <v>45805</v>
@@ -2342,10 +2366,10 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="160.30000000000001" x14ac:dyDescent="0.4">
-      <c r="A23" s="27"/>
+    <row r="23" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="28"/>
       <c r="B23" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C23" s="15">
         <v>45815</v>
@@ -2354,85 +2378,96 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="102" x14ac:dyDescent="0.4">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27" t="s">
-        <v>125</v>
+    <row r="24" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="28"/>
+      <c r="B24" s="28" t="s">
+        <v>124</v>
       </c>
       <c r="C24" s="15">
         <v>45817</v>
       </c>
-      <c r="D24" s="33" t="s">
-        <v>129</v>
+      <c r="D24" s="35" t="s">
+        <v>127</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A25" s="27"/>
-      <c r="B25" s="27"/>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="28"/>
+      <c r="B25" s="28"/>
       <c r="C25" s="15">
         <v>45820</v>
       </c>
-      <c r="D25" s="34" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A26" s="27"/>
-      <c r="B26" s="27"/>
+      <c r="D25" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="28"/>
+      <c r="B26" s="28"/>
       <c r="C26" s="15">
         <v>45820</v>
       </c>
-      <c r="D26" s="34" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="116.6" x14ac:dyDescent="0.4">
-      <c r="A27" s="27"/>
-      <c r="B27" s="2" t="s">
-        <v>126</v>
+      <c r="D26" s="16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="28"/>
+      <c r="B27" s="28" t="s">
+        <v>125</v>
       </c>
       <c r="C27" s="15">
         <v>45819</v>
       </c>
-      <c r="D27" s="33" t="s">
-        <v>127</v>
+      <c r="D27" s="35" t="s">
+        <v>130</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="174.9" x14ac:dyDescent="0.4">
-      <c r="A28" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="20"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="15">
+        <v>45821</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="174" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C29" s="15">
         <v>45806</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D29" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="145.75" x14ac:dyDescent="0.4">
-      <c r="A29" s="2" t="s">
+    <row r="30" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C30" s="15">
         <v>45814</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D30" s="16" t="s">
         <v>120</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A22:A27"/>
     <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B27:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2447,12 +2482,12 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="54.23046875" customWidth="1"/>
+    <col min="1" max="1" width="54.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>117</v>
       </c>

</xml_diff>

<commit_message>
refactor: refactror to make easy modifications for future multi channel implementations
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F94236-8382-4F50-9BF9-98A87D1401A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245C88E0-6401-4A1D-BAA9-FC94EC6B64F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="134">
   <si>
     <t>Import file</t>
   </si>
@@ -606,6 +606,9 @@
      - what is the defination of "block case" in the file?
 4. Which channel should I hook up to just connect to single channel?(input and output)
 </t>
+  </si>
+  <si>
+    <t>I was going to just append the pacing part of Lumans simulink model the C program's signal processing and detection pipeline, but I struggled to come up with a strategy to link the two together due to how its bufferings were different. So I just recreated all of Luman's activation detection and pacing alg. I tested Luman's activation detection and pacing alg that I created in C, linked with the gut model and it generates a pace exactly like the pacemaker in the Simulink model. Next I will try to link the pacing output back to the simulink model and check if it works.</t>
   </si>
 </sst>
 </file>
@@ -763,7 +766,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -831,6 +834,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -852,9 +858,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -866,9 +869,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1276,7 +1276,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1360,10 +1360,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="32"/>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="25" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -1385,8 +1385,8 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="32"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
       <c r="D5" s="5" t="s">
         <v>40</v>
       </c>
@@ -1406,8 +1406,8 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="32"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
       <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1427,8 +1427,8 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="32"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24" t="s">
+      <c r="B7" s="25"/>
+      <c r="C7" s="25" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1452,8 +1452,8 @@
     </row>
     <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="32"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
       <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1477,7 +1477,7 @@
     </row>
     <row r="9" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="32"/>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="25" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="22" t="s">
@@ -1510,8 +1510,8 @@
     </row>
     <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="32"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="30"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1539,7 +1539,7 @@
     </row>
     <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="32"/>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="25" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="22" t="s">
@@ -1572,8 +1572,8 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="32"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="23"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="5" t="s">
         <v>53</v>
       </c>
@@ -1593,8 +1593,8 @@
     </row>
     <row r="13" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="32"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="30"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="23"/>
       <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
@@ -1656,7 +1656,7 @@
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="30"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1706,10 +1706,10 @@
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="26" t="s">
         <v>76</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -1733,8 +1733,8 @@
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="28"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="5" t="s">
         <v>93</v>
       </c>
@@ -1758,7 +1758,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="28"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="19" t="s">
         <v>77</v>
       </c>
@@ -1785,8 +1785,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="28"/>
-      <c r="B20" s="24" t="s">
+      <c r="A20" s="29"/>
+      <c r="B20" s="25" t="s">
         <v>97</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -1808,8 +1808,8 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="28"/>
-      <c r="B21" s="24"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="5" t="s">
         <v>99</v>
       </c>
@@ -1831,8 +1831,8 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="14.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="28"/>
-      <c r="B22" s="25" t="s">
+      <c r="A22" s="29"/>
+      <c r="B22" s="26" t="s">
         <v>105</v>
       </c>
       <c r="C22" s="5" t="s">
@@ -1854,7 +1854,7 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="28"/>
+      <c r="A23" s="29"/>
       <c r="B23" s="33"/>
       <c r="C23" s="5" t="s">
         <v>107</v>
@@ -1875,7 +1875,7 @@
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="28"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="33"/>
       <c r="C24" s="5" t="s">
         <v>108</v>
@@ -1896,8 +1896,8 @@
       <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="28"/>
-      <c r="B25" s="26"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="27"/>
       <c r="C25" s="5" t="s">
         <v>109</v>
       </c>
@@ -1915,7 +1915,7 @@
       <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="29"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="5" t="s">
         <v>78</v>
       </c>
@@ -1965,7 +1965,7 @@
       <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="23"/>
+      <c r="A28" s="24"/>
       <c r="B28" s="5" t="s">
         <v>80</v>
       </c>
@@ -1988,7 +1988,7 @@
       <c r="K28" s="5"/>
     </row>
     <row r="29" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="23"/>
+      <c r="A29" s="24"/>
       <c r="B29" s="5" t="s">
         <v>81</v>
       </c>
@@ -2011,7 +2011,7 @@
       <c r="K29" s="5"/>
     </row>
     <row r="30" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="23"/>
+      <c r="A30" s="24"/>
       <c r="B30" s="5" t="s">
         <v>84</v>
       </c>
@@ -2022,13 +2022,17 @@
       <c r="G30" s="11">
         <v>45810</v>
       </c>
-      <c r="H30" s="11"/>
+      <c r="H30" s="11">
+        <v>45814</v>
+      </c>
       <c r="I30" s="11"/>
-      <c r="J30" s="4"/>
+      <c r="J30" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="K30" s="5"/>
     </row>
     <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="30"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="5" t="s">
         <v>94</v>
       </c>
@@ -2064,7 +2068,7 @@
       <c r="K32" s="5"/>
     </row>
     <row r="33" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="23"/>
+      <c r="A33" s="24"/>
       <c r="B33" s="5" t="s">
         <v>85</v>
       </c>
@@ -2081,7 +2085,7 @@
       <c r="K33" s="5"/>
     </row>
     <row r="34" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="23"/>
+      <c r="A34" s="24"/>
       <c r="B34" s="5" t="s">
         <v>86</v>
       </c>
@@ -2116,13 +2120,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C7:C8"/>
     <mergeCell ref="A32:A34"/>
     <mergeCell ref="B4:B8"/>
     <mergeCell ref="B17:B18"/>
@@ -2131,6 +2128,13 @@
     <mergeCell ref="A3:A16"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C7:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2139,10 +2143,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A2:E30"/>
+  <dimension ref="A2:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2353,7 +2357,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="29" t="s">
         <v>113</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2367,7 +2371,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="28"/>
+      <c r="A23" s="29"/>
       <c r="B23" s="2" t="s">
         <v>124</v>
       </c>
@@ -2379,14 +2383,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28" t="s">
+      <c r="A24" s="29"/>
+      <c r="B24" s="29" t="s">
         <v>124</v>
       </c>
       <c r="C24" s="15">
         <v>45817</v>
       </c>
-      <c r="D24" s="35" t="s">
+      <c r="D24" s="16" t="s">
         <v>127</v>
       </c>
       <c r="E24" s="14" t="s">
@@ -2394,8 +2398,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="28"/>
-      <c r="B25" s="28"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
       <c r="C25" s="15">
         <v>45820</v>
       </c>
@@ -2404,8 +2408,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="28"/>
-      <c r="B26" s="28"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
       <c r="C26" s="15">
         <v>45820</v>
       </c>
@@ -2414,14 +2418,14 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28" t="s">
+      <c r="A27" s="29"/>
+      <c r="B27" s="29" t="s">
         <v>125</v>
       </c>
       <c r="C27" s="15">
         <v>45819</v>
       </c>
-      <c r="D27" s="35" t="s">
+      <c r="D27" s="16" t="s">
         <v>130</v>
       </c>
       <c r="E27" s="14" t="s">
@@ -2430,7 +2434,7 @@
     </row>
     <row r="28" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A28" s="20"/>
-      <c r="B28" s="28"/>
+      <c r="B28" s="29"/>
       <c r="C28" s="15">
         <v>45821</v>
       </c>
@@ -2458,6 +2462,17 @@
       </c>
       <c r="D30" s="16" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="15">
+        <v>45832</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: rename pointer vars in shared data to enhance readability, update progress.xlsx
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Personal\Research\gut-pacemaker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245C88E0-6401-4A1D-BAA9-FC94EC6B64F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97496167-D3E3-4AB1-9711-1606234B88FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="149">
   <si>
     <t>Import file</t>
   </si>
@@ -441,16 +441,10 @@
     <t>Initial env prep for DE1-Soc</t>
   </si>
   <si>
-    <t>Initial bare metal dev env prep</t>
-  </si>
-  <si>
     <t>Research &amp; Review</t>
   </si>
   <si>
     <t>Implementation</t>
-  </si>
-  <si>
-    <t>Migrate pacing functionality to board</t>
   </si>
   <si>
     <t>Implemented TCP server in C program</t>
@@ -609,6 +603,57 @@
   </si>
   <si>
     <t>I was going to just append the pacing part of Lumans simulink model the C program's signal processing and detection pipeline, but I struggled to come up with a strategy to link the two together due to how its bufferings were different. So I just recreated all of Luman's activation detection and pacing alg. I tested Luman's activation detection and pacing alg that I created in C, linked with the gut model and it generates a pace exactly like the pacemaker in the Simulink model. Next I will try to link the pacing output back to the simulink model and check if it works.</t>
+  </si>
+  <si>
+    <t>Replace TCP comm to UART</t>
+  </si>
+  <si>
+    <t>Setup FlexPRET in Verilator</t>
+  </si>
+  <si>
+    <t>Understanding FlexPRET &amp; Verilator</t>
+  </si>
+  <si>
+    <t>Setup</t>
+  </si>
+  <si>
+    <t>Test UART comm and pacing functionality on DE1-Soc on ARM Linux</t>
+  </si>
+  <si>
+    <t>Replace pthread with bare-metal task scheduling</t>
+  </si>
+  <si>
+    <t>Replace TCP-based communication with UART to enable direct serial transfer of data from the gut model. This change eliminates the overhead of socket programming and aligns with the hardware interface typically used in embedded systems, such as STM32 or DE1-SoC platforms.</t>
+  </si>
+  <si>
+    <t>Replace pthread with a bare-metal-compatible task scheduling approach, as the final system will run without an OS. Since pthread isn’t supported on bare-metal platforms like STM32 or DE1-SoC, alternatives approaches such as a cooperative super loop, timer-based scheduling, or interrupt-driven execution. This change ensures compatibility while maintaining real-time responsiveness for tasks like signal reception and pacing control.</t>
+  </si>
+  <si>
+    <t>Step 7 - Research Thesis</t>
+  </si>
+  <si>
+    <t>Planning &amp; Context</t>
+  </si>
+  <si>
+    <t>Finalizing</t>
+  </si>
+  <si>
+    <t>UART</t>
+  </si>
+  <si>
+    <t>Separate Pacemaker and GES</t>
+  </si>
+  <si>
+    <t>Testing on DE1-SoC's HPS bare metal mode</t>
+  </si>
+  <si>
+    <t>Understanding bare metal programming</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>The TCP communication of the gut model and the pacemaker will not be possible eventually on FlexPRET. Transitioning from TCP to UART at this stage and then testing on DE1SoC's HPS(Hard Processor System)'s bare metal mode will make the migration to FlexPRET easier, thus seems to be a nessesary process. I plan use virtual UART port pairing to simulate this within PC, then test on the board.</t>
   </si>
 </sst>
 </file>
@@ -832,23 +877,26 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -863,9 +911,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1273,10 +1318,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1334,7 +1379,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="32" t="s">
         <v>82</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1359,11 +1404,11 @@
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="32"/>
-      <c r="B4" s="25" t="s">
+      <c r="A4" s="33"/>
+      <c r="B4" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="28" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -1384,9 +1429,9 @@
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="32"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="5" t="s">
         <v>40</v>
       </c>
@@ -1405,9 +1450,9 @@
       <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="32"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1426,9 +1471,9 @@
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="32"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25" t="s">
+      <c r="A7" s="33"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1451,9 +1496,9 @@
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="32"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1476,11 +1521,11 @@
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="32"/>
-      <c r="B9" s="25" t="s">
+      <c r="A9" s="33"/>
+      <c r="B9" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="24" t="s">
         <v>57</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1509,9 +1554,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="32"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="23"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1538,11 +1583,11 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="32"/>
-      <c r="B11" s="25" t="s">
+      <c r="A11" s="33"/>
+      <c r="B11" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="24" t="s">
         <v>58</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1571,9 +1616,9 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="32"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="24"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="5" t="s">
         <v>53</v>
       </c>
@@ -1592,9 +1637,9 @@
       <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="32"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="23"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="26"/>
       <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
@@ -1621,11 +1666,11 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="32"/>
+      <c r="A14" s="33"/>
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="24" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -1652,11 +1697,11 @@
       <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="32"/>
+      <c r="A15" s="33"/>
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="23"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1681,7 +1726,7 @@
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="32"/>
+      <c r="A16" s="33"/>
       <c r="B16" s="5" t="s">
         <v>43</v>
       </c>
@@ -1706,14 +1751,14 @@
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="22" t="s">
         <v>76</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1733,10 +1778,10 @@
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="29"/>
-      <c r="B18" s="27"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1754,16 +1799,16 @@
         <v>24</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="29"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="19" t="s">
         <v>77</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1781,16 +1826,16 @@
         <v>24</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="29"/>
-      <c r="B20" s="25" t="s">
-        <v>97</v>
+      <c r="A20" s="30"/>
+      <c r="B20" s="28" t="s">
+        <v>95</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -1808,10 +1853,10 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="29"/>
-      <c r="B21" s="25"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="28"/>
       <c r="C21" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -1827,16 +1872,16 @@
         <v>24</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="14.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="29"/>
-      <c r="B22" s="26" t="s">
-        <v>105</v>
+      <c r="A22" s="30"/>
+      <c r="B22" s="22" t="s">
+        <v>103</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -1854,10 +1899,10 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="29"/>
-      <c r="B23" s="33"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="27"/>
       <c r="C23" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -1875,10 +1920,10 @@
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="29"/>
-      <c r="B24" s="33"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="27"/>
       <c r="C24" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -1896,10 +1941,10 @@
       <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="29"/>
-      <c r="B25" s="27"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
@@ -1915,7 +1960,7 @@
       <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="30"/>
+      <c r="A26" s="31"/>
       <c r="B26" s="5" t="s">
         <v>78</v>
       </c>
@@ -1933,14 +1978,14 @@
         <v>45820</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="24" t="s">
         <v>79</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -1965,7 +2010,7 @@
       <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="24"/>
+      <c r="A28" s="25"/>
       <c r="B28" s="5" t="s">
         <v>80</v>
       </c>
@@ -1988,7 +2033,7 @@
       <c r="K28" s="5"/>
     </row>
     <row r="29" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="24"/>
+      <c r="A29" s="25"/>
       <c r="B29" s="5" t="s">
         <v>81</v>
       </c>
@@ -2011,7 +2056,7 @@
       <c r="K29" s="5"/>
     </row>
     <row r="30" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="24"/>
+      <c r="A30" s="25"/>
       <c r="B30" s="5" t="s">
         <v>84</v>
       </c>
@@ -2025,106 +2070,287 @@
       <c r="H30" s="11">
         <v>45814</v>
       </c>
-      <c r="I30" s="11"/>
+      <c r="I30" s="11">
+        <v>45835</v>
+      </c>
       <c r="J30" s="4" t="s">
-        <v>121</v>
+        <v>24</v>
       </c>
       <c r="K30" s="5"/>
     </row>
     <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="23"/>
-      <c r="B31" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C31" s="5"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>144</v>
+      </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="11">
-        <v>45817</v>
-      </c>
-      <c r="H31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11">
+        <v>45835</v>
+      </c>
       <c r="I31" s="11"/>
-      <c r="J31" s="4"/>
+      <c r="J31" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" s="5"/>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32" s="25"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="5" t="s">
+        <v>143</v>
+      </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="11">
-        <v>45824</v>
-      </c>
-      <c r="H32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11">
+        <v>45835</v>
+      </c>
       <c r="I32" s="11"/>
-      <c r="J32" s="4"/>
+      <c r="J32" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="K32" s="5"/>
     </row>
-    <row r="33" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="24"/>
+    <row r="33" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A33" s="25"/>
       <c r="B33" s="5" t="s">
-        <v>85</v>
+        <v>136</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="11">
-        <v>45831</v>
+        <v>45838</v>
       </c>
       <c r="H33" s="11"/>
       <c r="I33" s="11"/>
       <c r="J33" s="4"/>
-      <c r="K33" s="5"/>
-    </row>
-    <row r="34" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="24"/>
-      <c r="B34" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C34" s="5"/>
+      <c r="K33" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="25"/>
+      <c r="B34" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>92</v>
+      </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="11">
-        <v>45838</v>
+        <v>45845</v>
       </c>
       <c r="H34" s="11"/>
       <c r="I34" s="11"/>
       <c r="J34" s="4"/>
-      <c r="K34" s="5"/>
-    </row>
-    <row r="35" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A35" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="K34" s="22" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="25"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>146</v>
+      </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="11">
-        <v>45845</v>
+        <v>45852</v>
       </c>
       <c r="H35" s="11"/>
       <c r="I35" s="11"/>
       <c r="J35" s="4"/>
-      <c r="K35" s="5"/>
+      <c r="K35" s="27"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A36" s="26"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="11">
+        <v>45859</v>
+      </c>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="23"/>
+    </row>
+    <row r="37" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="11">
+        <v>45866</v>
+      </c>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="5"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A38" s="25"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="11">
+        <v>45873</v>
+      </c>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="5"/>
+    </row>
+    <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" s="25"/>
+      <c r="B39" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="11">
+        <v>45880</v>
+      </c>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="5"/>
+    </row>
+    <row r="40" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A40" s="25"/>
+      <c r="B40" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="11">
+        <v>45887</v>
+      </c>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="5"/>
+    </row>
+    <row r="41" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A41" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="11">
+        <v>45894</v>
+      </c>
+      <c r="H41" s="11">
+        <v>45900</v>
+      </c>
+      <c r="I41" s="11"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="5"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A42" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="11">
+        <v>45901</v>
+      </c>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="5"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A43" s="27"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="5"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A44" s="23"/>
+      <c r="B44" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="11">
+        <v>45929</v>
+      </c>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="5"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="B4:B8"/>
+  <mergeCells count="21">
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="A17:A26"/>
-    <mergeCell ref="A27:A31"/>
     <mergeCell ref="A3:A16"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B25"/>
@@ -2135,6 +2361,15 @@
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="A27:A36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="K34:K36"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B37:B38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2143,10 +2378,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A2:E31"/>
+  <dimension ref="A2:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2219,7 +2454,7 @@
         <v>45798</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="87" x14ac:dyDescent="0.35">
@@ -2323,7 +2558,7 @@
         <v>45765</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="87" x14ac:dyDescent="0.35">
@@ -2331,126 +2566,126 @@
         <v>45770</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C20" s="15">
         <v>45783</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C21" s="15">
         <v>45794</v>
       </c>
       <c r="D21" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A22" s="30" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A22" s="29" t="s">
-        <v>113</v>
-      </c>
       <c r="B22" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C22" s="15">
         <v>45805</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="29"/>
+      <c r="A23" s="30"/>
       <c r="B23" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C23" s="15">
         <v>45815</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="29"/>
-      <c r="B24" s="29" t="s">
-        <v>124</v>
+      <c r="A24" s="30"/>
+      <c r="B24" s="30" t="s">
+        <v>122</v>
       </c>
       <c r="C24" s="15">
         <v>45817</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="29"/>
-      <c r="B25" s="29"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="30"/>
       <c r="C25" s="15">
         <v>45820</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="29"/>
-      <c r="B26" s="29"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
       <c r="C26" s="15">
         <v>45820</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="29"/>
-      <c r="B27" s="29" t="s">
-        <v>125</v>
+      <c r="A27" s="30"/>
+      <c r="B27" s="30" t="s">
+        <v>123</v>
       </c>
       <c r="C27" s="15">
         <v>45819</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A28" s="20"/>
-      <c r="B28" s="29"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="15">
         <v>45821</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C29" s="15">
         <v>45806</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="145" x14ac:dyDescent="0.35">
@@ -2461,7 +2696,7 @@
         <v>45814</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
@@ -2472,7 +2707,18 @@
         <v>45832</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>133</v>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" s="15">
+        <v>45836</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2504,13 +2750,13 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: restructure directories for ease of future implementations
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97496167-D3E3-4AB1-9711-1606234B88FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB8F1EC-E392-475F-B6E6-417C4F07A914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -638,9 +638,6 @@
     <t>Finalizing</t>
   </si>
   <si>
-    <t>UART</t>
-  </si>
-  <si>
     <t>Separate Pacemaker and GES</t>
   </si>
   <si>
@@ -654,6 +651,9 @@
   </si>
   <si>
     <t>The TCP communication of the gut model and the pacemaker will not be possible eventually on FlexPRET. Transitioning from TCP to UART at this stage and then testing on DE1SoC's HPS(Hard Processor System)'s bare metal mode will make the migration to FlexPRET easier, thus seems to be a nessesary process. I plan use virtual UART port pairing to simulate this within PC, then test on the board.</t>
+  </si>
+  <si>
+    <t>Create UART driver</t>
   </si>
 </sst>
 </file>
@@ -882,35 +882,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1318,10 +1318,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1379,7 +1379,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="27" t="s">
         <v>82</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1404,11 +1404,11 @@
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="33"/>
-      <c r="B4" s="28" t="s">
+      <c r="A4" s="28"/>
+      <c r="B4" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="29" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -1429,9 +1429,9 @@
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="33"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="5" t="s">
         <v>40</v>
       </c>
@@ -1450,9 +1450,9 @@
       <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="33"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1471,9 +1471,9 @@
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="33"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28" t="s">
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1496,9 +1496,9 @@
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="33"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1521,11 +1521,11 @@
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="33"/>
-      <c r="B9" s="28" t="s">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="31" t="s">
         <v>57</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1554,9 +1554,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="33"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="26"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="32"/>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1583,11 +1583,11 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="33"/>
-      <c r="B11" s="28" t="s">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="31" t="s">
         <v>58</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1616,9 +1616,9 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="33"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="25"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="33"/>
       <c r="D12" s="5" t="s">
         <v>53</v>
       </c>
@@ -1637,9 +1637,9 @@
       <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="33"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="26"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
@@ -1666,11 +1666,11 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="33"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="31" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -1697,11 +1697,11 @@
       <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="33"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="26"/>
+      <c r="C15" s="32"/>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1726,7 +1726,7 @@
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="33"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="5" t="s">
         <v>43</v>
       </c>
@@ -1751,7 +1751,7 @@
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="24" t="s">
         <v>75</v>
       </c>
       <c r="B17" s="22" t="s">
@@ -1778,7 +1778,7 @@
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="30"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="23"/>
       <c r="C18" s="5" t="s">
         <v>92</v>
@@ -1803,7 +1803,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="30"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="19" t="s">
         <v>77</v>
       </c>
@@ -1830,8 +1830,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="30"/>
-      <c r="B20" s="28" t="s">
+      <c r="A20" s="25"/>
+      <c r="B20" s="29" t="s">
         <v>95</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -1853,8 +1853,8 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="30"/>
-      <c r="B21" s="28"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="5" t="s">
         <v>97</v>
       </c>
@@ -1876,7 +1876,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="14.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="30"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="22" t="s">
         <v>103</v>
       </c>
@@ -1899,8 +1899,8 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="30"/>
-      <c r="B23" s="27"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="5" t="s">
         <v>105</v>
       </c>
@@ -1920,8 +1920,8 @@
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="30"/>
-      <c r="B24" s="27"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="5" t="s">
         <v>106</v>
       </c>
@@ -1941,7 +1941,7 @@
       <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="30"/>
+      <c r="A25" s="25"/>
       <c r="B25" s="23"/>
       <c r="C25" s="5" t="s">
         <v>107</v>
@@ -1960,7 +1960,7 @@
       <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="31"/>
+      <c r="A26" s="26"/>
       <c r="B26" s="5" t="s">
         <v>78</v>
       </c>
@@ -1985,7 +1985,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="31" t="s">
         <v>79</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -2010,7 +2010,7 @@
       <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="25"/>
+      <c r="A28" s="33"/>
       <c r="B28" s="5" t="s">
         <v>80</v>
       </c>
@@ -2033,7 +2033,7 @@
       <c r="K28" s="5"/>
     </row>
     <row r="29" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="25"/>
+      <c r="A29" s="33"/>
       <c r="B29" s="5" t="s">
         <v>81</v>
       </c>
@@ -2056,7 +2056,7 @@
       <c r="K29" s="5"/>
     </row>
     <row r="30" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="25"/>
+      <c r="A30" s="33"/>
       <c r="B30" s="5" t="s">
         <v>84</v>
       </c>
@@ -2079,12 +2079,12 @@
       <c r="K30" s="5"/>
     </row>
     <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="25"/>
+      <c r="A31" s="33"/>
       <c r="B31" s="22" t="s">
         <v>132</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
@@ -2100,10 +2100,10 @@
       <c r="K31" s="5"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" s="25"/>
+      <c r="A32" s="33"/>
       <c r="B32" s="23"/>
       <c r="C32" s="5" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
@@ -2119,7 +2119,7 @@
       <c r="K32" s="5"/>
     </row>
     <row r="33" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A33" s="25"/>
+      <c r="A33" s="33"/>
       <c r="B33" s="5" t="s">
         <v>136</v>
       </c>
@@ -2137,112 +2137,108 @@
         <v>138</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="25"/>
-      <c r="B34" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>92</v>
-      </c>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A34" s="33"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
-      <c r="G34" s="11">
-        <v>45845</v>
-      </c>
+      <c r="G34" s="11"/>
       <c r="H34" s="11"/>
       <c r="I34" s="11"/>
       <c r="J34" s="4"/>
-      <c r="K34" s="22" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="25"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>146</v>
-      </c>
+      <c r="K34" s="12"/>
+    </row>
+    <row r="35" spans="1:11" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="33"/>
+      <c r="B35" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="11">
-        <v>45852</v>
+        <v>45845</v>
       </c>
       <c r="H35" s="11"/>
       <c r="I35" s="11"/>
       <c r="J35" s="4"/>
-      <c r="K35" s="27"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A36" s="26"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
+      <c r="K35" s="22" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" s="33"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="22" t="s">
+        <v>144</v>
+      </c>
       <c r="D36" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="11">
-        <v>45859</v>
+        <v>45852</v>
       </c>
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
       <c r="J36" s="4"/>
-      <c r="K36" s="23"/>
-    </row>
-    <row r="37" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="B37" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D37" s="5"/>
+      <c r="K36" s="30"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A37" s="32"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="5" t="s">
+        <v>146</v>
+      </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="11">
-        <v>45866</v>
+        <v>45859</v>
       </c>
       <c r="H37" s="11"/>
       <c r="I37" s="11"/>
       <c r="J37" s="4"/>
-      <c r="K37" s="5"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A38" s="25"/>
-      <c r="B38" s="27"/>
+      <c r="K37" s="23"/>
+    </row>
+    <row r="38" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>133</v>
+      </c>
       <c r="C38" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="11">
-        <v>45873</v>
+        <v>45866</v>
       </c>
       <c r="H38" s="11"/>
       <c r="I38" s="11"/>
       <c r="J38" s="4"/>
       <c r="K38" s="5"/>
     </row>
-    <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="25"/>
-      <c r="B39" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C39" s="5"/>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A39" s="33"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="5" t="s">
+        <v>135</v>
+      </c>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="11">
-        <v>45880</v>
+        <v>45873</v>
       </c>
       <c r="H39" s="11"/>
       <c r="I39" s="11"/>
@@ -2250,110 +2246,130 @@
       <c r="K39" s="5"/>
     </row>
     <row r="40" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="25"/>
+      <c r="A40" s="33"/>
       <c r="B40" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="11">
-        <v>45887</v>
+        <v>45880</v>
       </c>
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
       <c r="J40" s="4"/>
       <c r="K40" s="5"/>
     </row>
-    <row r="41" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A41" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B41" s="5"/>
+    <row r="41" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="33"/>
+      <c r="B41" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
       <c r="G41" s="11">
-        <v>45894</v>
-      </c>
-      <c r="H41" s="11">
-        <v>45900</v>
-      </c>
+        <v>45887</v>
+      </c>
+      <c r="H41" s="11"/>
       <c r="I41" s="11"/>
       <c r="J41" s="4"/>
       <c r="K41" s="5"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A42" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>141</v>
-      </c>
+    <row r="42" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A42" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="11">
-        <v>45901</v>
-      </c>
-      <c r="H42" s="11"/>
+        <v>45894</v>
+      </c>
+      <c r="H42" s="11">
+        <v>45900</v>
+      </c>
       <c r="I42" s="11"/>
       <c r="J42" s="4"/>
       <c r="K42" s="5"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A43" s="27"/>
-      <c r="B43" s="5"/>
+      <c r="A43" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>141</v>
+      </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
-      <c r="G43" s="11"/>
+      <c r="G43" s="11">
+        <v>45901</v>
+      </c>
       <c r="H43" s="11"/>
       <c r="I43" s="11"/>
       <c r="J43" s="4"/>
       <c r="K43" s="5"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A44" s="23"/>
-      <c r="B44" s="5" t="s">
-        <v>142</v>
-      </c>
+      <c r="A44" s="30"/>
+      <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
-      <c r="G44" s="11">
-        <v>45929</v>
-      </c>
+      <c r="G44" s="11"/>
       <c r="H44" s="11"/>
       <c r="I44" s="11"/>
       <c r="J44" s="4"/>
       <c r="K44" s="5"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="5" t="s">
+        <v>142</v>
+      </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
-      <c r="G45" s="11"/>
+      <c r="G45" s="11">
+        <v>45929</v>
+      </c>
       <c r="H45" s="11"/>
       <c r="I45" s="11"/>
       <c r="J45" s="4"/>
       <c r="K45" s="5"/>
     </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A17:A26"/>
-    <mergeCell ref="A3:A16"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="A27:A37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="K35:K37"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B38:B39"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C15"/>
@@ -2362,14 +2378,11 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B4:B8"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="A27:A36"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="K34:K36"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A17:A26"/>
+    <mergeCell ref="A3:A16"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2380,7 +2393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
   <dimension ref="A2:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -2592,7 +2605,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="25" t="s">
         <v>111</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2606,7 +2619,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="30"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="2" t="s">
         <v>122</v>
       </c>
@@ -2618,8 +2631,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30" t="s">
+      <c r="A24" s="25"/>
+      <c r="B24" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C24" s="15">
@@ -2633,8 +2646,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="30"/>
-      <c r="B25" s="30"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="25"/>
       <c r="C25" s="15">
         <v>45820</v>
       </c>
@@ -2643,8 +2656,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="30"/>
-      <c r="B26" s="30"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="25"/>
       <c r="C26" s="15">
         <v>45820</v>
       </c>
@@ -2653,8 +2666,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="30"/>
-      <c r="B27" s="30" t="s">
+      <c r="A27" s="25"/>
+      <c r="B27" s="25" t="s">
         <v>123</v>
       </c>
       <c r="C27" s="15">
@@ -2669,7 +2682,7 @@
     </row>
     <row r="28" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A28" s="20"/>
-      <c r="B28" s="30"/>
+      <c r="B28" s="25"/>
       <c r="C28" s="15">
         <v>45821</v>
       </c>
@@ -2718,7 +2731,7 @@
         <v>45836</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature: add execution time timer and enhance logging
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB8F1EC-E392-475F-B6E6-417C4F07A914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B9B367-1469-4E45-AA65-1651D7525016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="152">
   <si>
     <t>Import file</t>
   </si>
@@ -654,6 +654,23 @@
   </si>
   <si>
     <t>Create UART driver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">folder restructuring -&gt; commited
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buffer skipping error fix. 
+- Add buffer skip check
+- Add execution time check
+- Skipping buffer found in pc mode(after DETECTION IGNORE)
+- Skipping buffer also found in board, after DETECTION IGNORE when running via ssh teminal, and randomly much more frequently when running via putty
+I found that using PuTTY over USB-UART causes printf() to block due to slow serial output, which delays your processing thread and leads to buffer skips — unlike SSH, which handles output quickly over a fast, buffered TCP connection.
+I removed the pace signal sending code block(which was right before the signal recieve block in the server funciton) and it didnt skip any buffers.  </t>
+  </si>
+  <si>
+    <t>The process skipping only happens when the scope is connected to the input signal and the output sample signal in simulink. It seems to cause some kind of blocking because of the matlab excecutions. interestingly, when I test the pacemaker and the simulink on the same device(both in pc), skipping occures with or without scope(more so when the pace signal is connected to the scope), especially after detection ignore. but if i run the pacemaker in the board, without scopes connectedot just the gut signal connected, no skipping occurs. I am assuming the gut model's reaction computation to the pace signal is requires alot of performance power. 
+So it is recommended to run the gut model or the pacemaker terminal in a different device to not get any buffer skips. Although the skips(if not running via UART in putty) are process thread skips, thus not skipping signals, which is not critical in the outcome of  pacmaker.</t>
   </si>
 </sst>
 </file>
@@ -882,6 +899,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -896,21 +928,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1320,8 +1337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1329,7 +1346,7 @@
     <col min="1" max="1" width="10.7265625" style="2" customWidth="1"/>
     <col min="2" max="2" width="17.1796875" style="2" customWidth="1"/>
     <col min="3" max="3" width="16.7265625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="25.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.453125" style="2" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="72.26953125" style="2" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="6.7265625" style="2" bestFit="1" customWidth="1"/>
@@ -1379,7 +1396,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="32" t="s">
         <v>82</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1404,11 +1421,11 @@
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29" t="s">
+      <c r="A4" s="33"/>
+      <c r="B4" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="28" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -1429,9 +1446,9 @@
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="28"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="5" t="s">
         <v>40</v>
       </c>
@@ -1450,9 +1467,9 @@
       <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1470,10 +1487,10 @@
       </c>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="28"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29" t="s">
+    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="33"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1496,9 +1513,9 @@
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1521,11 +1538,11 @@
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="28"/>
-      <c r="B9" s="29" t="s">
+      <c r="A9" s="33"/>
+      <c r="B9" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="24" t="s">
         <v>57</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1554,9 +1571,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="28"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="32"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1583,11 +1600,11 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="28"/>
-      <c r="B11" s="29" t="s">
+      <c r="A11" s="33"/>
+      <c r="B11" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="24" t="s">
         <v>58</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1616,9 +1633,9 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="28"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="33"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="5" t="s">
         <v>53</v>
       </c>
@@ -1637,9 +1654,9 @@
       <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="28"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="32"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="26"/>
       <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
@@ -1666,11 +1683,11 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="28"/>
+      <c r="A14" s="33"/>
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="24" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -1697,11 +1714,11 @@
       <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="28"/>
+      <c r="A15" s="33"/>
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="32"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1726,7 +1743,7 @@
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="28"/>
+      <c r="A16" s="33"/>
       <c r="B16" s="5" t="s">
         <v>43</v>
       </c>
@@ -1751,7 +1768,7 @@
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="29" t="s">
         <v>75</v>
       </c>
       <c r="B17" s="22" t="s">
@@ -1778,7 +1795,7 @@
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="25"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="23"/>
       <c r="C18" s="5" t="s">
         <v>92</v>
@@ -1803,7 +1820,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="25"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="19" t="s">
         <v>77</v>
       </c>
@@ -1830,8 +1847,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="25"/>
-      <c r="B20" s="29" t="s">
+      <c r="A20" s="30"/>
+      <c r="B20" s="28" t="s">
         <v>95</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -1853,8 +1870,8 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="25"/>
-      <c r="B21" s="29"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="28"/>
       <c r="C21" s="5" t="s">
         <v>97</v>
       </c>
@@ -1876,7 +1893,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="14.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="25"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="22" t="s">
         <v>103</v>
       </c>
@@ -1899,8 +1916,8 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="25"/>
-      <c r="B23" s="30"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="27"/>
       <c r="C23" s="5" t="s">
         <v>105</v>
       </c>
@@ -1920,8 +1937,8 @@
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="25"/>
-      <c r="B24" s="30"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="27"/>
       <c r="C24" s="5" t="s">
         <v>106</v>
       </c>
@@ -1941,7 +1958,7 @@
       <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="25"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="23"/>
       <c r="C25" s="5" t="s">
         <v>107</v>
@@ -1960,7 +1977,7 @@
       <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="26"/>
+      <c r="A26" s="31"/>
       <c r="B26" s="5" t="s">
         <v>78</v>
       </c>
@@ -1985,7 +2002,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="24" t="s">
         <v>79</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -2010,7 +2027,7 @@
       <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="33"/>
+      <c r="A28" s="25"/>
       <c r="B28" s="5" t="s">
         <v>80</v>
       </c>
@@ -2033,7 +2050,7 @@
       <c r="K28" s="5"/>
     </row>
     <row r="29" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="33"/>
+      <c r="A29" s="25"/>
       <c r="B29" s="5" t="s">
         <v>81</v>
       </c>
@@ -2056,7 +2073,7 @@
       <c r="K29" s="5"/>
     </row>
     <row r="30" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="33"/>
+      <c r="A30" s="25"/>
       <c r="B30" s="5" t="s">
         <v>84</v>
       </c>
@@ -2079,7 +2096,7 @@
       <c r="K30" s="5"/>
     </row>
     <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="33"/>
+      <c r="A31" s="25"/>
       <c r="B31" s="22" t="s">
         <v>132</v>
       </c>
@@ -2100,7 +2117,7 @@
       <c r="K31" s="5"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" s="33"/>
+      <c r="A32" s="25"/>
       <c r="B32" s="23"/>
       <c r="C32" s="5" t="s">
         <v>148</v>
@@ -2119,7 +2136,7 @@
       <c r="K32" s="5"/>
     </row>
     <row r="33" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A33" s="33"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="5" t="s">
         <v>136</v>
       </c>
@@ -2138,7 +2155,7 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A34" s="33"/>
+      <c r="A34" s="25"/>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="5"/>
@@ -2151,7 +2168,7 @@
       <c r="K34" s="12"/>
     </row>
     <row r="35" spans="1:11" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="33"/>
+      <c r="A35" s="25"/>
       <c r="B35" s="22" t="s">
         <v>137</v>
       </c>
@@ -2172,8 +2189,8 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="33"/>
-      <c r="B36" s="30"/>
+      <c r="A36" s="25"/>
+      <c r="B36" s="27"/>
       <c r="C36" s="22" t="s">
         <v>144</v>
       </c>
@@ -2188,10 +2205,10 @@
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
       <c r="J36" s="4"/>
-      <c r="K36" s="30"/>
+      <c r="K36" s="27"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A37" s="32"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="23"/>
       <c r="C37" s="23"/>
       <c r="D37" s="5" t="s">
@@ -2207,8 +2224,8 @@
       <c r="J37" s="4"/>
       <c r="K37" s="23"/>
     </row>
-    <row r="38" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="31" t="s">
+    <row r="38" spans="1:11" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="24" t="s">
         <v>83</v>
       </c>
       <c r="B38" s="22" t="s">
@@ -2229,8 +2246,8 @@
       <c r="K38" s="5"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A39" s="33"/>
-      <c r="B39" s="30"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="27"/>
       <c r="C39" s="5" t="s">
         <v>135</v>
       </c>
@@ -2246,7 +2263,7 @@
       <c r="K39" s="5"/>
     </row>
     <row r="40" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="33"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="5" t="s">
         <v>85</v>
       </c>
@@ -2263,7 +2280,7 @@
       <c r="K40" s="5"/>
     </row>
     <row r="41" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="33"/>
+      <c r="A41" s="25"/>
       <c r="B41" s="5" t="s">
         <v>86</v>
       </c>
@@ -2318,7 +2335,7 @@
       <c r="K43" s="5"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A44" s="30"/>
+      <c r="A44" s="27"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
@@ -2362,6 +2379,19 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A17:A26"/>
+    <mergeCell ref="A3:A16"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B4:B8"/>
     <mergeCell ref="C36:C37"/>
     <mergeCell ref="A27:A37"/>
     <mergeCell ref="B35:B37"/>
@@ -2370,19 +2400,6 @@
     <mergeCell ref="A38:A41"/>
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A17:A26"/>
-    <mergeCell ref="A3:A16"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2391,16 +2408,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A2:E32"/>
+  <dimension ref="A2:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.453125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.08984375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" style="2" customWidth="1"/>
     <col min="3" max="3" width="9.26953125" style="15"/>
     <col min="4" max="4" width="114.26953125" style="16" customWidth="1"/>
     <col min="5" max="5" width="47.1796875" style="14" customWidth="1"/>
@@ -2605,7 +2622,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="30" t="s">
         <v>111</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2619,7 +2636,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="25"/>
+      <c r="A23" s="30"/>
       <c r="B23" s="2" t="s">
         <v>122</v>
       </c>
@@ -2631,8 +2648,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="25"/>
-      <c r="B24" s="25" t="s">
+      <c r="A24" s="30"/>
+      <c r="B24" s="30" t="s">
         <v>122</v>
       </c>
       <c r="C24" s="15">
@@ -2646,8 +2663,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="25"/>
-      <c r="B25" s="25"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="30"/>
       <c r="C25" s="15">
         <v>45820</v>
       </c>
@@ -2656,8 +2673,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="25"/>
-      <c r="B26" s="25"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
       <c r="C26" s="15">
         <v>45820</v>
       </c>
@@ -2666,8 +2683,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="25"/>
-      <c r="B27" s="25" t="s">
+      <c r="A27" s="30"/>
+      <c r="B27" s="30" t="s">
         <v>123</v>
       </c>
       <c r="C27" s="15">
@@ -2682,7 +2699,7 @@
     </row>
     <row r="28" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A28" s="20"/>
-      <c r="B28" s="25"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="15">
         <v>45821</v>
       </c>
@@ -2732,6 +2749,30 @@
       </c>
       <c r="D32" s="16" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="C33" s="15">
+        <v>45838</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" ht="145" x14ac:dyDescent="0.35">
+      <c r="C34" s="15">
+        <v>45839</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" ht="116" x14ac:dyDescent="0.35">
+      <c r="C35" s="15">
+        <v>45840</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature: create linux UART driver and made replacement from tcp to uart comm in test mode
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B9B367-1469-4E45-AA65-1651D7525016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED7038C-47D0-4DCB-A5F4-9480DDBE71AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="156">
   <si>
     <t>Import file</t>
   </si>
@@ -617,15 +617,9 @@
     <t>Setup</t>
   </si>
   <si>
-    <t>Test UART comm and pacing functionality on DE1-Soc on ARM Linux</t>
-  </si>
-  <si>
     <t>Replace pthread with bare-metal task scheduling</t>
   </si>
   <si>
-    <t>Replace TCP-based communication with UART to enable direct serial transfer of data from the gut model. This change eliminates the overhead of socket programming and aligns with the hardware interface typically used in embedded systems, such as STM32 or DE1-SoC platforms.</t>
-  </si>
-  <si>
     <t>Replace pthread with a bare-metal-compatible task scheduling approach, as the final system will run without an OS. Since pthread isn’t supported on bare-metal platforms like STM32 or DE1-SoC, alternatives approaches such as a cooperative super loop, timer-based scheduling, or interrupt-driven execution. This change ensures compatibility while maintaining real-time responsiveness for tasks like signal reception and pacing control.</t>
   </si>
   <si>
@@ -647,13 +641,7 @@
     <t>Understanding bare metal programming</t>
   </si>
   <si>
-    <t>Testing</t>
-  </si>
-  <si>
     <t>The TCP communication of the gut model and the pacemaker will not be possible eventually on FlexPRET. Transitioning from TCP to UART at this stage and then testing on DE1SoC's HPS(Hard Processor System)'s bare metal mode will make the migration to FlexPRET easier, thus seems to be a nessesary process. I plan use virtual UART port pairing to simulate this within PC, then test on the board.</t>
-  </si>
-  <si>
-    <t>Create UART driver</t>
   </si>
   <si>
     <t xml:space="preserve">folder restructuring -&gt; commited
@@ -671,6 +659,31 @@
   <si>
     <t>The process skipping only happens when the scope is connected to the input signal and the output sample signal in simulink. It seems to cause some kind of blocking because of the matlab excecutions. interestingly, when I test the pacemaker and the simulink on the same device(both in pc), skipping occures with or without scope(more so when the pace signal is connected to the scope), especially after detection ignore. but if i run the pacemaker in the board, without scopes connectedot just the gut signal connected, no skipping occurs. I am assuming the gut model's reaction computation to the pace signal is requires alot of performance power. 
 So it is recommended to run the gut model or the pacemaker terminal in a different device to not get any buffer skips. Although the skips(if not running via UART in putty) are process thread skips, thus not skipping signals, which is not critical in the outcome of  pacmaker.</t>
+  </si>
+  <si>
+    <t>Restructuring folder structure</t>
+  </si>
+  <si>
+    <t>Create UART driver for DE1SoC HPS</t>
+  </si>
+  <si>
+    <t>Test UART comm and pacing functionality on DE1-Soc HPS</t>
+  </si>
+  <si>
+    <t>Implement UART comm for ARM Linux</t>
+  </si>
+  <si>
+    <t>Test on ARM Linux</t>
+  </si>
+  <si>
+    <t>Driver dev</t>
+  </si>
+  <si>
+    <t>Create a test trans and recv app for testing</t>
+  </si>
+  <si>
+    <t>Created UART driver for linux(not arm_linux)
+Create a Virtual UART TCP server bridge in Ubuntu</t>
   </si>
 </sst>
 </file>
@@ -828,7 +841,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -899,38 +912,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1335,9 +1351,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -1396,7 +1412,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="27" t="s">
         <v>82</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1421,11 +1437,11 @@
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="33"/>
-      <c r="B4" s="28" t="s">
+      <c r="A4" s="28"/>
+      <c r="B4" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="29" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -1446,9 +1462,9 @@
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="33"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="5" t="s">
         <v>40</v>
       </c>
@@ -1467,9 +1483,9 @@
       <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="33"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1488,9 +1504,9 @@
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="33"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28" t="s">
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1513,9 +1529,9 @@
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="33"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1538,11 +1554,11 @@
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="33"/>
-      <c r="B9" s="28" t="s">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="31" t="s">
         <v>57</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1571,9 +1587,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="33"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="26"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="32"/>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1600,11 +1616,11 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="33"/>
-      <c r="B11" s="28" t="s">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="31" t="s">
         <v>58</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1633,9 +1649,9 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="33"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="25"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="33"/>
       <c r="D12" s="5" t="s">
         <v>53</v>
       </c>
@@ -1654,9 +1670,9 @@
       <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="33"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="26"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
@@ -1683,11 +1699,11 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="33"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="31" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -1714,11 +1730,11 @@
       <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="33"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="26"/>
+      <c r="C15" s="32"/>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1743,7 +1759,7 @@
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="33"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="5" t="s">
         <v>43</v>
       </c>
@@ -1768,7 +1784,7 @@
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="24" t="s">
         <v>75</v>
       </c>
       <c r="B17" s="22" t="s">
@@ -1795,7 +1811,7 @@
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="30"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="23"/>
       <c r="C18" s="5" t="s">
         <v>92</v>
@@ -1820,7 +1836,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="30"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="19" t="s">
         <v>77</v>
       </c>
@@ -1847,8 +1863,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="30"/>
-      <c r="B20" s="28" t="s">
+      <c r="A20" s="25"/>
+      <c r="B20" s="29" t="s">
         <v>95</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -1870,8 +1886,8 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="30"/>
-      <c r="B21" s="28"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="5" t="s">
         <v>97</v>
       </c>
@@ -1893,7 +1909,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="14.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="30"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="22" t="s">
         <v>103</v>
       </c>
@@ -1916,8 +1932,8 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="30"/>
-      <c r="B23" s="27"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="5" t="s">
         <v>105</v>
       </c>
@@ -1937,8 +1953,8 @@
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="30"/>
-      <c r="B24" s="27"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="5" t="s">
         <v>106</v>
       </c>
@@ -1958,7 +1974,7 @@
       <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="30"/>
+      <c r="A25" s="25"/>
       <c r="B25" s="23"/>
       <c r="C25" s="5" t="s">
         <v>107</v>
@@ -1977,7 +1993,7 @@
       <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="31"/>
+      <c r="A26" s="26"/>
       <c r="B26" s="5" t="s">
         <v>78</v>
       </c>
@@ -2002,7 +2018,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="31" t="s">
         <v>79</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -2027,7 +2043,7 @@
       <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="25"/>
+      <c r="A28" s="33"/>
       <c r="B28" s="5" t="s">
         <v>80</v>
       </c>
@@ -2050,7 +2066,7 @@
       <c r="K28" s="5"/>
     </row>
     <row r="29" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="25"/>
+      <c r="A29" s="33"/>
       <c r="B29" s="5" t="s">
         <v>81</v>
       </c>
@@ -2073,7 +2089,7 @@
       <c r="K29" s="5"/>
     </row>
     <row r="30" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="25"/>
+      <c r="A30" s="33"/>
       <c r="B30" s="5" t="s">
         <v>84</v>
       </c>
@@ -2095,13 +2111,13 @@
       </c>
       <c r="K30" s="5"/>
     </row>
-    <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="25"/>
+    <row r="31" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="33"/>
       <c r="B31" s="22" t="s">
         <v>132</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
@@ -2110,24 +2126,26 @@
       <c r="H31" s="11">
         <v>45835</v>
       </c>
-      <c r="I31" s="11"/>
+      <c r="I31" s="11">
+        <v>45840</v>
+      </c>
       <c r="J31" s="4" t="s">
-        <v>119</v>
+        <v>24</v>
       </c>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" s="25"/>
-      <c r="B32" s="23"/>
+    <row r="32" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="33"/>
+      <c r="B32" s="30"/>
       <c r="C32" s="5" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="11"/>
       <c r="H32" s="11">
-        <v>45835</v>
+        <v>45841</v>
       </c>
       <c r="I32" s="11"/>
       <c r="J32" s="4" t="s">
@@ -2135,85 +2153,77 @@
       </c>
       <c r="K32" s="5"/>
     </row>
-    <row r="33" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A33" s="25"/>
-      <c r="B33" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C33" s="5"/>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A33" s="33"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="5" t="s">
+        <v>152</v>
+      </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="11">
-        <v>45838</v>
-      </c>
+      <c r="G33" s="11"/>
       <c r="H33" s="11"/>
       <c r="I33" s="11"/>
       <c r="J33" s="4"/>
-      <c r="K33" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A34" s="25"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="5"/>
+      <c r="K33" s="5"/>
+    </row>
+    <row r="34" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="33"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>143</v>
+      </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
       <c r="I34" s="11"/>
       <c r="J34" s="4"/>
-      <c r="K34" s="12"/>
-    </row>
-    <row r="35" spans="1:11" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="25"/>
-      <c r="B35" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D35" s="5"/>
+      <c r="K34" s="5"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A35" s="33"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="5" t="s">
+        <v>153</v>
+      </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
-      <c r="G35" s="11">
-        <v>45845</v>
-      </c>
+      <c r="G35" s="11"/>
       <c r="H35" s="11"/>
       <c r="I35" s="11"/>
       <c r="J35" s="4"/>
-      <c r="K35" s="22" t="s">
-        <v>139</v>
-      </c>
+      <c r="K35" s="5"/>
     </row>
     <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="25"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="22" t="s">
-        <v>144</v>
-      </c>
+      <c r="A36" s="33"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="23"/>
       <c r="D36" s="5" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
-      <c r="G36" s="11">
-        <v>45852</v>
-      </c>
+      <c r="G36" s="11"/>
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
       <c r="J36" s="4"/>
-      <c r="K36" s="27"/>
+      <c r="K36" s="5"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A37" s="26"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="5" t="s">
-        <v>146</v>
-      </c>
+      <c r="A37" s="33"/>
+      <c r="B37" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="11">
@@ -2222,168 +2232,262 @@
       <c r="H37" s="11"/>
       <c r="I37" s="11"/>
       <c r="J37" s="4"/>
-      <c r="K37" s="23"/>
-    </row>
-    <row r="38" spans="1:11" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="B38" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>134</v>
+      <c r="K37" s="22" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="33"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="12" t="s">
+        <v>142</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
-      <c r="G38" s="11">
-        <v>45866</v>
-      </c>
+      <c r="G38" s="11"/>
       <c r="H38" s="11"/>
       <c r="I38" s="11"/>
       <c r="J38" s="4"/>
-      <c r="K38" s="5"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A39" s="25"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D39" s="5"/>
+      <c r="K38" s="30"/>
+    </row>
+    <row r="39" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="33"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="1"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="11">
-        <v>45873</v>
+        <v>45866</v>
       </c>
       <c r="H39" s="11"/>
       <c r="I39" s="11"/>
       <c r="J39" s="4"/>
-      <c r="K39" s="5"/>
-    </row>
-    <row r="40" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="25"/>
-      <c r="B40" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C40" s="5"/>
+      <c r="K39" s="30"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A40" s="33"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="35"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
-      <c r="G40" s="11">
-        <v>45880</v>
-      </c>
+      <c r="G40" s="11"/>
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
       <c r="J40" s="4"/>
-      <c r="K40" s="5"/>
-    </row>
-    <row r="41" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="25"/>
-      <c r="B41" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C41" s="5"/>
+      <c r="K40" s="30"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A41" s="33"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="35"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
       <c r="G41" s="11">
-        <v>45887</v>
+        <v>45873</v>
       </c>
       <c r="H41" s="11"/>
       <c r="I41" s="11"/>
       <c r="J41" s="4"/>
-      <c r="K41" s="5"/>
-    </row>
-    <row r="42" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A42" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
+      <c r="K41" s="23"/>
+    </row>
+    <row r="42" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="33"/>
+      <c r="B42" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>141</v>
+      </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="11">
-        <v>45894</v>
-      </c>
-      <c r="H42" s="11">
-        <v>45900</v>
-      </c>
+        <v>45845</v>
+      </c>
+      <c r="H42" s="11"/>
       <c r="I42" s="11"/>
       <c r="J42" s="4"/>
       <c r="K42" s="5"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A43" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C43" s="5"/>
+      <c r="A43" s="33"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="12"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
       <c r="G43" s="11">
-        <v>45901</v>
+        <v>45852</v>
       </c>
       <c r="H43" s="11"/>
       <c r="I43" s="11"/>
       <c r="J43" s="4"/>
-      <c r="K43" s="5"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A44" s="27"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
+      <c r="K43" s="12"/>
+    </row>
+    <row r="44" spans="1:11" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>134</v>
+      </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
-      <c r="G44" s="11"/>
+      <c r="G44" s="11">
+        <v>45880</v>
+      </c>
       <c r="H44" s="11"/>
       <c r="I44" s="11"/>
       <c r="J44" s="4"/>
       <c r="K44" s="5"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A45" s="23"/>
-      <c r="B45" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C45" s="5"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="5" t="s">
+        <v>135</v>
+      </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="11">
-        <v>45929</v>
+        <v>45887</v>
       </c>
       <c r="H45" s="11"/>
       <c r="I45" s="11"/>
       <c r="J45" s="4"/>
       <c r="K45" s="5"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
+    <row r="46" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A46" s="33"/>
+      <c r="B46" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
-      <c r="G46" s="11"/>
+      <c r="G46" s="11">
+        <v>45894</v>
+      </c>
       <c r="H46" s="11"/>
       <c r="I46" s="11"/>
       <c r="J46" s="4"/>
       <c r="K46" s="5"/>
     </row>
+    <row r="47" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A47" s="33"/>
+      <c r="B47" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="5"/>
+    </row>
+    <row r="48" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11">
+        <v>45900</v>
+      </c>
+      <c r="I48" s="11"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="5"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A49" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="11">
+        <v>45901</v>
+      </c>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="5"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A50" s="30"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="5"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A51" s="23"/>
+      <c r="B51" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="11">
+        <v>45929</v>
+      </c>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="5"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A17:A26"/>
-    <mergeCell ref="A3:A16"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B25"/>
+  <mergeCells count="22">
+    <mergeCell ref="A27:A43"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="K37:K41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C34:C36"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C15"/>
@@ -2392,14 +2496,11 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B4:B8"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="A27:A37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="K35:K37"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A17:A26"/>
+    <mergeCell ref="A3:A16"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2408,7 +2509,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A2:E35"/>
+  <dimension ref="A2:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
@@ -2622,7 +2723,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="25" t="s">
         <v>111</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2636,7 +2737,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="30"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="2" t="s">
         <v>122</v>
       </c>
@@ -2648,8 +2749,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30" t="s">
+      <c r="A24" s="25"/>
+      <c r="B24" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C24" s="15">
@@ -2663,8 +2764,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="30"/>
-      <c r="B25" s="30"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="25"/>
       <c r="C25" s="15">
         <v>45820</v>
       </c>
@@ -2673,8 +2774,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="30"/>
-      <c r="B26" s="30"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="25"/>
       <c r="C26" s="15">
         <v>45820</v>
       </c>
@@ -2683,8 +2784,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="30"/>
-      <c r="B27" s="30" t="s">
+      <c r="A27" s="25"/>
+      <c r="B27" s="25" t="s">
         <v>123</v>
       </c>
       <c r="C27" s="15">
@@ -2699,7 +2800,7 @@
     </row>
     <row r="28" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A28" s="20"/>
-      <c r="B28" s="30"/>
+      <c r="B28" s="25"/>
       <c r="C28" s="15">
         <v>45821</v>
       </c>
@@ -2748,7 +2849,7 @@
         <v>45836</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="3:4" ht="29" x14ac:dyDescent="0.35">
@@ -2756,7 +2857,7 @@
         <v>45838</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="3:4" ht="145" x14ac:dyDescent="0.35">
@@ -2764,7 +2865,7 @@
         <v>45839</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="3:4" ht="116" x14ac:dyDescent="0.35">
@@ -2772,7 +2873,15 @@
         <v>45840</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>151</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="C36" s="15">
+        <v>45841</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature: create UART gut model mode with UART comm instead of TCP and test within pc
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED7038C-47D0-4DCB-A5F4-9480DDBE71AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB27767B-4B81-42A8-BE53-9CB24A6D2182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
-    <sheet name="Journal" sheetId="3" r:id="rId2"/>
+    <sheet name="Notes" sheetId="3" r:id="rId2"/>
     <sheet name="README" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="166">
   <si>
     <t>Import file</t>
   </si>
@@ -648,42 +648,75 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Buffer skipping error fix. 
+    <t>The process skipping only happens when the scope is connected to the input signal and the output sample signal in simulink. It seems to cause some kind of blocking because of the matlab excecutions. interestingly, when I test the pacemaker and the simulink on the same device(both in pc), skipping occures with or without scope(more so when the pace signal is connected to the scope), especially after detection ignore. but if i run the pacemaker in the board, without scopes connectedot just the gut signal connected, no skipping occurs. I am assuming the gut model's reaction computation to the pace signal is requires alot of performance power. 
+So it is recommended to run the gut model or the pacemaker terminal in a different device to not get any buffer skips. Although the skips(if not running via UART in putty) are process thread skips, thus not skipping signals, which is not critical in the outcome of  pacmaker.</t>
+  </si>
+  <si>
+    <t>Restructuring folder structure</t>
+  </si>
+  <si>
+    <t>Create UART driver for DE1SoC HPS</t>
+  </si>
+  <si>
+    <t>Test UART comm and pacing functionality on DE1-Soc HPS</t>
+  </si>
+  <si>
+    <t>Implement UART comm for ARM Linux</t>
+  </si>
+  <si>
+    <t>Test on ARM Linux</t>
+  </si>
+  <si>
+    <t>Driver dev</t>
+  </si>
+  <si>
+    <t>Create a test trans and recv app for testing</t>
+  </si>
+  <si>
+    <t>1. virtual UART(pacemaker) &lt;-&gt; TCP(gut model) connection within PC
+2. PC com</t>
+  </si>
+  <si>
+    <t>journal</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>Buffer skipping error fix. 
 - Add buffer skip check
 - Add execution time check
 - Skipping buffer found in pc mode(after DETECTION IGNORE)
-- Skipping buffer also found in board, after DETECTION IGNORE when running via ssh teminal, and randomly much more frequently when running via putty
-I found that using PuTTY over USB-UART causes printf() to block due to slow serial output, which delays your processing thread and leads to buffer skips — unlike SSH, which handles output quickly over a fast, buffered TCP connection.
+- Skipping buffer also found in board, after DETECTION IGNORE when running via ssh teminal, and randomly much more frequently when running via putty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I found that using PuTTY over USB-UART causes printf() to block due to slow serial output, which delays your processing thread and leads to buffer skips — unlike SSH, which handles output quickly over a fast, buffered TCP connection.
 I removed the pace signal sending code block(which was right before the signal recieve block in the server funciton) and it didnt skip any buffers.  </t>
   </si>
   <si>
-    <t>The process skipping only happens when the scope is connected to the input signal and the output sample signal in simulink. It seems to cause some kind of blocking because of the matlab excecutions. interestingly, when I test the pacemaker and the simulink on the same device(both in pc), skipping occures with or without scope(more so when the pace signal is connected to the scope), especially after detection ignore. but if i run the pacemaker in the board, without scopes connectedot just the gut signal connected, no skipping occurs. I am assuming the gut model's reaction computation to the pace signal is requires alot of performance power. 
-So it is recommended to run the gut model or the pacemaker terminal in a different device to not get any buffer skips. Although the skips(if not running via UART in putty) are process thread skips, thus not skipping signals, which is not critical in the outcome of  pacmaker.</t>
-  </si>
-  <si>
-    <t>Restructuring folder structure</t>
-  </si>
-  <si>
-    <t>Create UART driver for DE1SoC HPS</t>
-  </si>
-  <si>
-    <t>Test UART comm and pacing functionality on DE1-Soc HPS</t>
-  </si>
-  <si>
-    <t>Implement UART comm for ARM Linux</t>
-  </si>
-  <si>
-    <t>Test on ARM Linux</t>
-  </si>
-  <si>
-    <t>Driver dev</t>
-  </si>
-  <si>
-    <t>Create a test trans and recv app for testing</t>
-  </si>
-  <si>
     <t>Created UART driver for linux(not arm_linux)
-Create a Virtual UART TCP server bridge in Ubuntu</t>
+Create a Virtual UART TCP server bridge in Ubuntu using socat</t>
+  </si>
+  <si>
+    <t>Create UART gut model mode with UART comm instead of TCP
+(gut model connect to port 8080 and pacemaker connect to UART path)
+Gut signal transmition implementation
+Pace signal transmitiion implementation</t>
+  </si>
+  <si>
+    <t>Interestingly, when running both pacemaker and gut model on same device, skipping doesn’t happen anymore even with both gut and pacing signals connecte st scope. I really don’t understand why this is…</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Sub Steps</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> type</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -841,7 +874,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -906,12 +939,30 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -927,26 +978,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1353,8 +1392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1412,7 +1451,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="33" t="s">
         <v>82</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1437,7 +1476,7 @@
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="28"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="29" t="s">
         <v>67</v>
       </c>
@@ -1462,7 +1501,7 @@
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="28"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
       <c r="D5" s="5" t="s">
@@ -1483,7 +1522,7 @@
       <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="28"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="29"/>
       <c r="C6" s="29"/>
       <c r="D6" s="5" t="s">
@@ -1504,7 +1543,7 @@
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="28"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="29"/>
       <c r="C7" s="29" t="s">
         <v>26</v>
@@ -1529,7 +1568,7 @@
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="28"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
       <c r="D8" s="5" t="s">
@@ -1554,11 +1593,11 @@
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="28"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="23" t="s">
         <v>57</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1587,9 +1626,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="28"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="29"/>
-      <c r="C10" s="32"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1616,11 +1655,11 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="28"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="23" t="s">
         <v>58</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1649,9 +1688,9 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="28"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="29"/>
-      <c r="C12" s="33"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="5" t="s">
         <v>53</v>
       </c>
@@ -1670,9 +1709,9 @@
       <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="28"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="29"/>
-      <c r="C13" s="32"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
@@ -1699,11 +1738,11 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="28"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="23" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -1730,11 +1769,11 @@
       <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="28"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="32"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1759,7 +1798,7 @@
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="28"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="5" t="s">
         <v>43</v>
       </c>
@@ -1784,10 +1823,10 @@
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="25" t="s">
         <v>76</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -1811,8 +1850,8 @@
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="25"/>
-      <c r="B18" s="23"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="5" t="s">
         <v>92</v>
       </c>
@@ -1836,7 +1875,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="25"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="19" t="s">
         <v>77</v>
       </c>
@@ -1863,7 +1902,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="25"/>
+      <c r="A20" s="31"/>
       <c r="B20" s="29" t="s">
         <v>95</v>
       </c>
@@ -1886,7 +1925,7 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="25"/>
+      <c r="A21" s="31"/>
       <c r="B21" s="29"/>
       <c r="C21" s="5" t="s">
         <v>97</v>
@@ -1909,8 +1948,8 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="14.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="25"/>
-      <c r="B22" s="22" t="s">
+      <c r="A22" s="31"/>
+      <c r="B22" s="25" t="s">
         <v>103</v>
       </c>
       <c r="C22" s="5" t="s">
@@ -1932,8 +1971,8 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="25"/>
-      <c r="B23" s="30"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="26"/>
       <c r="C23" s="5" t="s">
         <v>105</v>
       </c>
@@ -1953,8 +1992,8 @@
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="25"/>
-      <c r="B24" s="30"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="26"/>
       <c r="C24" s="5" t="s">
         <v>106</v>
       </c>
@@ -1974,8 +2013,8 @@
       <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="25"/>
-      <c r="B25" s="23"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="27"/>
       <c r="C25" s="5" t="s">
         <v>107</v>
       </c>
@@ -1993,7 +2032,7 @@
       <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="26"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="5" t="s">
         <v>78</v>
       </c>
@@ -2018,7 +2057,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="23" t="s">
         <v>79</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -2043,7 +2082,7 @@
       <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="33"/>
+      <c r="A28" s="24"/>
       <c r="B28" s="5" t="s">
         <v>80</v>
       </c>
@@ -2066,7 +2105,7 @@
       <c r="K28" s="5"/>
     </row>
     <row r="29" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="33"/>
+      <c r="A29" s="24"/>
       <c r="B29" s="5" t="s">
         <v>81</v>
       </c>
@@ -2089,7 +2128,7 @@
       <c r="K29" s="5"/>
     </row>
     <row r="30" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="33"/>
+      <c r="A30" s="24"/>
       <c r="B30" s="5" t="s">
         <v>84</v>
       </c>
@@ -2112,12 +2151,12 @@
       <c r="K30" s="5"/>
     </row>
     <row r="31" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="33"/>
-      <c r="B31" s="22" t="s">
+      <c r="A31" s="24"/>
+      <c r="B31" s="25" t="s">
         <v>132</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
@@ -2135,10 +2174,10 @@
       <c r="K31" s="5"/>
     </row>
     <row r="32" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="33"/>
-      <c r="B32" s="30"/>
+      <c r="A32" s="24"/>
+      <c r="B32" s="26"/>
       <c r="C32" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
@@ -2151,13 +2190,15 @@
       <c r="J32" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="K32" s="5"/>
+      <c r="K32" s="5" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A33" s="33"/>
-      <c r="B33" s="30"/>
+      <c r="A33" s="24"/>
+      <c r="B33" s="26"/>
       <c r="C33" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
@@ -2169,10 +2210,10 @@
       <c r="K33" s="5"/>
     </row>
     <row r="34" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="33"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="22" t="s">
-        <v>149</v>
+      <c r="A34" s="24"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="25" t="s">
+        <v>148</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>143</v>
@@ -2186,11 +2227,11 @@
       <c r="K34" s="5"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A35" s="33"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
+      <c r="A35" s="24"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
       <c r="D35" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -2201,11 +2242,11 @@
       <c r="K35" s="5"/>
     </row>
     <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="33"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="23"/>
+      <c r="A36" s="24"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="27"/>
       <c r="D36" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -2216,8 +2257,8 @@
       <c r="K36" s="5"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A37" s="33"/>
-      <c r="B37" s="22" t="s">
+      <c r="A37" s="24"/>
+      <c r="B37" s="25" t="s">
         <v>136</v>
       </c>
       <c r="C37" s="12" t="s">
@@ -2232,13 +2273,13 @@
       <c r="H37" s="11"/>
       <c r="I37" s="11"/>
       <c r="J37" s="4"/>
-      <c r="K37" s="22" t="s">
+      <c r="K37" s="25" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="33"/>
-      <c r="B38" s="30"/>
+      <c r="A38" s="24"/>
+      <c r="B38" s="26"/>
       <c r="C38" s="12" t="s">
         <v>142</v>
       </c>
@@ -2249,12 +2290,12 @@
       <c r="H38" s="11"/>
       <c r="I38" s="11"/>
       <c r="J38" s="4"/>
-      <c r="K38" s="30"/>
+      <c r="K38" s="26"/>
     </row>
     <row r="39" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="33"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="35"/>
+      <c r="A39" s="24"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="22"/>
       <c r="D39" s="1"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -2264,12 +2305,12 @@
       <c r="H39" s="11"/>
       <c r="I39" s="11"/>
       <c r="J39" s="4"/>
-      <c r="K39" s="30"/>
+      <c r="K39" s="26"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A40" s="33"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="35"/>
+      <c r="A40" s="24"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="22"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
@@ -2277,12 +2318,12 @@
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
       <c r="J40" s="4"/>
-      <c r="K40" s="30"/>
+      <c r="K40" s="26"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A41" s="33"/>
-      <c r="B41" s="23"/>
-      <c r="C41" s="35"/>
+      <c r="A41" s="24"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="22"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -2292,12 +2333,12 @@
       <c r="H41" s="11"/>
       <c r="I41" s="11"/>
       <c r="J41" s="4"/>
-      <c r="K41" s="23"/>
+      <c r="K41" s="27"/>
     </row>
     <row r="42" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="33"/>
-      <c r="B42" s="22" t="s">
-        <v>150</v>
+      <c r="A42" s="24"/>
+      <c r="B42" s="25" t="s">
+        <v>149</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>141</v>
@@ -2314,8 +2355,8 @@
       <c r="K42" s="5"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A43" s="33"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="24"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="12"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
@@ -2329,10 +2370,10 @@
       <c r="K43" s="12"/>
     </row>
     <row r="44" spans="1:11" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="22" t="s">
+      <c r="B44" s="25" t="s">
         <v>133</v>
       </c>
       <c r="C44" s="5" t="s">
@@ -2350,8 +2391,8 @@
       <c r="K44" s="5"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A45" s="33"/>
-      <c r="B45" s="30"/>
+      <c r="A45" s="24"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="5" t="s">
         <v>135</v>
       </c>
@@ -2367,7 +2408,7 @@
       <c r="K45" s="5"/>
     </row>
     <row r="46" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="33"/>
+      <c r="A46" s="24"/>
       <c r="B46" s="5" t="s">
         <v>85</v>
       </c>
@@ -2384,7 +2425,7 @@
       <c r="K46" s="5"/>
     </row>
     <row r="47" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A47" s="33"/>
+      <c r="A47" s="24"/>
       <c r="B47" s="5" t="s">
         <v>86</v>
       </c>
@@ -2416,7 +2457,7 @@
       <c r="K48" s="5"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A49" s="22" t="s">
+      <c r="A49" s="25" t="s">
         <v>138</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -2435,7 +2476,7 @@
       <c r="K49" s="5"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A50" s="30"/>
+      <c r="A50" s="26"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -2448,7 +2489,7 @@
       <c r="K50" s="5"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A51" s="23"/>
+      <c r="A51" s="27"/>
       <c r="B51" s="5" t="s">
         <v>140</v>
       </c>
@@ -2479,28 +2520,28 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A17:A26"/>
+    <mergeCell ref="A3:A16"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="K37:K41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B17:B18"/>
     <mergeCell ref="A27:A43"/>
     <mergeCell ref="A49:A51"/>
     <mergeCell ref="A44:A47"/>
     <mergeCell ref="B31:B36"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="B37:B41"/>
-    <mergeCell ref="K37:K41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A17:A26"/>
-    <mergeCell ref="A3:A16"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2509,383 +2550,465 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A2:E36"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.453125" style="2" customWidth="1"/>
     <col min="2" max="2" width="10.1796875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" style="15"/>
-    <col min="4" max="4" width="114.26953125" style="16" customWidth="1"/>
-    <col min="5" max="5" width="47.1796875" style="14" customWidth="1"/>
-    <col min="6" max="16384" width="9.26953125" style="14"/>
+    <col min="3" max="3" width="10.1796875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" style="15"/>
+    <col min="5" max="5" width="114.26953125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="47.1796875" style="14" customWidth="1"/>
+    <col min="7" max="16384" width="9.26953125" style="14"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="34" t="s">
+    <row r="1" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>165</v>
+      </c>
+      <c r="E1" s="20"/>
+    </row>
+    <row r="2" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="15">
+      <c r="D2" s="15">
         <v>45723</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="E2" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="14" t="e" vm="1">
+      <c r="F2" s="14" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="34"/>
-      <c r="D3" s="16" t="s">
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="35"/>
+      <c r="E3" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="14" t="e" vm="2">
+      <c r="F3" s="14" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="34"/>
-      <c r="C4" s="15">
+    <row r="4" spans="1:6" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="35"/>
+      <c r="D4" s="15">
         <v>45728</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="E4" s="16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="15">
+      <c r="D5" s="15">
         <v>45730</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="E5" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="34" t="s">
+    <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="15">
+      <c r="D6" s="15">
         <v>45733</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="E6" s="16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="34"/>
-      <c r="C7" s="15">
+    <row r="7" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="35"/>
+      <c r="D7" s="15">
         <v>45798</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="E7" s="16" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="15">
+      <c r="D8" s="15">
         <v>45734</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="E8" s="16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="116" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="15">
+      <c r="D9" s="15">
         <v>45734</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="E9" s="16" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="145" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="15">
+      <c r="D10" s="15">
         <v>45736</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="E10" s="16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="15">
+      <c r="D11" s="15">
         <v>45742</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="E11" s="16" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="34" t="s">
+    <row r="12" spans="1:6" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="15">
+      <c r="D12" s="15">
         <v>45743</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="E12" s="16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="290" x14ac:dyDescent="0.35">
-      <c r="A13" s="34"/>
-      <c r="C13" s="15">
+    <row r="13" spans="1:6" ht="290" x14ac:dyDescent="0.35">
+      <c r="A13" s="35"/>
+      <c r="D13" s="15">
         <v>45743</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="E13" s="16" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="116" x14ac:dyDescent="0.35">
-      <c r="C14" s="15">
+    <row r="14" spans="1:6" ht="116" x14ac:dyDescent="0.35">
+      <c r="D14" s="15">
         <v>45743</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="E14" s="16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="C15" s="15">
+    <row r="15" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="D15" s="15">
         <v>45743</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="E15" s="16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="232" x14ac:dyDescent="0.35">
-      <c r="C16" s="15">
+    <row r="16" spans="1:6" ht="232" x14ac:dyDescent="0.35">
+      <c r="D16" s="15">
         <v>45747</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="E16" s="16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="C17" s="15">
+    <row r="17" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="D17" s="15">
         <v>45747</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="E17" s="17" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="C18" s="15">
+    <row r="18" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+      <c r="D18" s="15">
         <v>45765</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="E18" s="16" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="C19" s="15">
+    <row r="19" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+      <c r="D19" s="15">
         <v>45770</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="E19" s="16" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="145" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="15">
+      <c r="D20" s="15">
         <v>45783</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="E20" s="16" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C21" s="15">
+      <c r="D21" s="15">
         <v>45794</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="E21" s="16" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A22" s="25" t="s">
+    <row r="22" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+      <c r="A22" s="31" t="s">
         <v>111</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C22" s="15">
+      <c r="D22" s="15">
         <v>45805</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="E22" s="16" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="25"/>
+    <row r="23" spans="1:6" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="31"/>
       <c r="B23" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="15">
+      <c r="D23" s="15">
         <v>45815</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="E23" s="16" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="25"/>
-      <c r="B24" s="25" t="s">
+    <row r="24" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="31"/>
+      <c r="B24" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="C24" s="15">
+      <c r="D24" s="15">
         <v>45817</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="E24" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="F24" s="14" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="25"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="15">
+    <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="31"/>
+      <c r="B25" s="31"/>
+      <c r="D25" s="15">
         <v>45820</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="E25" s="16" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="25"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="15">
+    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="31"/>
+      <c r="B26" s="31"/>
+      <c r="D26" s="15">
         <v>45820</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="E26" s="16" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="25"/>
-      <c r="B27" s="25" t="s">
+    <row r="27" spans="1:6" ht="333.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="31"/>
+      <c r="B27" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="C27" s="15">
+      <c r="D27" s="15">
         <v>45819</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="E27" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="F27" s="14" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A28" s="20"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="15">
+      <c r="B28" s="31"/>
+      <c r="D28" s="15">
         <v>45821</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="E28" s="21" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="174" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="174" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="D29" s="15">
         <v>45806</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="E29" s="16" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="145" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="D30" s="15">
         <v>45814</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="E30" s="16" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C31" s="15">
+      <c r="C31" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="D31" s="15">
         <v>45832</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="E31" s="16" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="C32" s="15">
+      <c r="C32" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="D32" s="15">
         <v>45836</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="E32" s="16" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="33" spans="3:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="C33" s="15">
+    <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33" s="35"/>
+      <c r="C33" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="D33" s="15">
         <v>45838</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="E33" s="16" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="3:4" ht="145" x14ac:dyDescent="0.35">
-      <c r="C34" s="15">
+    <row r="34" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A34" s="35"/>
+      <c r="C34" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="D34" s="15">
         <v>45839</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="E34" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A35" s="35"/>
+      <c r="C35" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="D35" s="15">
+        <v>45839</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+      <c r="A36" s="35"/>
+      <c r="C36" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="D36" s="15">
+        <v>45840</v>
+      </c>
+      <c r="E36" s="16" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="3:4" ht="116" x14ac:dyDescent="0.35">
-      <c r="C35" s="15">
-        <v>45840</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="36" spans="3:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="C36" s="15">
+    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" s="35"/>
+      <c r="C37" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="D37" s="15">
         <v>45841</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="E37" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A38" s="35"/>
+      <c r="C38" s="20" t="s">
         <v>155</v>
       </c>
+      <c r="D38" s="15">
+        <v>45842</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" s="35"/>
+      <c r="C39" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="D39" s="15">
+        <v>45842</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>161</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A32:A39"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A6:A7"/>

</xml_diff>

<commit_message>
chore: update uartname for de1soc
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Research\gut-pacemaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB27767B-4B81-42A8-BE53-9CB24A6D2182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD20EF64-0782-46C3-8F4C-DE50B4ACAF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
+    <workbookView xWindow="2660" yWindow="2660" windowWidth="19200" windowHeight="11170" xr2:uid="{FF07EFFA-5070-42E1-91C3-AF06B4048632}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="167">
   <si>
     <t>Import file</t>
   </si>
@@ -717,6 +717,10 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>I attempted to use /dev/ttyS0 for custom UART communication in my application, but quickly realized that the interface was already claimed by Linux—either for console output during boot or for launching a login shell.
+Since ttyS0 was the only available UART port on my system, using an alternative would have meant modifying hardware configurations which introduced unnecessary complexity. To avoid that overhead, I researched how to properly release the interface from system control and documented the steps.</t>
   </si>
 </sst>
 </file>
@@ -942,50 +946,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1392,8 +1396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA6F03D-76AC-4C98-896C-92FC84817ECF}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1451,7 +1455,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="28" t="s">
         <v>82</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1476,11 +1480,11 @@
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="34"/>
-      <c r="B4" s="29" t="s">
+      <c r="A4" s="29"/>
+      <c r="B4" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="30" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -1501,9 +1505,9 @@
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="34"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="5" t="s">
         <v>40</v>
       </c>
@@ -1522,9 +1526,9 @@
       <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="34"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1543,9 +1547,9 @@
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="34"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29" t="s">
+      <c r="A7" s="29"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1568,9 +1572,9 @@
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="34"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
@@ -1593,11 +1597,11 @@
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="34"/>
-      <c r="B9" s="29" t="s">
+      <c r="A9" s="29"/>
+      <c r="B9" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="34" t="s">
         <v>57</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1626,9 +1630,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="34"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="28"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1655,11 +1659,11 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="34"/>
-      <c r="B11" s="29" t="s">
+      <c r="A11" s="29"/>
+      <c r="B11" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="34" t="s">
         <v>58</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1688,9 +1692,9 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="34"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="24"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="36"/>
       <c r="D12" s="5" t="s">
         <v>53</v>
       </c>
@@ -1709,9 +1713,9 @@
       <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="34"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="28"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="35"/>
       <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
@@ -1738,11 +1742,11 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="34"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="34" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -1769,11 +1773,11 @@
       <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="34"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="28"/>
+      <c r="C15" s="35"/>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1798,7 +1802,7 @@
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="34"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="5" t="s">
         <v>43</v>
       </c>
@@ -1823,10 +1827,10 @@
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="31" t="s">
         <v>76</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -1850,8 +1854,8 @@
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="31"/>
-      <c r="B18" s="27"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="5" t="s">
         <v>92</v>
       </c>
@@ -1875,7 +1879,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="31"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="19" t="s">
         <v>77</v>
       </c>
@@ -1902,8 +1906,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="31"/>
-      <c r="B20" s="29" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="30" t="s">
         <v>95</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -1925,8 +1929,8 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="31"/>
-      <c r="B21" s="29"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="30"/>
       <c r="C21" s="5" t="s">
         <v>97</v>
       </c>
@@ -1948,8 +1952,8 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="14.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="31"/>
-      <c r="B22" s="25" t="s">
+      <c r="A22" s="26"/>
+      <c r="B22" s="31" t="s">
         <v>103</v>
       </c>
       <c r="C22" s="5" t="s">
@@ -1971,8 +1975,8 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="31"/>
-      <c r="B23" s="26"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="32"/>
       <c r="C23" s="5" t="s">
         <v>105</v>
       </c>
@@ -1992,8 +1996,8 @@
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="31"/>
-      <c r="B24" s="26"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="32"/>
       <c r="C24" s="5" t="s">
         <v>106</v>
       </c>
@@ -2013,8 +2017,8 @@
       <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="31"/>
-      <c r="B25" s="27"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="33"/>
       <c r="C25" s="5" t="s">
         <v>107</v>
       </c>
@@ -2032,7 +2036,7 @@
       <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="32"/>
+      <c r="A26" s="27"/>
       <c r="B26" s="5" t="s">
         <v>78</v>
       </c>
@@ -2057,7 +2061,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="34" t="s">
         <v>79</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -2082,7 +2086,7 @@
       <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="24"/>
+      <c r="A28" s="36"/>
       <c r="B28" s="5" t="s">
         <v>80</v>
       </c>
@@ -2105,7 +2109,7 @@
       <c r="K28" s="5"/>
     </row>
     <row r="29" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="24"/>
+      <c r="A29" s="36"/>
       <c r="B29" s="5" t="s">
         <v>81</v>
       </c>
@@ -2128,7 +2132,7 @@
       <c r="K29" s="5"/>
     </row>
     <row r="30" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="24"/>
+      <c r="A30" s="36"/>
       <c r="B30" s="5" t="s">
         <v>84</v>
       </c>
@@ -2151,8 +2155,8 @@
       <c r="K30" s="5"/>
     </row>
     <row r="31" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="24"/>
-      <c r="B31" s="25" t="s">
+      <c r="A31" s="36"/>
+      <c r="B31" s="31" t="s">
         <v>132</v>
       </c>
       <c r="C31" s="5" t="s">
@@ -2174,8 +2178,8 @@
       <c r="K31" s="5"/>
     </row>
     <row r="32" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="24"/>
-      <c r="B32" s="26"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="32"/>
       <c r="C32" s="5" t="s">
         <v>150</v>
       </c>
@@ -2195,8 +2199,8 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A33" s="24"/>
-      <c r="B33" s="26"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="32"/>
       <c r="C33" s="5" t="s">
         <v>151</v>
       </c>
@@ -2210,9 +2214,9 @@
       <c r="K33" s="5"/>
     </row>
     <row r="34" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="24"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="25" t="s">
+      <c r="A34" s="36"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="31" t="s">
         <v>148</v>
       </c>
       <c r="D34" s="5" t="s">
@@ -2227,9 +2231,9 @@
       <c r="K34" s="5"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A35" s="24"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
+      <c r="A35" s="36"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
       <c r="D35" s="5" t="s">
         <v>152</v>
       </c>
@@ -2242,9 +2246,9 @@
       <c r="K35" s="5"/>
     </row>
     <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="24"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="27"/>
+      <c r="A36" s="36"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="33"/>
       <c r="D36" s="5" t="s">
         <v>153</v>
       </c>
@@ -2257,8 +2261,8 @@
       <c r="K36" s="5"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A37" s="24"/>
-      <c r="B37" s="25" t="s">
+      <c r="A37" s="36"/>
+      <c r="B37" s="31" t="s">
         <v>136</v>
       </c>
       <c r="C37" s="12" t="s">
@@ -2273,13 +2277,13 @@
       <c r="H37" s="11"/>
       <c r="I37" s="11"/>
       <c r="J37" s="4"/>
-      <c r="K37" s="25" t="s">
+      <c r="K37" s="31" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="24"/>
-      <c r="B38" s="26"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="32"/>
       <c r="C38" s="12" t="s">
         <v>142</v>
       </c>
@@ -2290,11 +2294,11 @@
       <c r="H38" s="11"/>
       <c r="I38" s="11"/>
       <c r="J38" s="4"/>
-      <c r="K38" s="26"/>
+      <c r="K38" s="32"/>
     </row>
     <row r="39" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="24"/>
-      <c r="B39" s="26"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="32"/>
       <c r="C39" s="22"/>
       <c r="D39" s="1"/>
       <c r="E39" s="5"/>
@@ -2305,11 +2309,11 @@
       <c r="H39" s="11"/>
       <c r="I39" s="11"/>
       <c r="J39" s="4"/>
-      <c r="K39" s="26"/>
+      <c r="K39" s="32"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A40" s="24"/>
-      <c r="B40" s="26"/>
+      <c r="A40" s="36"/>
+      <c r="B40" s="32"/>
       <c r="C40" s="22"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
@@ -2318,11 +2322,11 @@
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
       <c r="J40" s="4"/>
-      <c r="K40" s="26"/>
+      <c r="K40" s="32"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A41" s="24"/>
-      <c r="B41" s="27"/>
+      <c r="A41" s="36"/>
+      <c r="B41" s="33"/>
       <c r="C41" s="22"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
@@ -2333,11 +2337,11 @@
       <c r="H41" s="11"/>
       <c r="I41" s="11"/>
       <c r="J41" s="4"/>
-      <c r="K41" s="27"/>
+      <c r="K41" s="33"/>
     </row>
     <row r="42" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="24"/>
-      <c r="B42" s="25" t="s">
+      <c r="A42" s="36"/>
+      <c r="B42" s="31" t="s">
         <v>149</v>
       </c>
       <c r="C42" s="5" t="s">
@@ -2355,8 +2359,8 @@
       <c r="K42" s="5"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A43" s="24"/>
-      <c r="B43" s="27"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="33"/>
       <c r="C43" s="12"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
@@ -2370,10 +2374,10 @@
       <c r="K43" s="12"/>
     </row>
     <row r="44" spans="1:11" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="25" t="s">
+      <c r="B44" s="31" t="s">
         <v>133</v>
       </c>
       <c r="C44" s="5" t="s">
@@ -2391,8 +2395,8 @@
       <c r="K44" s="5"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A45" s="24"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="32"/>
       <c r="C45" s="5" t="s">
         <v>135</v>
       </c>
@@ -2408,7 +2412,7 @@
       <c r="K45" s="5"/>
     </row>
     <row r="46" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="24"/>
+      <c r="A46" s="36"/>
       <c r="B46" s="5" t="s">
         <v>85</v>
       </c>
@@ -2425,7 +2429,7 @@
       <c r="K46" s="5"/>
     </row>
     <row r="47" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A47" s="24"/>
+      <c r="A47" s="36"/>
       <c r="B47" s="5" t="s">
         <v>86</v>
       </c>
@@ -2457,7 +2461,7 @@
       <c r="K48" s="5"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A49" s="25" t="s">
+      <c r="A49" s="31" t="s">
         <v>138</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -2476,7 +2480,7 @@
       <c r="K49" s="5"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A50" s="26"/>
+      <c r="A50" s="32"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -2489,7 +2493,7 @@
       <c r="K50" s="5"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A51" s="27"/>
+      <c r="A51" s="33"/>
       <c r="B51" s="5" t="s">
         <v>140</v>
       </c>
@@ -2520,6 +2524,19 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A27:A43"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="K37:K41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B17:B18"/>
     <mergeCell ref="A17:A26"/>
     <mergeCell ref="A3:A16"/>
     <mergeCell ref="B20:B21"/>
@@ -2529,19 +2546,6 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B4:B8"/>
-    <mergeCell ref="K37:K41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A27:A43"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B31:B36"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B37:B41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2550,11 +2554,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE0EB01-4489-47F9-AEE0-AC6F6BCD780A}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2568,7 +2572,7 @@
     <col min="7" max="16384" width="9.26953125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>162</v>
       </c>
@@ -2578,13 +2582,13 @@
       <c r="C1" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="23" t="s">
         <v>165</v>
       </c>
       <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="37" t="s">
         <v>44</v>
       </c>
       <c r="D2" s="15">
@@ -2598,7 +2602,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="35"/>
+      <c r="A3" s="37"/>
       <c r="E3" s="16" t="s">
         <v>46</v>
       </c>
@@ -2607,7 +2611,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="304.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="35"/>
+      <c r="A4" s="37"/>
       <c r="D4" s="15">
         <v>45728</v>
       </c>
@@ -2627,7 +2631,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="37" t="s">
         <v>50</v>
       </c>
       <c r="D6" s="15">
@@ -2638,7 +2642,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="35"/>
+      <c r="A7" s="37"/>
       <c r="D7" s="15">
         <v>45798</v>
       </c>
@@ -2691,7 +2695,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="37" t="s">
         <v>65</v>
       </c>
       <c r="D12" s="15">
@@ -2702,7 +2706,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="290" x14ac:dyDescent="0.35">
-      <c r="A13" s="35"/>
+      <c r="A13" s="37"/>
       <c r="D13" s="15">
         <v>45743</v>
       </c>
@@ -2781,7 +2785,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="87" x14ac:dyDescent="0.35">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="26" t="s">
         <v>111</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2795,7 +2799,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="31"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="2" t="s">
         <v>122</v>
       </c>
@@ -2807,8 +2811,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31" t="s">
+      <c r="A24" s="26"/>
+      <c r="B24" s="26" t="s">
         <v>122</v>
       </c>
       <c r="D24" s="15">
@@ -2822,8 +2826,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="31"/>
-      <c r="B25" s="31"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="26"/>
       <c r="D25" s="15">
         <v>45820</v>
       </c>
@@ -2832,8 +2836,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="31"/>
-      <c r="B26" s="31"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
       <c r="D26" s="15">
         <v>45820</v>
       </c>
@@ -2842,8 +2846,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="333.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="31"/>
-      <c r="B27" s="31" t="s">
+      <c r="A27" s="26"/>
+      <c r="B27" s="26" t="s">
         <v>123</v>
       </c>
       <c r="D27" s="15">
@@ -2858,7 +2862,7 @@
     </row>
     <row r="28" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A28" s="20"/>
-      <c r="B28" s="31"/>
+      <c r="B28" s="26"/>
       <c r="D28" s="15">
         <v>45821</v>
       </c>
@@ -2909,7 +2913,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="37" t="s">
         <v>132</v>
       </c>
       <c r="C32" s="20" t="s">
@@ -2923,7 +2927,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="35"/>
+      <c r="A33" s="37"/>
       <c r="C33" s="20" t="s">
         <v>155</v>
       </c>
@@ -2935,7 +2939,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A34" s="35"/>
+      <c r="A34" s="37"/>
       <c r="C34" s="20" t="s">
         <v>155</v>
       </c>
@@ -2947,7 +2951,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A35" s="35"/>
+      <c r="A35" s="37"/>
       <c r="C35" s="20" t="s">
         <v>156</v>
       </c>
@@ -2959,7 +2963,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="116" x14ac:dyDescent="0.35">
-      <c r="A36" s="35"/>
+      <c r="A36" s="37"/>
       <c r="C36" s="20" t="s">
         <v>156</v>
       </c>
@@ -2971,7 +2975,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="35"/>
+      <c r="A37" s="37"/>
       <c r="C37" s="20" t="s">
         <v>155</v>
       </c>
@@ -2983,7 +2987,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A38" s="35"/>
+      <c r="A38" s="37"/>
       <c r="C38" s="20" t="s">
         <v>155</v>
       </c>
@@ -2995,7 +2999,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="35"/>
+      <c r="A39" s="37"/>
       <c r="C39" s="20" t="s">
         <v>156</v>
       </c>
@@ -3006,15 +3010,26 @@
         <v>161</v>
       </c>
     </row>
+    <row r="40" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="C40" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="D40" s="15">
+        <v>45843</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>166</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B27:B28"/>
     <mergeCell ref="A32:A39"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A22:A27"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B27:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>